<commit_message>
Code updated 23-03-17 11:30:51
</commit_message>
<xml_diff>
--- a/Season_Attack/86.xlsx
+++ b/Season_Attack/86.xlsx
@@ -82,8 +82,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G163"/>
+  <dimension ref="A1:I164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,6 +426,16 @@
           <t>03-15_0</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>03-16_A</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>03-16_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -452,9 +462,15 @@
       <c r="F2" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2913</t>
+      <c r="G2" t="n">
+        <v>2913</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2939</t>
         </is>
       </c>
     </row>
@@ -483,9 +499,15 @@
       <c r="F3" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>4038</t>
+      <c r="G3" t="n">
+        <v>4038</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>4314</t>
         </is>
       </c>
     </row>
@@ -511,12 +533,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>4431</t>
+      <c r="G4" t="n">
+        <v>4431</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>4506</t>
         </is>
       </c>
     </row>
@@ -539,15 +567,21 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F5" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>4014</t>
+      <c r="G5" t="n">
+        <v>4014</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>4409</t>
         </is>
       </c>
     </row>
@@ -576,9 +610,15 @@
       <c r="F6" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>3920</t>
+      <c r="G6" t="n">
+        <v>3920</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>4269</t>
         </is>
       </c>
     </row>
@@ -601,15 +641,21 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F7" s="3" t="n">
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F7" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>4404</t>
+      <c r="G7" t="n">
+        <v>4404</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>4776</t>
         </is>
       </c>
     </row>
@@ -638,9 +684,15 @@
       <c r="F8" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>3806</t>
+      <c r="G8" t="n">
+        <v>3806</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>4120</t>
         </is>
       </c>
     </row>
@@ -663,15 +715,21 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F9" s="3" t="n">
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F9" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>4188</t>
+      <c r="G9" t="n">
+        <v>4188</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>4483</t>
         </is>
       </c>
     </row>
@@ -700,9 +758,15 @@
       <c r="F10" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>4096</t>
+      <c r="G10" t="n">
+        <v>4096</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>4464</t>
         </is>
       </c>
     </row>
@@ -731,9 +795,15 @@
       <c r="F11" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>3745</t>
+      <c r="G11" t="n">
+        <v>3745</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>4234</t>
         </is>
       </c>
     </row>
@@ -759,10 +829,16 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" t="inlineStr">
+      <c r="F12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>2815</v>
+      </c>
+      <c r="H12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="inlineStr">
         <is>
           <t>2815</t>
         </is>
@@ -790,12 +866,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F13" s="3" t="n">
+      <c r="F13" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>4721</t>
+      <c r="G13" t="n">
+        <v>4721</v>
+      </c>
+      <c r="H13" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>5103</t>
         </is>
       </c>
     </row>
@@ -824,9 +906,15 @@
       <c r="F14" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>3963</t>
+      <c r="G14" t="n">
+        <v>3963</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>4326</t>
         </is>
       </c>
     </row>
@@ -850,6 +938,8 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" s="2" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
+      <c r="H15" s="2" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -873,12 +963,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F16" s="3" t="n">
+      <c r="F16" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>3879</t>
+      <c r="G16" t="n">
+        <v>3879</v>
+      </c>
+      <c r="H16" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>4155</t>
         </is>
       </c>
     </row>
@@ -907,9 +1003,15 @@
       <c r="F17" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>3787</t>
+      <c r="G17" t="n">
+        <v>3787</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>4053</t>
         </is>
       </c>
     </row>
@@ -938,9 +1040,15 @@
       <c r="F18" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>3798</t>
+      <c r="G18" t="n">
+        <v>3798</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>4133</t>
         </is>
       </c>
     </row>
@@ -964,6 +1072,8 @@
       <c r="E19" t="inlineStr"/>
       <c r="F19" s="2" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
+      <c r="H19" s="2" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -990,9 +1100,15 @@
       <c r="F20" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>3136</t>
+      <c r="G20" t="n">
+        <v>3136</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>3467</t>
         </is>
       </c>
     </row>
@@ -1018,12 +1134,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F21" s="3" t="n">
+      <c r="F21" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>4309</t>
+      <c r="G21" t="n">
+        <v>4309</v>
+      </c>
+      <c r="H21" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>4594</t>
         </is>
       </c>
     </row>
@@ -1052,9 +1174,15 @@
       <c r="F22" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>2919</t>
+      <c r="G22" t="n">
+        <v>2919</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>3446</t>
         </is>
       </c>
     </row>
@@ -1077,15 +1205,21 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F23" s="3" t="n">
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>4291</t>
+      <c r="G23" t="n">
+        <v>4291</v>
+      </c>
+      <c r="H23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>4458</t>
         </is>
       </c>
     </row>
@@ -1111,10 +1245,16 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F24" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" t="inlineStr">
+      <c r="F24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1142,10 +1282,16 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F25" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" t="inlineStr">
+      <c r="F25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>2588</v>
+      </c>
+      <c r="H25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="inlineStr">
         <is>
           <t>2588</t>
         </is>
@@ -1171,6 +1317,8 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" s="2" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
+      <c r="H26" s="2" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1192,6 +1340,8 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" s="2" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
+      <c r="H27" s="2" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1215,12 +1365,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F28" s="3" t="n">
+      <c r="F28" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>4450</t>
+      <c r="G28" t="n">
+        <v>4450</v>
+      </c>
+      <c r="H28" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>4962</t>
         </is>
       </c>
     </row>
@@ -1244,6 +1400,8 @@
       <c r="E29" t="inlineStr"/>
       <c r="F29" s="2" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
+      <c r="H29" s="2" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1270,9 +1428,15 @@
       <c r="F30" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>3524</t>
+      <c r="G30" t="n">
+        <v>3524</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>3854</t>
         </is>
       </c>
     </row>
@@ -1298,12 +1462,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F31" s="3" t="n">
+      <c r="F31" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>4565</t>
+      <c r="G31" t="n">
+        <v>4565</v>
+      </c>
+      <c r="H31" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>4954</t>
         </is>
       </c>
     </row>
@@ -1332,9 +1502,15 @@
       <c r="F32" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>3343</t>
+      <c r="G32" t="n">
+        <v>3343</v>
+      </c>
+      <c r="H32" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>3562</t>
         </is>
       </c>
     </row>
@@ -1363,9 +1539,15 @@
       <c r="F33" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>4180</t>
+      <c r="G33" t="n">
+        <v>4180</v>
+      </c>
+      <c r="H33" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>4444</t>
         </is>
       </c>
     </row>
@@ -1391,12 +1573,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F34" s="3" t="n">
+      <c r="F34" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>4167</t>
+      <c r="G34" t="n">
+        <v>4167</v>
+      </c>
+      <c r="H34" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>4390</t>
         </is>
       </c>
     </row>
@@ -1425,9 +1613,15 @@
       <c r="F35" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>3694</t>
+      <c r="G35" t="n">
+        <v>3694</v>
+      </c>
+      <c r="H35" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>4086</t>
         </is>
       </c>
     </row>
@@ -1451,6 +1645,8 @@
       <c r="E36" t="inlineStr"/>
       <c r="F36" s="2" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
+      <c r="H36" s="2" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1474,12 +1670,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F37" s="3" t="n">
+      <c r="F37" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>4288</t>
+      <c r="G37" t="n">
+        <v>4288</v>
+      </c>
+      <c r="H37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>4585</t>
         </is>
       </c>
     </row>
@@ -1508,9 +1710,15 @@
       <c r="F38" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>4289</t>
+      <c r="G38" t="n">
+        <v>4289</v>
+      </c>
+      <c r="H38" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>4624</t>
         </is>
       </c>
     </row>
@@ -1539,9 +1747,15 @@
       <c r="F39" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>4259</t>
+      <c r="G39" t="n">
+        <v>4259</v>
+      </c>
+      <c r="H39" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>4568</t>
         </is>
       </c>
     </row>
@@ -1567,12 +1781,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F40" s="3" t="n">
+      <c r="F40" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>4532</t>
+      <c r="G40" t="n">
+        <v>4532</v>
+      </c>
+      <c r="H40" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>4921</t>
         </is>
       </c>
     </row>
@@ -1598,12 +1818,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F41" s="3" t="n">
+      <c r="F41" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>4468</t>
+      <c r="G41" t="n">
+        <v>4468</v>
+      </c>
+      <c r="H41" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>4775</t>
         </is>
       </c>
     </row>
@@ -1629,12 +1855,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F42" s="3" t="n">
+      <c r="F42" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>4211</t>
+      <c r="G42" t="n">
+        <v>4211</v>
+      </c>
+      <c r="H42" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>4440</t>
         </is>
       </c>
     </row>
@@ -1663,9 +1895,15 @@
       <c r="F43" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>3918</t>
+      <c r="G43" t="n">
+        <v>3918</v>
+      </c>
+      <c r="H43" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>4191</t>
         </is>
       </c>
     </row>
@@ -1694,9 +1932,15 @@
       <c r="F44" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>3797</t>
+      <c r="G44" t="n">
+        <v>3797</v>
+      </c>
+      <c r="H44" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>4135</t>
         </is>
       </c>
     </row>
@@ -1725,9 +1969,15 @@
       <c r="F45" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>3860</t>
+      <c r="G45" t="n">
+        <v>3860</v>
+      </c>
+      <c r="H45" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>4098</t>
         </is>
       </c>
     </row>
@@ -1753,12 +2003,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F46" s="3" t="n">
+      <c r="F46" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>4410</t>
+      <c r="G46" t="n">
+        <v>4410</v>
+      </c>
+      <c r="H46" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>4767</t>
         </is>
       </c>
     </row>
@@ -1787,9 +2043,15 @@
       <c r="F47" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>3607</t>
+      <c r="G47" t="n">
+        <v>3607</v>
+      </c>
+      <c r="H47" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>3947</t>
         </is>
       </c>
     </row>
@@ -1815,10 +2077,16 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F48" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G48" t="inlineStr">
+      <c r="F48" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H48" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1844,6 +2112,8 @@
       <c r="E49" t="inlineStr"/>
       <c r="F49" s="2" t="inlineStr"/>
       <c r="G49" t="inlineStr"/>
+      <c r="H49" s="2" t="inlineStr"/>
+      <c r="I49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -1867,10 +2137,16 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F50" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G50" t="inlineStr">
+      <c r="F50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1898,12 +2174,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F51" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>2529</t>
+      <c r="F51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>2529</v>
+      </c>
+      <c r="H51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>2547</t>
         </is>
       </c>
     </row>
@@ -1929,12 +2211,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F52" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>2773</t>
+      <c r="F52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="n">
+        <v>2773</v>
+      </c>
+      <c r="H52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>2801</t>
         </is>
       </c>
     </row>
@@ -1963,9 +2251,15 @@
       <c r="F53" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>4100</t>
+      <c r="G53" t="n">
+        <v>4100</v>
+      </c>
+      <c r="H53" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>4451</t>
         </is>
       </c>
     </row>
@@ -1991,12 +2285,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F54" s="3" t="n">
+      <c r="F54" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>3933</t>
+      <c r="G54" t="n">
+        <v>3933</v>
+      </c>
+      <c r="H54" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>4086</t>
         </is>
       </c>
     </row>
@@ -2025,9 +2325,15 @@
       <c r="F55" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>3745</t>
+      <c r="G55" t="n">
+        <v>3745</v>
+      </c>
+      <c r="H55" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>3972</t>
         </is>
       </c>
     </row>
@@ -2056,9 +2362,15 @@
       <c r="F56" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>3908</t>
+      <c r="G56" t="n">
+        <v>3908</v>
+      </c>
+      <c r="H56" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>4266</t>
         </is>
       </c>
     </row>
@@ -2084,12 +2396,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F57" s="3" t="n">
+      <c r="F57" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>3993</t>
+      <c r="G57" t="n">
+        <v>3993</v>
+      </c>
+      <c r="H57" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>4056</t>
         </is>
       </c>
     </row>
@@ -2118,9 +2436,15 @@
       <c r="F58" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>3929</t>
+      <c r="G58" t="n">
+        <v>3929</v>
+      </c>
+      <c r="H58" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>4010</t>
         </is>
       </c>
     </row>
@@ -2146,10 +2470,16 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F59" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G59" t="inlineStr">
+      <c r="F59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2180,9 +2510,15 @@
       <c r="F60" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>4098</t>
+      <c r="G60" t="n">
+        <v>4098</v>
+      </c>
+      <c r="H60" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>4433</t>
         </is>
       </c>
     </row>
@@ -2208,12 +2544,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F61" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>2498</t>
+      <c r="F61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="n">
+        <v>2498</v>
+      </c>
+      <c r="H61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>2496</t>
         </is>
       </c>
     </row>
@@ -2242,9 +2584,15 @@
       <c r="F62" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>3235</t>
+      <c r="G62" t="n">
+        <v>3235</v>
+      </c>
+      <c r="H62" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>3251</t>
         </is>
       </c>
     </row>
@@ -2273,9 +2621,15 @@
       <c r="F63" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>3829</t>
+      <c r="G63" t="n">
+        <v>3829</v>
+      </c>
+      <c r="H63" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>4134</t>
         </is>
       </c>
     </row>
@@ -2304,9 +2658,15 @@
       <c r="F64" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>4158</t>
+      <c r="G64" t="n">
+        <v>4158</v>
+      </c>
+      <c r="H64" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>4346</t>
         </is>
       </c>
     </row>
@@ -2332,12 +2692,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F65" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>2931</t>
+      <c r="F65" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" t="n">
+        <v>2931</v>
+      </c>
+      <c r="H65" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>2930</t>
         </is>
       </c>
     </row>
@@ -2363,12 +2729,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F66" s="3" t="n">
+      <c r="F66" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>3998</t>
+      <c r="G66" t="n">
+        <v>3998</v>
+      </c>
+      <c r="H66" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>4089</t>
         </is>
       </c>
     </row>
@@ -2394,12 +2766,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F67" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>2639</t>
+      <c r="F67" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" t="n">
+        <v>2639</v>
+      </c>
+      <c r="H67" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>2653</t>
         </is>
       </c>
     </row>
@@ -2425,10 +2803,16 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F68" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G68" t="inlineStr">
+      <c r="F68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2459,9 +2843,15 @@
       <c r="F69" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>3842</t>
+      <c r="G69" t="n">
+        <v>3842</v>
+      </c>
+      <c r="H69" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>4109</t>
         </is>
       </c>
     </row>
@@ -2490,9 +2880,15 @@
       <c r="F70" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>3692</t>
+      <c r="G70" t="n">
+        <v>3692</v>
+      </c>
+      <c r="H70" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>3962</t>
         </is>
       </c>
     </row>
@@ -2518,12 +2914,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F71" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>2658</t>
+      <c r="F71" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" t="n">
+        <v>2658</v>
+      </c>
+      <c r="H71" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>2685</t>
         </is>
       </c>
     </row>
@@ -2552,9 +2954,15 @@
       <c r="F72" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>3765</t>
+      <c r="G72" t="n">
+        <v>3765</v>
+      </c>
+      <c r="H72" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>4000</t>
         </is>
       </c>
     </row>
@@ -2583,9 +2991,15 @@
       <c r="F73" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>4019</t>
+      <c r="G73" t="n">
+        <v>4019</v>
+      </c>
+      <c r="H73" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>4357</t>
         </is>
       </c>
     </row>
@@ -2611,10 +3025,16 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F74" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G74" t="inlineStr">
+      <c r="F74" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2642,10 +3062,16 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F75" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G75" t="inlineStr">
+      <c r="F75" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2676,9 +3102,15 @@
       <c r="F76" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>4321</t>
+      <c r="G76" t="n">
+        <v>4321</v>
+      </c>
+      <c r="H76" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>4362</t>
         </is>
       </c>
     </row>
@@ -2704,10 +3136,16 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F77" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G77" t="inlineStr">
+      <c r="F77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0</v>
+      </c>
+      <c r="H77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2738,9 +3176,15 @@
       <c r="F78" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>4083</t>
+      <c r="G78" t="n">
+        <v>4083</v>
+      </c>
+      <c r="H78" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>4260</t>
         </is>
       </c>
     </row>
@@ -2769,9 +3213,15 @@
       <c r="F79" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>3036</t>
+      <c r="G79" t="n">
+        <v>3036</v>
+      </c>
+      <c r="H79" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>3041</t>
         </is>
       </c>
     </row>
@@ -2795,6 +3245,8 @@
       <c r="E80" t="inlineStr"/>
       <c r="F80" s="2" t="inlineStr"/>
       <c r="G80" t="inlineStr"/>
+      <c r="H80" s="2" t="inlineStr"/>
+      <c r="I80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -2818,12 +3270,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F81" s="3" t="n">
+      <c r="F81" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>4121</t>
+      <c r="G81" t="n">
+        <v>4121</v>
+      </c>
+      <c r="H81" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>4319</t>
         </is>
       </c>
     </row>
@@ -2852,9 +3310,15 @@
       <c r="F82" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>4121</t>
+      <c r="G82" t="n">
+        <v>4121</v>
+      </c>
+      <c r="H82" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>4286</t>
         </is>
       </c>
     </row>
@@ -2883,9 +3347,15 @@
       <c r="F83" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>3989</t>
+      <c r="G83" t="n">
+        <v>3989</v>
+      </c>
+      <c r="H83" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>4138</t>
         </is>
       </c>
     </row>
@@ -2911,12 +3381,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F84" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>3343</t>
+      <c r="F84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" t="n">
+        <v>3343</v>
+      </c>
+      <c r="H84" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>3673</t>
         </is>
       </c>
     </row>
@@ -2945,9 +3421,15 @@
       <c r="F85" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>3848</t>
+      <c r="G85" t="n">
+        <v>3848</v>
+      </c>
+      <c r="H85" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>4008</t>
         </is>
       </c>
     </row>
@@ -2976,9 +3458,15 @@
       <c r="F86" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>2731</t>
+      <c r="G86" t="n">
+        <v>2731</v>
+      </c>
+      <c r="H86" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>2791</t>
         </is>
       </c>
     </row>
@@ -3004,12 +3492,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F87" s="3" t="n">
+      <c r="F87" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>4145</t>
+      <c r="G87" t="n">
+        <v>4145</v>
+      </c>
+      <c r="H87" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>4217</t>
         </is>
       </c>
     </row>
@@ -3038,9 +3532,15 @@
       <c r="F88" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>2992</t>
+      <c r="G88" t="n">
+        <v>2992</v>
+      </c>
+      <c r="H88" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>3048</t>
         </is>
       </c>
     </row>
@@ -3069,9 +3569,15 @@
       <c r="F89" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>3365</t>
+      <c r="G89" t="n">
+        <v>3365</v>
+      </c>
+      <c r="H89" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>3588</t>
         </is>
       </c>
     </row>
@@ -3097,12 +3603,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F90" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>2846</t>
+      <c r="F90" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G90" t="n">
+        <v>2846</v>
+      </c>
+      <c r="H90" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>2875</t>
         </is>
       </c>
     </row>
@@ -3131,9 +3643,15 @@
       <c r="F91" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>3161</t>
+      <c r="G91" t="n">
+        <v>3161</v>
+      </c>
+      <c r="H91" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>3360</t>
         </is>
       </c>
     </row>
@@ -3159,10 +3677,16 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F92" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G92" t="inlineStr">
+      <c r="F92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G92" t="n">
+        <v>0</v>
+      </c>
+      <c r="H92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3193,9 +3717,15 @@
       <c r="F93" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>3109</t>
+      <c r="G93" t="n">
+        <v>3109</v>
+      </c>
+      <c r="H93" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>3238</t>
         </is>
       </c>
     </row>
@@ -3221,10 +3751,16 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F94" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G94" t="inlineStr">
+      <c r="F94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G94" t="n">
+        <v>0</v>
+      </c>
+      <c r="H94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3255,9 +3791,15 @@
       <c r="F95" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>3296</t>
+      <c r="G95" t="n">
+        <v>3296</v>
+      </c>
+      <c r="H95" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>3545</t>
         </is>
       </c>
     </row>
@@ -3283,12 +3825,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F96" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>2521</t>
+      <c r="F96" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G96" t="n">
+        <v>2521</v>
+      </c>
+      <c r="H96" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>2512</t>
         </is>
       </c>
     </row>
@@ -3314,12 +3862,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F97" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>2092</t>
+      <c r="F97" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G97" t="n">
+        <v>2092</v>
+      </c>
+      <c r="H97" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>2119</t>
         </is>
       </c>
     </row>
@@ -3345,12 +3899,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F98" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>2496</t>
+      <c r="F98" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G98" t="n">
+        <v>2496</v>
+      </c>
+      <c r="H98" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>2858</t>
         </is>
       </c>
     </row>
@@ -3376,12 +3936,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F99" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>2507</t>
+      <c r="F99" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G99" t="n">
+        <v>2507</v>
+      </c>
+      <c r="H99" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>2506</t>
         </is>
       </c>
     </row>
@@ -3410,9 +3976,15 @@
       <c r="F100" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>3093</t>
+      <c r="G100" t="n">
+        <v>3093</v>
+      </c>
+      <c r="H100" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>3372</t>
         </is>
       </c>
     </row>
@@ -3438,12 +4010,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F101" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>2250</t>
+      <c r="F101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G101" t="n">
+        <v>2250</v>
+      </c>
+      <c r="H101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>2248</t>
         </is>
       </c>
     </row>
@@ -3472,9 +4050,15 @@
       <c r="F102" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>3994</t>
+      <c r="G102" t="n">
+        <v>3994</v>
+      </c>
+      <c r="H102" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>4190</t>
         </is>
       </c>
     </row>
@@ -3503,9 +4087,15 @@
       <c r="F103" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>3327</t>
+      <c r="G103" t="n">
+        <v>3327</v>
+      </c>
+      <c r="H103" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>3640</t>
         </is>
       </c>
     </row>
@@ -3534,9 +4124,15 @@
       <c r="F104" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>3512</t>
+      <c r="G104" t="n">
+        <v>3512</v>
+      </c>
+      <c r="H104" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>3775</t>
         </is>
       </c>
     </row>
@@ -3562,12 +4158,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F105" s="3" t="n">
+      <c r="F105" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>3870</t>
+      <c r="G105" t="n">
+        <v>3870</v>
+      </c>
+      <c r="H105" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>4108</t>
         </is>
       </c>
     </row>
@@ -3596,9 +4198,15 @@
       <c r="F106" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>3966</t>
+      <c r="G106" t="n">
+        <v>3966</v>
+      </c>
+      <c r="H106" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>4041</t>
         </is>
       </c>
     </row>
@@ -3624,12 +4232,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F107" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>3493</t>
+      <c r="F107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G107" t="n">
+        <v>3493</v>
+      </c>
+      <c r="H107" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>3839</t>
         </is>
       </c>
     </row>
@@ -3655,10 +4269,16 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F108" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G108" t="inlineStr">
+      <c r="F108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G108" t="n">
+        <v>0</v>
+      </c>
+      <c r="H108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3686,12 +4306,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F109" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>2820</t>
+      <c r="F109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G109" t="n">
+        <v>2820</v>
+      </c>
+      <c r="H109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>2861</t>
         </is>
       </c>
     </row>
@@ -3717,10 +4343,16 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F110" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G110" t="inlineStr">
+      <c r="F110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G110" t="n">
+        <v>0</v>
+      </c>
+      <c r="H110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I110" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3751,9 +4383,15 @@
       <c r="F111" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="G111" t="inlineStr">
-        <is>
-          <t>3286</t>
+      <c r="G111" t="n">
+        <v>3286</v>
+      </c>
+      <c r="H111" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>3372</t>
         </is>
       </c>
     </row>
@@ -3782,9 +4420,15 @@
       <c r="F112" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>3737</t>
+      <c r="G112" t="n">
+        <v>3737</v>
+      </c>
+      <c r="H112" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>3982</t>
         </is>
       </c>
     </row>
@@ -3813,9 +4457,15 @@
       <c r="F113" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G113" t="inlineStr">
-        <is>
-          <t>3345</t>
+      <c r="G113" t="n">
+        <v>3345</v>
+      </c>
+      <c r="H113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>3328</t>
         </is>
       </c>
     </row>
@@ -3841,12 +4491,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F114" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G114" t="inlineStr">
-        <is>
-          <t>2559</t>
+      <c r="F114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G114" t="n">
+        <v>2559</v>
+      </c>
+      <c r="H114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>2556</t>
         </is>
       </c>
     </row>
@@ -3872,12 +4528,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F115" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>3339</t>
+      <c r="F115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G115" t="n">
+        <v>3339</v>
+      </c>
+      <c r="H115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>3456</t>
         </is>
       </c>
     </row>
@@ -3903,12 +4565,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F116" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G116" t="inlineStr">
-        <is>
-          <t>2831</t>
+      <c r="F116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G116" t="n">
+        <v>2831</v>
+      </c>
+      <c r="H116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>3000</t>
         </is>
       </c>
     </row>
@@ -3934,12 +4602,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F117" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>2376</t>
+      <c r="F117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G117" t="n">
+        <v>2376</v>
+      </c>
+      <c r="H117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>2385</t>
         </is>
       </c>
     </row>
@@ -3968,9 +4642,15 @@
       <c r="F118" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G118" t="inlineStr">
-        <is>
-          <t>2820</t>
+      <c r="G118" t="n">
+        <v>2820</v>
+      </c>
+      <c r="H118" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>2945</t>
         </is>
       </c>
     </row>
@@ -3999,9 +4679,15 @@
       <c r="F119" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G119" t="inlineStr">
-        <is>
-          <t>3836</t>
+      <c r="G119" t="n">
+        <v>3836</v>
+      </c>
+      <c r="H119" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>4014</t>
         </is>
       </c>
     </row>
@@ -4027,12 +4713,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F120" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="F120" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G120" t="n">
+        <v>0</v>
+      </c>
+      <c r="H120" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>2517</t>
         </is>
       </c>
     </row>
@@ -4058,10 +4750,16 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F121" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G121" t="inlineStr">
+      <c r="F121" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G121" t="n">
+        <v>1575</v>
+      </c>
+      <c r="H121" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I121" t="inlineStr">
         <is>
           <t>1575</t>
         </is>
@@ -4089,12 +4787,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F122" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G122" t="inlineStr">
-        <is>
-          <t>2514</t>
+      <c r="F122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G122" t="n">
+        <v>2514</v>
+      </c>
+      <c r="H122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>2506</t>
         </is>
       </c>
     </row>
@@ -4123,9 +4827,15 @@
       <c r="F123" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G123" t="inlineStr">
-        <is>
-          <t>3543</t>
+      <c r="G123" t="n">
+        <v>3543</v>
+      </c>
+      <c r="H123" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>3872</t>
         </is>
       </c>
     </row>
@@ -4151,10 +4861,16 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F124" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G124" t="inlineStr">
+      <c r="F124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G124" t="n">
+        <v>0</v>
+      </c>
+      <c r="H124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I124" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4185,9 +4901,15 @@
       <c r="F125" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G125" t="inlineStr">
-        <is>
-          <t>3407</t>
+      <c r="G125" t="n">
+        <v>3407</v>
+      </c>
+      <c r="H125" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>3547</t>
         </is>
       </c>
     </row>
@@ -4216,9 +4938,15 @@
       <c r="F126" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G126" t="inlineStr">
-        <is>
-          <t>3424</t>
+      <c r="G126" t="n">
+        <v>3424</v>
+      </c>
+      <c r="H126" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>3548</t>
         </is>
       </c>
     </row>
@@ -4244,12 +4972,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F127" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G127" t="inlineStr">
-        <is>
-          <t>2800</t>
+      <c r="F127" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G127" t="n">
+        <v>2800</v>
+      </c>
+      <c r="H127" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>3040</t>
         </is>
       </c>
     </row>
@@ -4278,9 +5012,15 @@
       <c r="F128" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="G128" t="inlineStr">
-        <is>
-          <t>3597</t>
+      <c r="G128" t="n">
+        <v>3597</v>
+      </c>
+      <c r="H128" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>3786</t>
         </is>
       </c>
     </row>
@@ -4306,12 +5046,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F129" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G129" t="inlineStr">
-        <is>
-          <t>1990</t>
+      <c r="F129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G129" t="n">
+        <v>1990</v>
+      </c>
+      <c r="H129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>2025</t>
         </is>
       </c>
     </row>
@@ -4337,10 +5083,16 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F130" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G130" t="inlineStr">
+      <c r="F130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G130" t="n">
+        <v>0</v>
+      </c>
+      <c r="H130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4368,10 +5120,16 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F131" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G131" t="inlineStr">
+      <c r="F131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G131" t="n">
+        <v>0</v>
+      </c>
+      <c r="H131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4402,9 +5160,15 @@
       <c r="F132" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="G132" t="inlineStr">
-        <is>
-          <t>3284</t>
+      <c r="G132" t="n">
+        <v>3284</v>
+      </c>
+      <c r="H132" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>3440</t>
         </is>
       </c>
     </row>
@@ -4430,10 +5194,16 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F133" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G133" t="inlineStr">
+      <c r="F133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G133" t="n">
+        <v>0</v>
+      </c>
+      <c r="H133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4464,9 +5234,15 @@
       <c r="F134" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G134" t="inlineStr">
-        <is>
-          <t>2837</t>
+      <c r="G134" t="n">
+        <v>2837</v>
+      </c>
+      <c r="H134" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>2979</t>
         </is>
       </c>
     </row>
@@ -4492,12 +5268,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F135" s="3" t="n">
+      <c r="F135" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G135" t="inlineStr">
-        <is>
-          <t>3502</t>
+      <c r="G135" t="n">
+        <v>3502</v>
+      </c>
+      <c r="H135" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>3809</t>
         </is>
       </c>
     </row>
@@ -4526,9 +5308,15 @@
       <c r="F136" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G136" t="inlineStr">
-        <is>
-          <t>3485</t>
+      <c r="G136" t="n">
+        <v>3485</v>
+      </c>
+      <c r="H136" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>3632</t>
         </is>
       </c>
     </row>
@@ -4554,10 +5342,16 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F137" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G137" t="inlineStr">
+      <c r="F137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G137" t="n">
+        <v>0</v>
+      </c>
+      <c r="H137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4585,12 +5379,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F138" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G138" t="inlineStr">
-        <is>
-          <t>1500</t>
+      <c r="F138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G138" t="n">
+        <v>1500</v>
+      </c>
+      <c r="H138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>1499</t>
         </is>
       </c>
     </row>
@@ -4616,12 +5416,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F139" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G139" t="inlineStr">
-        <is>
-          <t>2831</t>
+      <c r="F139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G139" t="n">
+        <v>2831</v>
+      </c>
+      <c r="H139" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>3057</t>
         </is>
       </c>
     </row>
@@ -4647,10 +5453,16 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F140" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G140" t="inlineStr">
+      <c r="F140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G140" t="n">
+        <v>0</v>
+      </c>
+      <c r="H140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4678,10 +5490,16 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F141" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G141" t="inlineStr">
+      <c r="F141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G141" t="n">
+        <v>0</v>
+      </c>
+      <c r="H141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4712,9 +5530,15 @@
       <c r="F142" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G142" t="inlineStr">
-        <is>
-          <t>3157</t>
+      <c r="G142" t="n">
+        <v>3157</v>
+      </c>
+      <c r="H142" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>3168</t>
         </is>
       </c>
     </row>
@@ -4740,10 +5564,16 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F143" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G143" t="inlineStr">
+      <c r="F143" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G143" t="n">
+        <v>0</v>
+      </c>
+      <c r="H143" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4774,9 +5604,15 @@
       <c r="F144" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G144" t="inlineStr">
-        <is>
-          <t>2923</t>
+      <c r="G144" t="n">
+        <v>2923</v>
+      </c>
+      <c r="H144" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>2930</t>
         </is>
       </c>
     </row>
@@ -4802,10 +5638,16 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F145" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G145" t="inlineStr">
+      <c r="F145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G145" t="n">
+        <v>0</v>
+      </c>
+      <c r="H145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4833,10 +5675,16 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F146" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G146" t="inlineStr">
+      <c r="F146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G146" t="n">
+        <v>0</v>
+      </c>
+      <c r="H146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4867,9 +5715,15 @@
       <c r="F147" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="G147" t="inlineStr">
-        <is>
-          <t>2028</t>
+      <c r="G147" t="n">
+        <v>2028</v>
+      </c>
+      <c r="H147" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>2042</t>
         </is>
       </c>
     </row>
@@ -4895,10 +5749,16 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F148" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G148" t="inlineStr">
+      <c r="F148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G148" t="n">
+        <v>0</v>
+      </c>
+      <c r="H148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4926,10 +5786,16 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F149" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G149" t="inlineStr">
+      <c r="F149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G149" t="n">
+        <v>0</v>
+      </c>
+      <c r="H149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4957,10 +5823,16 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F150" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G150" t="inlineStr">
+      <c r="F150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G150" t="n">
+        <v>2530</v>
+      </c>
+      <c r="H150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I150" t="inlineStr">
         <is>
           <t>2530</t>
         </is>
@@ -4988,10 +5860,16 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F151" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G151" t="inlineStr">
+      <c r="F151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G151" t="n">
+        <v>0</v>
+      </c>
+      <c r="H151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5019,10 +5897,16 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F152" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G152" t="inlineStr">
+      <c r="F152" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G152" t="n">
+        <v>0</v>
+      </c>
+      <c r="H152" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5050,10 +5934,16 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F153" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G153" t="inlineStr">
+      <c r="F153" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G153" t="n">
+        <v>0</v>
+      </c>
+      <c r="H153" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5084,9 +5974,15 @@
       <c r="F154" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G154" t="inlineStr">
-        <is>
-          <t>2911</t>
+      <c r="G154" t="n">
+        <v>2911</v>
+      </c>
+      <c r="H154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>2893</t>
         </is>
       </c>
     </row>
@@ -5112,10 +6008,16 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F155" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G155" t="inlineStr">
+      <c r="F155" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G155" t="n">
+        <v>0</v>
+      </c>
+      <c r="H155" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5143,10 +6045,16 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F156" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G156" t="inlineStr">
+      <c r="F156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G156" t="n">
+        <v>0</v>
+      </c>
+      <c r="H156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5174,10 +6082,16 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F157" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G157" t="inlineStr">
+      <c r="F157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G157" t="n">
+        <v>0</v>
+      </c>
+      <c r="H157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5205,20 +6119,24 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F158" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G158" t="inlineStr">
-        <is>
-          <t>2783</t>
+      <c r="F158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G158" t="n">
+        <v>2783</v>
+      </c>
+      <c r="H158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>2850</t>
         </is>
       </c>
     </row>
     <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>47227626</t>
-        </is>
+      <c r="A159" t="n">
+        <v>47227626</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
@@ -5235,17 +6153,21 @@
       <c r="F159" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="G159" t="inlineStr">
-        <is>
-          <t>2711</t>
+      <c r="G159" t="n">
+        <v>2711</v>
+      </c>
+      <c r="H159" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>2721</t>
         </is>
       </c>
     </row>
     <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>55317038</t>
-        </is>
+      <c r="A160" t="n">
+        <v>55317038</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
@@ -5262,17 +6184,21 @@
       <c r="F160" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G160" t="inlineStr">
-        <is>
-          <t>3951</t>
+      <c r="G160" t="n">
+        <v>3951</v>
+      </c>
+      <c r="H160" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>4041</t>
         </is>
       </c>
     </row>
     <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>56829330</t>
-        </is>
+      <c r="A161" t="n">
+        <v>56829330</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
@@ -5289,17 +6215,15 @@
       <c r="F161" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="G161" t="inlineStr">
-        <is>
-          <t>3489</t>
-        </is>
-      </c>
+      <c r="G161" t="n">
+        <v>3489</v>
+      </c>
+      <c r="H161" s="2" t="inlineStr"/>
+      <c r="I161" t="inlineStr"/>
     </row>
     <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>48738257</t>
-        </is>
+      <c r="A162" t="n">
+        <v>48738257</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
@@ -5313,20 +6237,24 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F162" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G162" t="inlineStr">
-        <is>
-          <t>3083</t>
+      <c r="F162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G162" t="n">
+        <v>3083</v>
+      </c>
+      <c r="H162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>3148</t>
         </is>
       </c>
     </row>
     <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>58940575</t>
-        </is>
+      <c r="A163" t="n">
+        <v>58940575</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
@@ -5343,9 +6271,44 @@
       <c r="F163" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G163" t="inlineStr">
-        <is>
-          <t>2462</t>
+      <c r="G163" t="n">
+        <v>2462</v>
+      </c>
+      <c r="H163" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>2506</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>12434456</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Player-12434456</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr"/>
+      <c r="D164" t="inlineStr"/>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F164" s="2" t="inlineStr"/>
+      <c r="G164" t="inlineStr"/>
+      <c r="H164" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>2884</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-17 12:38:54
</commit_message>
<xml_diff>
--- a/Season_Attack/86.xlsx
+++ b/Season_Attack/86.xlsx
@@ -6284,10 +6284,8 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>12434456</t>
-        </is>
+      <c r="A164" t="n">
+        <v>12434456</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-03-18 11:31:05
</commit_message>
<xml_diff>
--- a/Season_Attack/86.xlsx
+++ b/Season_Attack/86.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I164"/>
+  <dimension ref="A1:K164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,6 +436,16 @@
           <t>03-16_0</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>03-17_A</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>03-17_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -468,9 +478,15 @@
       <c r="H2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>2939</t>
+      <c r="I2" t="n">
+        <v>2939</v>
+      </c>
+      <c r="J2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>3013</t>
         </is>
       </c>
     </row>
@@ -505,11 +521,11 @@
       <c r="H3" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>4314</t>
-        </is>
-      </c>
+      <c r="I3" t="n">
+        <v>4314</v>
+      </c>
+      <c r="J3" s="2" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -542,9 +558,15 @@
       <c r="H4" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>4506</t>
+      <c r="I4" t="n">
+        <v>4506</v>
+      </c>
+      <c r="J4" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>4908</t>
         </is>
       </c>
     </row>
@@ -579,9 +601,15 @@
       <c r="H5" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>4409</t>
+      <c r="I5" t="n">
+        <v>4409</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>4815</t>
         </is>
       </c>
     </row>
@@ -616,9 +644,15 @@
       <c r="H6" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>4269</t>
+      <c r="I6" t="n">
+        <v>4269</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>4594</t>
         </is>
       </c>
     </row>
@@ -653,9 +687,15 @@
       <c r="H7" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>4776</t>
+      <c r="I7" t="n">
+        <v>4776</v>
+      </c>
+      <c r="J7" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>4989</t>
         </is>
       </c>
     </row>
@@ -690,9 +730,15 @@
       <c r="H8" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>4120</t>
+      <c r="I8" t="n">
+        <v>4120</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>4414</t>
         </is>
       </c>
     </row>
@@ -727,9 +773,15 @@
       <c r="H9" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>4483</t>
+      <c r="I9" t="n">
+        <v>4483</v>
+      </c>
+      <c r="J9" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>4656</t>
         </is>
       </c>
     </row>
@@ -764,9 +816,15 @@
       <c r="H10" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>4464</t>
+      <c r="I10" t="n">
+        <v>4464</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>4794</t>
         </is>
       </c>
     </row>
@@ -801,11 +859,11 @@
       <c r="H11" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>4234</t>
-        </is>
-      </c>
+      <c r="I11" t="n">
+        <v>4234</v>
+      </c>
+      <c r="J11" s="2" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -838,9 +896,15 @@
       <c r="H12" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>2815</t>
+      <c r="I12" t="n">
+        <v>2815</v>
+      </c>
+      <c r="J12" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>3199</t>
         </is>
       </c>
     </row>
@@ -875,9 +939,15 @@
       <c r="H13" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>5103</t>
+      <c r="I13" t="n">
+        <v>5103</v>
+      </c>
+      <c r="J13" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>5496</t>
         </is>
       </c>
     </row>
@@ -912,9 +982,15 @@
       <c r="H14" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>4326</t>
+      <c r="I14" t="n">
+        <v>4326</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>4642</t>
         </is>
       </c>
     </row>
@@ -940,6 +1016,8 @@
       <c r="G15" t="inlineStr"/>
       <c r="H15" s="2" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
+      <c r="J15" s="2" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -972,9 +1050,15 @@
       <c r="H16" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>4155</t>
+      <c r="I16" t="n">
+        <v>4155</v>
+      </c>
+      <c r="J16" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>4280</t>
         </is>
       </c>
     </row>
@@ -1009,9 +1093,15 @@
       <c r="H17" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>4053</t>
+      <c r="I17" t="n">
+        <v>4053</v>
+      </c>
+      <c r="J17" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>4154</t>
         </is>
       </c>
     </row>
@@ -1046,9 +1136,15 @@
       <c r="H18" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>4133</t>
+      <c r="I18" t="n">
+        <v>4133</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>4457</t>
         </is>
       </c>
     </row>
@@ -1074,6 +1170,8 @@
       <c r="G19" t="inlineStr"/>
       <c r="H19" s="2" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
+      <c r="J19" s="2" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1106,9 +1204,15 @@
       <c r="H20" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>3467</t>
+      <c r="I20" t="n">
+        <v>3467</v>
+      </c>
+      <c r="J20" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>3782</t>
         </is>
       </c>
     </row>
@@ -1143,9 +1247,15 @@
       <c r="H21" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>4594</t>
+      <c r="I21" t="n">
+        <v>4594</v>
+      </c>
+      <c r="J21" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>4908</t>
         </is>
       </c>
     </row>
@@ -1180,9 +1290,15 @@
       <c r="H22" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>3446</t>
+      <c r="I22" t="n">
+        <v>3446</v>
+      </c>
+      <c r="J22" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>4053</t>
         </is>
       </c>
     </row>
@@ -1217,9 +1333,15 @@
       <c r="H23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>4458</t>
+      <c r="I23" t="n">
+        <v>4458</v>
+      </c>
+      <c r="J23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>4915</t>
         </is>
       </c>
     </row>
@@ -1254,7 +1376,13 @@
       <c r="H24" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I24" t="inlineStr">
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1291,7 +1419,13 @@
       <c r="H25" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="I25" t="n">
+        <v>2588</v>
+      </c>
+      <c r="J25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="inlineStr">
         <is>
           <t>2588</t>
         </is>
@@ -1319,6 +1453,8 @@
       <c r="G26" t="inlineStr"/>
       <c r="H26" s="2" t="inlineStr"/>
       <c r="I26" t="inlineStr"/>
+      <c r="J26" s="2" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1342,6 +1478,8 @@
       <c r="G27" t="inlineStr"/>
       <c r="H27" s="2" t="inlineStr"/>
       <c r="I27" t="inlineStr"/>
+      <c r="J27" s="2" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1374,9 +1512,15 @@
       <c r="H28" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>4962</t>
+      <c r="I28" t="n">
+        <v>4962</v>
+      </c>
+      <c r="J28" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>5119</t>
         </is>
       </c>
     </row>
@@ -1402,6 +1546,8 @@
       <c r="G29" t="inlineStr"/>
       <c r="H29" s="2" t="inlineStr"/>
       <c r="I29" t="inlineStr"/>
+      <c r="J29" s="2" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1434,9 +1580,15 @@
       <c r="H30" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>3854</t>
+      <c r="I30" t="n">
+        <v>3854</v>
+      </c>
+      <c r="J30" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>3974</t>
         </is>
       </c>
     </row>
@@ -1471,9 +1623,15 @@
       <c r="H31" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>4954</t>
+      <c r="I31" t="n">
+        <v>4954</v>
+      </c>
+      <c r="J31" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>5340</t>
         </is>
       </c>
     </row>
@@ -1508,11 +1666,11 @@
       <c r="H32" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>3562</t>
-        </is>
-      </c>
+      <c r="I32" t="n">
+        <v>3562</v>
+      </c>
+      <c r="J32" s="2" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1545,9 +1703,15 @@
       <c r="H33" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>4444</t>
+      <c r="I33" t="n">
+        <v>4444</v>
+      </c>
+      <c r="J33" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>4755</t>
         </is>
       </c>
     </row>
@@ -1582,9 +1746,15 @@
       <c r="H34" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>4390</t>
+      <c r="I34" t="n">
+        <v>4390</v>
+      </c>
+      <c r="J34" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>4983</t>
         </is>
       </c>
     </row>
@@ -1619,9 +1789,15 @@
       <c r="H35" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>4086</t>
+      <c r="I35" t="n">
+        <v>4086</v>
+      </c>
+      <c r="J35" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>4381</t>
         </is>
       </c>
     </row>
@@ -1647,6 +1823,8 @@
       <c r="G36" t="inlineStr"/>
       <c r="H36" s="2" t="inlineStr"/>
       <c r="I36" t="inlineStr"/>
+      <c r="J36" s="2" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1679,9 +1857,15 @@
       <c r="H37" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>4585</t>
+      <c r="I37" t="n">
+        <v>4585</v>
+      </c>
+      <c r="J37" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>4862</t>
         </is>
       </c>
     </row>
@@ -1716,9 +1900,15 @@
       <c r="H38" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>4624</t>
+      <c r="I38" t="n">
+        <v>4624</v>
+      </c>
+      <c r="J38" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>4737</t>
         </is>
       </c>
     </row>
@@ -1753,9 +1943,15 @@
       <c r="H39" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>4568</t>
+      <c r="I39" t="n">
+        <v>4568</v>
+      </c>
+      <c r="J39" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>4934</t>
         </is>
       </c>
     </row>
@@ -1790,9 +1986,15 @@
       <c r="H40" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>4921</t>
+      <c r="I40" t="n">
+        <v>4921</v>
+      </c>
+      <c r="J40" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>5132</t>
         </is>
       </c>
     </row>
@@ -1827,9 +2029,15 @@
       <c r="H41" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>4775</t>
+      <c r="I41" t="n">
+        <v>4775</v>
+      </c>
+      <c r="J41" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>5065</t>
         </is>
       </c>
     </row>
@@ -1864,9 +2072,15 @@
       <c r="H42" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>4440</t>
+      <c r="I42" t="n">
+        <v>4440</v>
+      </c>
+      <c r="J42" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>4732</t>
         </is>
       </c>
     </row>
@@ -1901,9 +2115,15 @@
       <c r="H43" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>4191</t>
+      <c r="I43" t="n">
+        <v>4191</v>
+      </c>
+      <c r="J43" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>4410</t>
         </is>
       </c>
     </row>
@@ -1938,9 +2158,15 @@
       <c r="H44" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>4135</t>
+      <c r="I44" t="n">
+        <v>4135</v>
+      </c>
+      <c r="J44" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>4480</t>
         </is>
       </c>
     </row>
@@ -1975,9 +2201,15 @@
       <c r="H45" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>4098</t>
+      <c r="I45" t="n">
+        <v>4098</v>
+      </c>
+      <c r="J45" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>4133</t>
         </is>
       </c>
     </row>
@@ -2012,9 +2244,15 @@
       <c r="H46" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>4767</t>
+      <c r="I46" t="n">
+        <v>4767</v>
+      </c>
+      <c r="J46" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>5004</t>
         </is>
       </c>
     </row>
@@ -2049,9 +2287,15 @@
       <c r="H47" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>3947</t>
+      <c r="I47" t="n">
+        <v>3947</v>
+      </c>
+      <c r="J47" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>4186</t>
         </is>
       </c>
     </row>
@@ -2086,9 +2330,15 @@
       <c r="H48" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="I48" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J48" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>2516</t>
         </is>
       </c>
     </row>
@@ -2114,6 +2364,8 @@
       <c r="G49" t="inlineStr"/>
       <c r="H49" s="2" t="inlineStr"/>
       <c r="I49" t="inlineStr"/>
+      <c r="J49" s="2" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -2146,7 +2398,13 @@
       <c r="H50" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I50" t="inlineStr">
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K50" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2183,9 +2441,15 @@
       <c r="H51" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>2547</t>
+      <c r="I51" t="n">
+        <v>2547</v>
+      </c>
+      <c r="J51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>2592</t>
         </is>
       </c>
     </row>
@@ -2220,7 +2484,13 @@
       <c r="H52" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I52" t="inlineStr">
+      <c r="I52" t="n">
+        <v>2801</v>
+      </c>
+      <c r="J52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" t="inlineStr">
         <is>
           <t>2801</t>
         </is>
@@ -2257,9 +2527,15 @@
       <c r="H53" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>4451</t>
+      <c r="I53" t="n">
+        <v>4451</v>
+      </c>
+      <c r="J53" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>4723</t>
         </is>
       </c>
     </row>
@@ -2294,9 +2570,15 @@
       <c r="H54" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>4086</t>
+      <c r="I54" t="n">
+        <v>4086</v>
+      </c>
+      <c r="J54" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>4196</t>
         </is>
       </c>
     </row>
@@ -2331,9 +2613,15 @@
       <c r="H55" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>3972</t>
+      <c r="I55" t="n">
+        <v>3972</v>
+      </c>
+      <c r="J55" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>4145</t>
         </is>
       </c>
     </row>
@@ -2368,9 +2656,15 @@
       <c r="H56" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>4266</t>
+      <c r="I56" t="n">
+        <v>4266</v>
+      </c>
+      <c r="J56" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>4530</t>
         </is>
       </c>
     </row>
@@ -2405,9 +2699,15 @@
       <c r="H57" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>4056</t>
+      <c r="I57" t="n">
+        <v>4056</v>
+      </c>
+      <c r="J57" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>4293</t>
         </is>
       </c>
     </row>
@@ -2442,9 +2742,15 @@
       <c r="H58" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>4010</t>
+      <c r="I58" t="n">
+        <v>4010</v>
+      </c>
+      <c r="J58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>4051</t>
         </is>
       </c>
     </row>
@@ -2479,7 +2785,13 @@
       <c r="H59" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I59" t="inlineStr">
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2516,9 +2828,15 @@
       <c r="H60" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>4433</t>
+      <c r="I60" t="n">
+        <v>4433</v>
+      </c>
+      <c r="J60" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>4693</t>
         </is>
       </c>
     </row>
@@ -2553,9 +2871,15 @@
       <c r="H61" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>2496</t>
+      <c r="I61" t="n">
+        <v>2496</v>
+      </c>
+      <c r="J61" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>2742</t>
         </is>
       </c>
     </row>
@@ -2590,9 +2914,15 @@
       <c r="H62" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>3251</t>
+      <c r="I62" t="n">
+        <v>3251</v>
+      </c>
+      <c r="J62" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>3241</t>
         </is>
       </c>
     </row>
@@ -2627,9 +2957,15 @@
       <c r="H63" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>4134</t>
+      <c r="I63" t="n">
+        <v>4134</v>
+      </c>
+      <c r="J63" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>4462</t>
         </is>
       </c>
     </row>
@@ -2664,9 +3000,15 @@
       <c r="H64" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>4346</t>
+      <c r="I64" t="n">
+        <v>4346</v>
+      </c>
+      <c r="J64" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>4612</t>
         </is>
       </c>
     </row>
@@ -2701,9 +3043,15 @@
       <c r="H65" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>2930</t>
+      <c r="I65" t="n">
+        <v>2930</v>
+      </c>
+      <c r="J65" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>2951</t>
         </is>
       </c>
     </row>
@@ -2738,9 +3086,15 @@
       <c r="H66" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>4089</t>
+      <c r="I66" t="n">
+        <v>4089</v>
+      </c>
+      <c r="J66" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>4251</t>
         </is>
       </c>
     </row>
@@ -2775,9 +3129,15 @@
       <c r="H67" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t>2653</t>
+      <c r="I67" t="n">
+        <v>2653</v>
+      </c>
+      <c r="J67" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>2803</t>
         </is>
       </c>
     </row>
@@ -2812,7 +3172,13 @@
       <c r="H68" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I68" t="inlineStr">
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2849,9 +3215,15 @@
       <c r="H69" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I69" t="inlineStr">
-        <is>
-          <t>4109</t>
+      <c r="I69" t="n">
+        <v>4109</v>
+      </c>
+      <c r="J69" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>4079</t>
         </is>
       </c>
     </row>
@@ -2886,9 +3258,15 @@
       <c r="H70" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>3962</t>
+      <c r="I70" t="n">
+        <v>3962</v>
+      </c>
+      <c r="J70" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>4146</t>
         </is>
       </c>
     </row>
@@ -2923,9 +3301,15 @@
       <c r="H71" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>2685</t>
+      <c r="I71" t="n">
+        <v>2685</v>
+      </c>
+      <c r="J71" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>2781</t>
         </is>
       </c>
     </row>
@@ -2960,9 +3344,15 @@
       <c r="H72" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>4000</t>
+      <c r="I72" t="n">
+        <v>4000</v>
+      </c>
+      <c r="J72" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>4114</t>
         </is>
       </c>
     </row>
@@ -2997,9 +3387,15 @@
       <c r="H73" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>4357</t>
+      <c r="I73" t="n">
+        <v>4357</v>
+      </c>
+      <c r="J73" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>4551</t>
         </is>
       </c>
     </row>
@@ -3034,7 +3430,13 @@
       <c r="H74" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I74" t="inlineStr">
+      <c r="I74" t="n">
+        <v>0</v>
+      </c>
+      <c r="J74" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3071,7 +3473,13 @@
       <c r="H75" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I75" t="inlineStr">
+      <c r="I75" t="n">
+        <v>0</v>
+      </c>
+      <c r="J75" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3108,9 +3516,15 @@
       <c r="H76" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I76" t="inlineStr">
-        <is>
-          <t>4362</t>
+      <c r="I76" t="n">
+        <v>4362</v>
+      </c>
+      <c r="J76" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>4563</t>
         </is>
       </c>
     </row>
@@ -3145,7 +3559,13 @@
       <c r="H77" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I77" t="inlineStr">
+      <c r="I77" t="n">
+        <v>0</v>
+      </c>
+      <c r="J77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3182,9 +3602,15 @@
       <c r="H78" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="I78" t="inlineStr">
-        <is>
-          <t>4260</t>
+      <c r="I78" t="n">
+        <v>4260</v>
+      </c>
+      <c r="J78" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>4487</t>
         </is>
       </c>
     </row>
@@ -3219,9 +3645,15 @@
       <c r="H79" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>3041</t>
+      <c r="I79" t="n">
+        <v>3041</v>
+      </c>
+      <c r="J79" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>3175</t>
         </is>
       </c>
     </row>
@@ -3247,6 +3679,8 @@
       <c r="G80" t="inlineStr"/>
       <c r="H80" s="2" t="inlineStr"/>
       <c r="I80" t="inlineStr"/>
+      <c r="J80" s="2" t="inlineStr"/>
+      <c r="K80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -3279,9 +3713,15 @@
       <c r="H81" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>4319</t>
+      <c r="I81" t="n">
+        <v>4319</v>
+      </c>
+      <c r="J81" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>4446</t>
         </is>
       </c>
     </row>
@@ -3316,9 +3756,15 @@
       <c r="H82" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>4286</t>
+      <c r="I82" t="n">
+        <v>4286</v>
+      </c>
+      <c r="J82" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>4415</t>
         </is>
       </c>
     </row>
@@ -3353,9 +3799,15 @@
       <c r="H83" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I83" t="inlineStr">
-        <is>
-          <t>4138</t>
+      <c r="I83" t="n">
+        <v>4138</v>
+      </c>
+      <c r="J83" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>4185</t>
         </is>
       </c>
     </row>
@@ -3390,9 +3842,15 @@
       <c r="H84" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>3673</t>
+      <c r="I84" t="n">
+        <v>3673</v>
+      </c>
+      <c r="J84" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>4050</t>
         </is>
       </c>
     </row>
@@ -3427,9 +3885,15 @@
       <c r="H85" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I85" t="inlineStr">
-        <is>
-          <t>4008</t>
+      <c r="I85" t="n">
+        <v>4008</v>
+      </c>
+      <c r="J85" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>4128</t>
         </is>
       </c>
     </row>
@@ -3464,9 +3928,15 @@
       <c r="H86" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>2791</t>
+      <c r="I86" t="n">
+        <v>2791</v>
+      </c>
+      <c r="J86" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>2836</t>
         </is>
       </c>
     </row>
@@ -3501,9 +3971,15 @@
       <c r="H87" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>4217</t>
+      <c r="I87" t="n">
+        <v>4217</v>
+      </c>
+      <c r="J87" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>4370</t>
         </is>
       </c>
     </row>
@@ -3538,9 +4014,15 @@
       <c r="H88" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I88" t="inlineStr">
-        <is>
-          <t>3048</t>
+      <c r="I88" t="n">
+        <v>3048</v>
+      </c>
+      <c r="J88" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>3165</t>
         </is>
       </c>
     </row>
@@ -3575,9 +4057,15 @@
       <c r="H89" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I89" t="inlineStr">
-        <is>
-          <t>3588</t>
+      <c r="I89" t="n">
+        <v>3588</v>
+      </c>
+      <c r="J89" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>3770</t>
         </is>
       </c>
     </row>
@@ -3612,9 +4100,15 @@
       <c r="H90" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>2875</t>
+      <c r="I90" t="n">
+        <v>2875</v>
+      </c>
+      <c r="J90" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>2868</t>
         </is>
       </c>
     </row>
@@ -3649,9 +4143,15 @@
       <c r="H91" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I91" t="inlineStr">
-        <is>
-          <t>3360</t>
+      <c r="I91" t="n">
+        <v>3360</v>
+      </c>
+      <c r="J91" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>3472</t>
         </is>
       </c>
     </row>
@@ -3686,7 +4186,13 @@
       <c r="H92" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I92" t="inlineStr">
+      <c r="I92" t="n">
+        <v>0</v>
+      </c>
+      <c r="J92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3723,9 +4229,15 @@
       <c r="H93" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I93" t="inlineStr">
-        <is>
-          <t>3238</t>
+      <c r="I93" t="n">
+        <v>3238</v>
+      </c>
+      <c r="J93" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>3479</t>
         </is>
       </c>
     </row>
@@ -3760,7 +4272,13 @@
       <c r="H94" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I94" t="inlineStr">
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
+      <c r="J94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3797,9 +4315,15 @@
       <c r="H95" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I95" t="inlineStr">
-        <is>
-          <t>3545</t>
+      <c r="I95" t="n">
+        <v>3545</v>
+      </c>
+      <c r="J95" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>3816</t>
         </is>
       </c>
     </row>
@@ -3834,9 +4358,15 @@
       <c r="H96" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>2512</t>
+      <c r="I96" t="n">
+        <v>2512</v>
+      </c>
+      <c r="J96" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>2564</t>
         </is>
       </c>
     </row>
@@ -3871,9 +4401,15 @@
       <c r="H97" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I97" t="inlineStr">
-        <is>
-          <t>2119</t>
+      <c r="I97" t="n">
+        <v>2119</v>
+      </c>
+      <c r="J97" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>2114</t>
         </is>
       </c>
     </row>
@@ -3908,9 +4444,15 @@
       <c r="H98" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I98" t="inlineStr">
-        <is>
-          <t>2858</t>
+      <c r="I98" t="n">
+        <v>2858</v>
+      </c>
+      <c r="J98" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>3174</t>
         </is>
       </c>
     </row>
@@ -3945,9 +4487,15 @@
       <c r="H99" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I99" t="inlineStr">
-        <is>
-          <t>2506</t>
+      <c r="I99" t="n">
+        <v>2506</v>
+      </c>
+      <c r="J99" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>2515</t>
         </is>
       </c>
     </row>
@@ -3982,9 +4530,15 @@
       <c r="H100" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>3372</t>
+      <c r="I100" t="n">
+        <v>3372</v>
+      </c>
+      <c r="J100" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>3517</t>
         </is>
       </c>
     </row>
@@ -4019,9 +4573,15 @@
       <c r="H101" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>2248</t>
+      <c r="I101" t="n">
+        <v>2248</v>
+      </c>
+      <c r="J101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>2305</t>
         </is>
       </c>
     </row>
@@ -4056,9 +4616,15 @@
       <c r="H102" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I102" t="inlineStr">
-        <is>
-          <t>4190</t>
+      <c r="I102" t="n">
+        <v>4190</v>
+      </c>
+      <c r="J102" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>4376</t>
         </is>
       </c>
     </row>
@@ -4093,9 +4659,15 @@
       <c r="H103" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I103" t="inlineStr">
-        <is>
-          <t>3640</t>
+      <c r="I103" t="n">
+        <v>3640</v>
+      </c>
+      <c r="J103" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>3928</t>
         </is>
       </c>
     </row>
@@ -4130,9 +4702,15 @@
       <c r="H104" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>3775</t>
+      <c r="I104" t="n">
+        <v>3775</v>
+      </c>
+      <c r="J104" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>4017</t>
         </is>
       </c>
     </row>
@@ -4167,9 +4745,15 @@
       <c r="H105" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I105" t="inlineStr">
-        <is>
-          <t>4108</t>
+      <c r="I105" t="n">
+        <v>4108</v>
+      </c>
+      <c r="J105" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>4268</t>
         </is>
       </c>
     </row>
@@ -4204,9 +4788,15 @@
       <c r="H106" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="I106" t="inlineStr">
-        <is>
-          <t>4041</t>
+      <c r="I106" t="n">
+        <v>4041</v>
+      </c>
+      <c r="J106" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>4068</t>
         </is>
       </c>
     </row>
@@ -4241,9 +4831,15 @@
       <c r="H107" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I107" t="inlineStr">
-        <is>
-          <t>3839</t>
+      <c r="I107" t="n">
+        <v>3839</v>
+      </c>
+      <c r="J107" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>4048</t>
         </is>
       </c>
     </row>
@@ -4278,7 +4874,13 @@
       <c r="H108" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I108" t="inlineStr">
+      <c r="I108" t="n">
+        <v>0</v>
+      </c>
+      <c r="J108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4315,9 +4917,15 @@
       <c r="H109" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I109" t="inlineStr">
-        <is>
-          <t>2861</t>
+      <c r="I109" t="n">
+        <v>2861</v>
+      </c>
+      <c r="J109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>2859</t>
         </is>
       </c>
     </row>
@@ -4352,7 +4960,13 @@
       <c r="H110" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I110" t="inlineStr">
+      <c r="I110" t="n">
+        <v>0</v>
+      </c>
+      <c r="J110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K110" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4389,9 +5003,15 @@
       <c r="H111" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I111" t="inlineStr">
-        <is>
-          <t>3372</t>
+      <c r="I111" t="n">
+        <v>3372</v>
+      </c>
+      <c r="J111" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>3827</t>
         </is>
       </c>
     </row>
@@ -4426,9 +5046,15 @@
       <c r="H112" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I112" t="inlineStr">
-        <is>
-          <t>3982</t>
+      <c r="I112" t="n">
+        <v>3982</v>
+      </c>
+      <c r="J112" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>4003</t>
         </is>
       </c>
     </row>
@@ -4463,9 +5089,15 @@
       <c r="H113" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I113" t="inlineStr">
-        <is>
-          <t>3328</t>
+      <c r="I113" t="n">
+        <v>3328</v>
+      </c>
+      <c r="J113" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>3640</t>
         </is>
       </c>
     </row>
@@ -4500,9 +5132,15 @@
       <c r="H114" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I114" t="inlineStr">
-        <is>
-          <t>2556</t>
+      <c r="I114" t="n">
+        <v>2556</v>
+      </c>
+      <c r="J114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>2552</t>
         </is>
       </c>
     </row>
@@ -4537,9 +5175,15 @@
       <c r="H115" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I115" t="inlineStr">
-        <is>
-          <t>3456</t>
+      <c r="I115" t="n">
+        <v>3456</v>
+      </c>
+      <c r="J115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>3563</t>
         </is>
       </c>
     </row>
@@ -4574,9 +5218,15 @@
       <c r="H116" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I116" t="inlineStr">
-        <is>
-          <t>3000</t>
+      <c r="I116" t="n">
+        <v>3000</v>
+      </c>
+      <c r="J116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>3055</t>
         </is>
       </c>
     </row>
@@ -4611,9 +5261,15 @@
       <c r="H117" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I117" t="inlineStr">
-        <is>
-          <t>2385</t>
+      <c r="I117" t="n">
+        <v>2385</v>
+      </c>
+      <c r="J117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>2397</t>
         </is>
       </c>
     </row>
@@ -4648,9 +5304,15 @@
       <c r="H118" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I118" t="inlineStr">
-        <is>
-          <t>2945</t>
+      <c r="I118" t="n">
+        <v>2945</v>
+      </c>
+      <c r="J118" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>3024</t>
         </is>
       </c>
     </row>
@@ -4685,9 +5347,15 @@
       <c r="H119" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I119" t="inlineStr">
-        <is>
-          <t>4014</t>
+      <c r="I119" t="n">
+        <v>4014</v>
+      </c>
+      <c r="J119" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>4021</t>
         </is>
       </c>
     </row>
@@ -4722,9 +5390,15 @@
       <c r="H120" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I120" t="inlineStr">
-        <is>
-          <t>2517</t>
+      <c r="I120" t="n">
+        <v>2517</v>
+      </c>
+      <c r="J120" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>2585</t>
         </is>
       </c>
     </row>
@@ -4759,9 +5433,15 @@
       <c r="H121" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I121" t="inlineStr">
-        <is>
-          <t>1575</t>
+      <c r="I121" t="n">
+        <v>1575</v>
+      </c>
+      <c r="J121" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>1574</t>
         </is>
       </c>
     </row>
@@ -4796,9 +5476,15 @@
       <c r="H122" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I122" t="inlineStr">
-        <is>
-          <t>2506</t>
+      <c r="I122" t="n">
+        <v>2506</v>
+      </c>
+      <c r="J122" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>2694</t>
         </is>
       </c>
     </row>
@@ -4833,9 +5519,15 @@
       <c r="H123" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I123" t="inlineStr">
-        <is>
-          <t>3872</t>
+      <c r="I123" t="n">
+        <v>3872</v>
+      </c>
+      <c r="J123" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>4029</t>
         </is>
       </c>
     </row>
@@ -4870,7 +5562,13 @@
       <c r="H124" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I124" t="inlineStr">
+      <c r="I124" t="n">
+        <v>0</v>
+      </c>
+      <c r="J124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K124" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4907,9 +5605,15 @@
       <c r="H125" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="I125" t="inlineStr">
-        <is>
-          <t>3547</t>
+      <c r="I125" t="n">
+        <v>3547</v>
+      </c>
+      <c r="J125" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>3807</t>
         </is>
       </c>
     </row>
@@ -4944,9 +5648,15 @@
       <c r="H126" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="I126" t="inlineStr">
-        <is>
-          <t>3548</t>
+      <c r="I126" t="n">
+        <v>3548</v>
+      </c>
+      <c r="J126" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>3646</t>
         </is>
       </c>
     </row>
@@ -4981,9 +5691,15 @@
       <c r="H127" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I127" t="inlineStr">
-        <is>
-          <t>3040</t>
+      <c r="I127" t="n">
+        <v>3040</v>
+      </c>
+      <c r="J127" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>3301</t>
         </is>
       </c>
     </row>
@@ -5018,9 +5734,15 @@
       <c r="H128" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I128" t="inlineStr">
-        <is>
-          <t>3786</t>
+      <c r="I128" t="n">
+        <v>3786</v>
+      </c>
+      <c r="J128" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>3980</t>
         </is>
       </c>
     </row>
@@ -5055,9 +5777,15 @@
       <c r="H129" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I129" t="inlineStr">
-        <is>
-          <t>2025</t>
+      <c r="I129" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>2021</t>
         </is>
       </c>
     </row>
@@ -5092,7 +5820,13 @@
       <c r="H130" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I130" t="inlineStr">
+      <c r="I130" t="n">
+        <v>0</v>
+      </c>
+      <c r="J130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5129,7 +5863,13 @@
       <c r="H131" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I131" t="inlineStr">
+      <c r="I131" t="n">
+        <v>0</v>
+      </c>
+      <c r="J131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5166,9 +5906,15 @@
       <c r="H132" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I132" t="inlineStr">
-        <is>
-          <t>3440</t>
+      <c r="I132" t="n">
+        <v>3440</v>
+      </c>
+      <c r="J132" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>3663</t>
         </is>
       </c>
     </row>
@@ -5203,7 +5949,13 @@
       <c r="H133" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I133" t="inlineStr">
+      <c r="I133" t="n">
+        <v>0</v>
+      </c>
+      <c r="J133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5240,9 +5992,15 @@
       <c r="H134" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I134" t="inlineStr">
-        <is>
-          <t>2979</t>
+      <c r="I134" t="n">
+        <v>2979</v>
+      </c>
+      <c r="J134" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>3104</t>
         </is>
       </c>
     </row>
@@ -5277,9 +6035,15 @@
       <c r="H135" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I135" t="inlineStr">
-        <is>
-          <t>3809</t>
+      <c r="I135" t="n">
+        <v>3809</v>
+      </c>
+      <c r="J135" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>3991</t>
         </is>
       </c>
     </row>
@@ -5314,9 +6078,15 @@
       <c r="H136" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I136" t="inlineStr">
-        <is>
-          <t>3632</t>
+      <c r="I136" t="n">
+        <v>3632</v>
+      </c>
+      <c r="J136" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>3913</t>
         </is>
       </c>
     </row>
@@ -5351,7 +6121,13 @@
       <c r="H137" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I137" t="inlineStr">
+      <c r="I137" t="n">
+        <v>0</v>
+      </c>
+      <c r="J137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5388,9 +6164,15 @@
       <c r="H138" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I138" t="inlineStr">
-        <is>
-          <t>1499</t>
+      <c r="I138" t="n">
+        <v>1499</v>
+      </c>
+      <c r="J138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -5425,9 +6207,15 @@
       <c r="H139" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="I139" t="inlineStr">
-        <is>
-          <t>3057</t>
+      <c r="I139" t="n">
+        <v>3057</v>
+      </c>
+      <c r="J139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>3072</t>
         </is>
       </c>
     </row>
@@ -5462,7 +6250,13 @@
       <c r="H140" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I140" t="inlineStr">
+      <c r="I140" t="n">
+        <v>0</v>
+      </c>
+      <c r="J140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5499,7 +6293,13 @@
       <c r="H141" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I141" t="inlineStr">
+      <c r="I141" t="n">
+        <v>0</v>
+      </c>
+      <c r="J141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5536,9 +6336,15 @@
       <c r="H142" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I142" t="inlineStr">
-        <is>
-          <t>3168</t>
+      <c r="I142" t="n">
+        <v>3168</v>
+      </c>
+      <c r="J142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>3147</t>
         </is>
       </c>
     </row>
@@ -5573,7 +6379,13 @@
       <c r="H143" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I143" t="inlineStr">
+      <c r="I143" t="n">
+        <v>0</v>
+      </c>
+      <c r="J143" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5610,9 +6422,15 @@
       <c r="H144" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I144" t="inlineStr">
-        <is>
-          <t>2930</t>
+      <c r="I144" t="n">
+        <v>2930</v>
+      </c>
+      <c r="J144" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>3232</t>
         </is>
       </c>
     </row>
@@ -5647,7 +6465,13 @@
       <c r="H145" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I145" t="inlineStr">
+      <c r="I145" t="n">
+        <v>0</v>
+      </c>
+      <c r="J145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5684,7 +6508,13 @@
       <c r="H146" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I146" t="inlineStr">
+      <c r="I146" t="n">
+        <v>0</v>
+      </c>
+      <c r="J146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5721,9 +6551,15 @@
       <c r="H147" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I147" t="inlineStr">
-        <is>
-          <t>2042</t>
+      <c r="I147" t="n">
+        <v>2042</v>
+      </c>
+      <c r="J147" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>2051</t>
         </is>
       </c>
     </row>
@@ -5758,7 +6594,13 @@
       <c r="H148" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I148" t="inlineStr">
+      <c r="I148" t="n">
+        <v>0</v>
+      </c>
+      <c r="J148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5795,7 +6637,13 @@
       <c r="H149" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I149" t="inlineStr">
+      <c r="I149" t="n">
+        <v>0</v>
+      </c>
+      <c r="J149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5832,7 +6680,13 @@
       <c r="H150" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I150" t="inlineStr">
+      <c r="I150" t="n">
+        <v>2530</v>
+      </c>
+      <c r="J150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K150" t="inlineStr">
         <is>
           <t>2530</t>
         </is>
@@ -5869,7 +6723,13 @@
       <c r="H151" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I151" t="inlineStr">
+      <c r="I151" t="n">
+        <v>0</v>
+      </c>
+      <c r="J151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5906,7 +6766,13 @@
       <c r="H152" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I152" t="inlineStr">
+      <c r="I152" t="n">
+        <v>0</v>
+      </c>
+      <c r="J152" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5943,7 +6809,13 @@
       <c r="H153" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I153" t="inlineStr">
+      <c r="I153" t="n">
+        <v>0</v>
+      </c>
+      <c r="J153" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5980,9 +6852,15 @@
       <c r="H154" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I154" t="inlineStr">
-        <is>
-          <t>2893</t>
+      <c r="I154" t="n">
+        <v>2893</v>
+      </c>
+      <c r="J154" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>2926</t>
         </is>
       </c>
     </row>
@@ -6017,7 +6895,13 @@
       <c r="H155" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I155" t="inlineStr">
+      <c r="I155" t="n">
+        <v>0</v>
+      </c>
+      <c r="J155" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6054,7 +6938,13 @@
       <c r="H156" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I156" t="inlineStr">
+      <c r="I156" t="n">
+        <v>0</v>
+      </c>
+      <c r="J156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6091,7 +6981,13 @@
       <c r="H157" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I157" t="inlineStr">
+      <c r="I157" t="n">
+        <v>0</v>
+      </c>
+      <c r="J157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6128,9 +7024,15 @@
       <c r="H158" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I158" t="inlineStr">
-        <is>
-          <t>2850</t>
+      <c r="I158" t="n">
+        <v>2850</v>
+      </c>
+      <c r="J158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>2884</t>
         </is>
       </c>
     </row>
@@ -6159,9 +7061,15 @@
       <c r="H159" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I159" t="inlineStr">
-        <is>
-          <t>2721</t>
+      <c r="I159" t="n">
+        <v>2721</v>
+      </c>
+      <c r="J159" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>2739</t>
         </is>
       </c>
     </row>
@@ -6190,9 +7098,15 @@
       <c r="H160" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I160" t="inlineStr">
-        <is>
-          <t>4041</t>
+      <c r="I160" t="n">
+        <v>4041</v>
+      </c>
+      <c r="J160" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>4220</t>
         </is>
       </c>
     </row>
@@ -6220,6 +7134,8 @@
       </c>
       <c r="H161" s="2" t="inlineStr"/>
       <c r="I161" t="inlineStr"/>
+      <c r="J161" s="2" t="inlineStr"/>
+      <c r="K161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="n">
@@ -6246,9 +7162,15 @@
       <c r="H162" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I162" t="inlineStr">
-        <is>
-          <t>3148</t>
+      <c r="I162" t="n">
+        <v>3148</v>
+      </c>
+      <c r="J162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>3240</t>
         </is>
       </c>
     </row>
@@ -6277,9 +7199,15 @@
       <c r="H163" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I163" t="inlineStr">
-        <is>
-          <t>2506</t>
+      <c r="I163" t="n">
+        <v>2506</v>
+      </c>
+      <c r="J163" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>2619</t>
         </is>
       </c>
     </row>
@@ -6304,9 +7232,15 @@
       <c r="H164" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="I164" t="inlineStr">
-        <is>
-          <t>2884</t>
+      <c r="I164" t="n">
+        <v>2884</v>
+      </c>
+      <c r="J164" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>2910</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-19 11:30:54
</commit_message>
<xml_diff>
--- a/Season_Attack/86.xlsx
+++ b/Season_Attack/86.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K164"/>
+  <dimension ref="A1:M164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,16 @@
           <t>03-17_0</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>03-18_A</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>03-18_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -484,9 +494,15 @@
       <c r="J2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>3013</t>
+      <c r="K2" t="n">
+        <v>3013</v>
+      </c>
+      <c r="L2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>3042</t>
         </is>
       </c>
     </row>
@@ -526,6 +542,8 @@
       </c>
       <c r="J3" s="2" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
+      <c r="L3" s="2" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -564,9 +582,15 @@
       <c r="J4" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>4908</t>
+      <c r="K4" t="n">
+        <v>4908</v>
+      </c>
+      <c r="L4" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>5190</t>
         </is>
       </c>
     </row>
@@ -607,9 +631,15 @@
       <c r="J5" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>4815</t>
+      <c r="K5" t="n">
+        <v>4815</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>5082</t>
         </is>
       </c>
     </row>
@@ -650,9 +680,15 @@
       <c r="J6" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>4594</t>
+      <c r="K6" t="n">
+        <v>4594</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>4962</t>
         </is>
       </c>
     </row>
@@ -693,9 +729,15 @@
       <c r="J7" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>4989</t>
+      <c r="K7" t="n">
+        <v>4989</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>5278</t>
         </is>
       </c>
     </row>
@@ -736,9 +778,15 @@
       <c r="J8" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>4414</t>
+      <c r="K8" t="n">
+        <v>4414</v>
+      </c>
+      <c r="L8" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>4694</t>
         </is>
       </c>
     </row>
@@ -779,9 +827,15 @@
       <c r="J9" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>4656</t>
+      <c r="K9" t="n">
+        <v>4656</v>
+      </c>
+      <c r="L9" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>4952</t>
         </is>
       </c>
     </row>
@@ -822,9 +876,15 @@
       <c r="J10" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>4794</t>
+      <c r="K10" t="n">
+        <v>4794</v>
+      </c>
+      <c r="L10" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>5027</t>
         </is>
       </c>
     </row>
@@ -864,6 +924,8 @@
       </c>
       <c r="J11" s="2" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
+      <c r="L11" s="2" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -902,9 +964,15 @@
       <c r="J12" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>3199</t>
+      <c r="K12" t="n">
+        <v>3199</v>
+      </c>
+      <c r="L12" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>3304</t>
         </is>
       </c>
     </row>
@@ -945,9 +1013,15 @@
       <c r="J13" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>5496</t>
+      <c r="K13" t="n">
+        <v>5496</v>
+      </c>
+      <c r="L13" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>5648</t>
         </is>
       </c>
     </row>
@@ -988,9 +1062,15 @@
       <c r="J14" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>4642</t>
+      <c r="K14" t="n">
+        <v>4642</v>
+      </c>
+      <c r="L14" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>4905</t>
         </is>
       </c>
     </row>
@@ -1018,6 +1098,8 @@
       <c r="I15" t="inlineStr"/>
       <c r="J15" s="2" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
+      <c r="L15" s="2" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1056,9 +1138,15 @@
       <c r="J16" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>4280</t>
+      <c r="K16" t="n">
+        <v>4280</v>
+      </c>
+      <c r="L16" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>4462</t>
         </is>
       </c>
     </row>
@@ -1099,9 +1187,15 @@
       <c r="J17" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>4154</t>
+      <c r="K17" t="n">
+        <v>4154</v>
+      </c>
+      <c r="L17" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>4447</t>
         </is>
       </c>
     </row>
@@ -1142,9 +1236,15 @@
       <c r="J18" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>4457</t>
+      <c r="K18" t="n">
+        <v>4457</v>
+      </c>
+      <c r="L18" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>4806</t>
         </is>
       </c>
     </row>
@@ -1172,6 +1272,8 @@
       <c r="I19" t="inlineStr"/>
       <c r="J19" s="2" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
+      <c r="L19" s="2" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1210,9 +1312,15 @@
       <c r="J20" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>3782</t>
+      <c r="K20" t="n">
+        <v>3782</v>
+      </c>
+      <c r="L20" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>4102</t>
         </is>
       </c>
     </row>
@@ -1253,9 +1361,15 @@
       <c r="J21" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>4908</t>
+      <c r="K21" t="n">
+        <v>4908</v>
+      </c>
+      <c r="L21" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>5190</t>
         </is>
       </c>
     </row>
@@ -1296,7 +1410,13 @@
       <c r="J22" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="K22" t="inlineStr">
+      <c r="K22" t="n">
+        <v>4053</v>
+      </c>
+      <c r="L22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="inlineStr">
         <is>
           <t>4053</t>
         </is>
@@ -1339,9 +1459,15 @@
       <c r="J23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>4915</t>
+      <c r="K23" t="n">
+        <v>4915</v>
+      </c>
+      <c r="L23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>5152</t>
         </is>
       </c>
     </row>
@@ -1382,7 +1508,13 @@
       <c r="J24" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K24" t="inlineStr">
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1425,9 +1557,15 @@
       <c r="J25" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>2588</t>
+      <c r="K25" t="n">
+        <v>2588</v>
+      </c>
+      <c r="L25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>2609</t>
         </is>
       </c>
     </row>
@@ -1455,6 +1593,8 @@
       <c r="I26" t="inlineStr"/>
       <c r="J26" s="2" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
+      <c r="L26" s="2" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1480,6 +1620,8 @@
       <c r="I27" t="inlineStr"/>
       <c r="J27" s="2" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
+      <c r="L27" s="2" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1518,9 +1660,15 @@
       <c r="J28" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>5119</t>
+      <c r="K28" t="n">
+        <v>5119</v>
+      </c>
+      <c r="L28" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>5301</t>
         </is>
       </c>
     </row>
@@ -1548,6 +1696,8 @@
       <c r="I29" t="inlineStr"/>
       <c r="J29" s="2" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
+      <c r="L29" s="2" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1586,9 +1736,15 @@
       <c r="J30" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>3974</t>
+      <c r="K30" t="n">
+        <v>3974</v>
+      </c>
+      <c r="L30" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>4266</t>
         </is>
       </c>
     </row>
@@ -1629,9 +1785,15 @@
       <c r="J31" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>5340</t>
+      <c r="K31" t="n">
+        <v>5340</v>
+      </c>
+      <c r="L31" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>5551</t>
         </is>
       </c>
     </row>
@@ -1671,6 +1833,8 @@
       </c>
       <c r="J32" s="2" t="inlineStr"/>
       <c r="K32" t="inlineStr"/>
+      <c r="L32" s="2" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1709,9 +1873,15 @@
       <c r="J33" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>4755</t>
+      <c r="K33" t="n">
+        <v>4755</v>
+      </c>
+      <c r="L33" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>4816</t>
         </is>
       </c>
     </row>
@@ -1752,9 +1922,15 @@
       <c r="J34" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>4983</t>
+      <c r="K34" t="n">
+        <v>4983</v>
+      </c>
+      <c r="L34" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>5328</t>
         </is>
       </c>
     </row>
@@ -1795,9 +1971,15 @@
       <c r="J35" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>4381</t>
+      <c r="K35" t="n">
+        <v>4381</v>
+      </c>
+      <c r="L35" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>4768</t>
         </is>
       </c>
     </row>
@@ -1825,6 +2007,8 @@
       <c r="I36" t="inlineStr"/>
       <c r="J36" s="2" t="inlineStr"/>
       <c r="K36" t="inlineStr"/>
+      <c r="L36" s="2" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1863,9 +2047,15 @@
       <c r="J37" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>4862</t>
+      <c r="K37" t="n">
+        <v>4862</v>
+      </c>
+      <c r="L37" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>5117</t>
         </is>
       </c>
     </row>
@@ -1906,9 +2096,15 @@
       <c r="J38" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>4737</t>
+      <c r="K38" t="n">
+        <v>4737</v>
+      </c>
+      <c r="L38" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>4921</t>
         </is>
       </c>
     </row>
@@ -1949,9 +2145,15 @@
       <c r="J39" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>4934</t>
+      <c r="K39" t="n">
+        <v>4934</v>
+      </c>
+      <c r="L39" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>5229</t>
         </is>
       </c>
     </row>
@@ -1992,9 +2194,15 @@
       <c r="J40" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>5132</t>
+      <c r="K40" t="n">
+        <v>5132</v>
+      </c>
+      <c r="L40" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>5547</t>
         </is>
       </c>
     </row>
@@ -2035,9 +2243,15 @@
       <c r="J41" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>5065</t>
+      <c r="K41" t="n">
+        <v>5065</v>
+      </c>
+      <c r="L41" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>5237</t>
         </is>
       </c>
     </row>
@@ -2078,9 +2292,15 @@
       <c r="J42" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>4732</t>
+      <c r="K42" t="n">
+        <v>4732</v>
+      </c>
+      <c r="L42" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>4918</t>
         </is>
       </c>
     </row>
@@ -2121,9 +2341,15 @@
       <c r="J43" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>4410</t>
+      <c r="K43" t="n">
+        <v>4410</v>
+      </c>
+      <c r="L43" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>4626</t>
         </is>
       </c>
     </row>
@@ -2164,9 +2390,15 @@
       <c r="J44" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>4480</t>
+      <c r="K44" t="n">
+        <v>4480</v>
+      </c>
+      <c r="L44" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>4772</t>
         </is>
       </c>
     </row>
@@ -2207,9 +2439,15 @@
       <c r="J45" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>4133</t>
+      <c r="K45" t="n">
+        <v>4133</v>
+      </c>
+      <c r="L45" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>4391</t>
         </is>
       </c>
     </row>
@@ -2250,9 +2488,15 @@
       <c r="J46" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>5004</t>
+      <c r="K46" t="n">
+        <v>5004</v>
+      </c>
+      <c r="L46" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>5297</t>
         </is>
       </c>
     </row>
@@ -2293,9 +2537,15 @@
       <c r="J47" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>4186</t>
+      <c r="K47" t="n">
+        <v>4186</v>
+      </c>
+      <c r="L47" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>4270</t>
         </is>
       </c>
     </row>
@@ -2336,7 +2586,13 @@
       <c r="J48" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K48" t="inlineStr">
+      <c r="K48" t="n">
+        <v>2516</v>
+      </c>
+      <c r="L48" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M48" t="inlineStr">
         <is>
           <t>2516</t>
         </is>
@@ -2366,6 +2622,8 @@
       <c r="I49" t="inlineStr"/>
       <c r="J49" s="2" t="inlineStr"/>
       <c r="K49" t="inlineStr"/>
+      <c r="L49" s="2" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -2404,7 +2662,13 @@
       <c r="J50" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K50" t="inlineStr">
+      <c r="K50" t="n">
+        <v>0</v>
+      </c>
+      <c r="L50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M50" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2447,7 +2711,13 @@
       <c r="J51" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K51" t="inlineStr">
+      <c r="K51" t="n">
+        <v>2592</v>
+      </c>
+      <c r="L51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M51" t="inlineStr">
         <is>
           <t>2592</t>
         </is>
@@ -2490,9 +2760,15 @@
       <c r="J52" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>2801</t>
+      <c r="K52" t="n">
+        <v>2801</v>
+      </c>
+      <c r="L52" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>3170</t>
         </is>
       </c>
     </row>
@@ -2533,9 +2809,15 @@
       <c r="J53" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>4723</t>
+      <c r="K53" t="n">
+        <v>4723</v>
+      </c>
+      <c r="L53" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>4981</t>
         </is>
       </c>
     </row>
@@ -2576,9 +2858,15 @@
       <c r="J54" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>4196</t>
+      <c r="K54" t="n">
+        <v>4196</v>
+      </c>
+      <c r="L54" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>4321</t>
         </is>
       </c>
     </row>
@@ -2619,9 +2907,15 @@
       <c r="J55" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>4145</t>
+      <c r="K55" t="n">
+        <v>4145</v>
+      </c>
+      <c r="L55" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>4387</t>
         </is>
       </c>
     </row>
@@ -2662,9 +2956,15 @@
       <c r="J56" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>4530</t>
+      <c r="K56" t="n">
+        <v>4530</v>
+      </c>
+      <c r="L56" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>4765</t>
         </is>
       </c>
     </row>
@@ -2705,9 +3005,15 @@
       <c r="J57" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>4293</t>
+      <c r="K57" t="n">
+        <v>4293</v>
+      </c>
+      <c r="L57" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>4477</t>
         </is>
       </c>
     </row>
@@ -2748,9 +3054,15 @@
       <c r="J58" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>4051</t>
+      <c r="K58" t="n">
+        <v>4051</v>
+      </c>
+      <c r="L58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>4067</t>
         </is>
       </c>
     </row>
@@ -2791,7 +3103,13 @@
       <c r="J59" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K59" t="inlineStr">
+      <c r="K59" t="n">
+        <v>0</v>
+      </c>
+      <c r="L59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M59" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2834,9 +3152,15 @@
       <c r="J60" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>4693</t>
+      <c r="K60" t="n">
+        <v>4693</v>
+      </c>
+      <c r="L60" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>4991</t>
         </is>
       </c>
     </row>
@@ -2877,7 +3201,13 @@
       <c r="J61" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="K61" t="inlineStr">
+      <c r="K61" t="n">
+        <v>2742</v>
+      </c>
+      <c r="L61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M61" t="inlineStr">
         <is>
           <t>2742</t>
         </is>
@@ -2920,9 +3250,15 @@
       <c r="J62" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>3241</t>
+      <c r="K62" t="n">
+        <v>3241</v>
+      </c>
+      <c r="L62" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>3229</t>
         </is>
       </c>
     </row>
@@ -2963,9 +3299,15 @@
       <c r="J63" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="K63" t="inlineStr">
-        <is>
-          <t>4462</t>
+      <c r="K63" t="n">
+        <v>4462</v>
+      </c>
+      <c r="L63" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>4701</t>
         </is>
       </c>
     </row>
@@ -3006,9 +3348,15 @@
       <c r="J64" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>4612</t>
+      <c r="K64" t="n">
+        <v>4612</v>
+      </c>
+      <c r="L64" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>5030</t>
         </is>
       </c>
     </row>
@@ -3049,9 +3397,15 @@
       <c r="J65" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>2951</t>
+      <c r="K65" t="n">
+        <v>2951</v>
+      </c>
+      <c r="L65" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>2947</t>
         </is>
       </c>
     </row>
@@ -3092,9 +3446,15 @@
       <c r="J66" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="K66" t="inlineStr">
-        <is>
-          <t>4251</t>
+      <c r="K66" t="n">
+        <v>4251</v>
+      </c>
+      <c r="L66" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>4465</t>
         </is>
       </c>
     </row>
@@ -3135,9 +3495,15 @@
       <c r="J67" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>2803</t>
+      <c r="K67" t="n">
+        <v>2803</v>
+      </c>
+      <c r="L67" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>2833</t>
         </is>
       </c>
     </row>
@@ -3178,7 +3544,13 @@
       <c r="J68" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K68" t="inlineStr">
+      <c r="K68" t="n">
+        <v>0</v>
+      </c>
+      <c r="L68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3221,9 +3593,15 @@
       <c r="J69" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="K69" t="inlineStr">
-        <is>
-          <t>4079</t>
+      <c r="K69" t="n">
+        <v>4079</v>
+      </c>
+      <c r="L69" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>4133</t>
         </is>
       </c>
     </row>
@@ -3264,9 +3642,15 @@
       <c r="J70" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K70" t="inlineStr">
-        <is>
-          <t>4146</t>
+      <c r="K70" t="n">
+        <v>4146</v>
+      </c>
+      <c r="L70" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>4399</t>
         </is>
       </c>
     </row>
@@ -3307,9 +3691,15 @@
       <c r="J71" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="K71" t="inlineStr">
-        <is>
-          <t>2781</t>
+      <c r="K71" t="n">
+        <v>2781</v>
+      </c>
+      <c r="L71" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>2869</t>
         </is>
       </c>
     </row>
@@ -3350,9 +3740,15 @@
       <c r="J72" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K72" t="inlineStr">
-        <is>
-          <t>4114</t>
+      <c r="K72" t="n">
+        <v>4114</v>
+      </c>
+      <c r="L72" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>4283</t>
         </is>
       </c>
     </row>
@@ -3393,9 +3789,15 @@
       <c r="J73" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="K73" t="inlineStr">
-        <is>
-          <t>4551</t>
+      <c r="K73" t="n">
+        <v>4551</v>
+      </c>
+      <c r="L73" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>4735</t>
         </is>
       </c>
     </row>
@@ -3436,7 +3838,13 @@
       <c r="J74" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K74" t="inlineStr">
+      <c r="K74" t="n">
+        <v>0</v>
+      </c>
+      <c r="L74" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3479,7 +3887,13 @@
       <c r="J75" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K75" t="inlineStr">
+      <c r="K75" t="n">
+        <v>0</v>
+      </c>
+      <c r="L75" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3522,9 +3936,15 @@
       <c r="J76" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K76" t="inlineStr">
-        <is>
-          <t>4563</t>
+      <c r="K76" t="n">
+        <v>4563</v>
+      </c>
+      <c r="L76" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>4844</t>
         </is>
       </c>
     </row>
@@ -3565,7 +3985,13 @@
       <c r="J77" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K77" t="inlineStr">
+      <c r="K77" t="n">
+        <v>0</v>
+      </c>
+      <c r="L77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3608,9 +4034,15 @@
       <c r="J78" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="K78" t="inlineStr">
-        <is>
-          <t>4487</t>
+      <c r="K78" t="n">
+        <v>4487</v>
+      </c>
+      <c r="L78" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>4592</t>
         </is>
       </c>
     </row>
@@ -3651,9 +4083,15 @@
       <c r="J79" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>3175</t>
+      <c r="K79" t="n">
+        <v>3175</v>
+      </c>
+      <c r="L79" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>3182</t>
         </is>
       </c>
     </row>
@@ -3681,6 +4119,8 @@
       <c r="I80" t="inlineStr"/>
       <c r="J80" s="2" t="inlineStr"/>
       <c r="K80" t="inlineStr"/>
+      <c r="L80" s="2" t="inlineStr"/>
+      <c r="M80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -3719,9 +4159,15 @@
       <c r="J81" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>4446</t>
+      <c r="K81" t="n">
+        <v>4446</v>
+      </c>
+      <c r="L81" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>4658</t>
         </is>
       </c>
     </row>
@@ -3762,9 +4208,15 @@
       <c r="J82" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>4415</t>
+      <c r="K82" t="n">
+        <v>4415</v>
+      </c>
+      <c r="L82" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>4676</t>
         </is>
       </c>
     </row>
@@ -3805,9 +4257,15 @@
       <c r="J83" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="K83" t="inlineStr">
-        <is>
-          <t>4185</t>
+      <c r="K83" t="n">
+        <v>4185</v>
+      </c>
+      <c r="L83" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>4414</t>
         </is>
       </c>
     </row>
@@ -3848,9 +4306,15 @@
       <c r="J84" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>4050</t>
+      <c r="K84" t="n">
+        <v>4050</v>
+      </c>
+      <c r="L84" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>4288</t>
         </is>
       </c>
     </row>
@@ -3891,9 +4355,15 @@
       <c r="J85" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>4128</t>
+      <c r="K85" t="n">
+        <v>4128</v>
+      </c>
+      <c r="L85" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M85" t="inlineStr">
+        <is>
+          <t>4236</t>
         </is>
       </c>
     </row>
@@ -3934,9 +4404,15 @@
       <c r="J86" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K86" t="inlineStr">
-        <is>
-          <t>2836</t>
+      <c r="K86" t="n">
+        <v>2836</v>
+      </c>
+      <c r="L86" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>3206</t>
         </is>
       </c>
     </row>
@@ -3977,9 +4453,15 @@
       <c r="J87" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>4370</t>
+      <c r="K87" t="n">
+        <v>4370</v>
+      </c>
+      <c r="L87" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>4510</t>
         </is>
       </c>
     </row>
@@ -4020,9 +4502,15 @@
       <c r="J88" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>3165</t>
+      <c r="K88" t="n">
+        <v>3165</v>
+      </c>
+      <c r="L88" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>3301</t>
         </is>
       </c>
     </row>
@@ -4063,9 +4551,15 @@
       <c r="J89" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="K89" t="inlineStr">
-        <is>
-          <t>3770</t>
+      <c r="K89" t="n">
+        <v>3770</v>
+      </c>
+      <c r="L89" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="M89" t="inlineStr">
+        <is>
+          <t>3893</t>
         </is>
       </c>
     </row>
@@ -4106,9 +4600,15 @@
       <c r="J90" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>2868</t>
+      <c r="K90" t="n">
+        <v>2868</v>
+      </c>
+      <c r="L90" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>2853</t>
         </is>
       </c>
     </row>
@@ -4149,9 +4649,15 @@
       <c r="J91" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K91" t="inlineStr">
-        <is>
-          <t>3472</t>
+      <c r="K91" t="n">
+        <v>3472</v>
+      </c>
+      <c r="L91" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>3568</t>
         </is>
       </c>
     </row>
@@ -4192,7 +4698,13 @@
       <c r="J92" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K92" t="inlineStr">
+      <c r="K92" t="n">
+        <v>0</v>
+      </c>
+      <c r="L92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4235,9 +4747,15 @@
       <c r="J93" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K93" t="inlineStr">
-        <is>
-          <t>3479</t>
+      <c r="K93" t="n">
+        <v>3479</v>
+      </c>
+      <c r="L93" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>3530</t>
         </is>
       </c>
     </row>
@@ -4278,7 +4796,13 @@
       <c r="J94" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K94" t="inlineStr">
+      <c r="K94" t="n">
+        <v>0</v>
+      </c>
+      <c r="L94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4321,9 +4845,15 @@
       <c r="J95" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="K95" t="inlineStr">
-        <is>
-          <t>3816</t>
+      <c r="K95" t="n">
+        <v>3816</v>
+      </c>
+      <c r="L95" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>3986</t>
         </is>
       </c>
     </row>
@@ -4364,9 +4894,15 @@
       <c r="J96" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="K96" t="inlineStr">
-        <is>
-          <t>2564</t>
+      <c r="K96" t="n">
+        <v>2564</v>
+      </c>
+      <c r="L96" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>2557</t>
         </is>
       </c>
     </row>
@@ -4407,9 +4943,15 @@
       <c r="J97" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K97" t="inlineStr">
-        <is>
-          <t>2114</t>
+      <c r="K97" t="n">
+        <v>2114</v>
+      </c>
+      <c r="L97" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>2187</t>
         </is>
       </c>
     </row>
@@ -4450,9 +4992,15 @@
       <c r="J98" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="K98" t="inlineStr">
-        <is>
-          <t>3174</t>
+      <c r="K98" t="n">
+        <v>3174</v>
+      </c>
+      <c r="L98" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>3326</t>
         </is>
       </c>
     </row>
@@ -4493,9 +5041,15 @@
       <c r="J99" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K99" t="inlineStr">
-        <is>
-          <t>2515</t>
+      <c r="K99" t="n">
+        <v>2515</v>
+      </c>
+      <c r="L99" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M99" t="inlineStr">
+        <is>
+          <t>2511</t>
         </is>
       </c>
     </row>
@@ -4536,9 +5090,15 @@
       <c r="J100" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="K100" t="inlineStr">
-        <is>
-          <t>3517</t>
+      <c r="K100" t="n">
+        <v>3517</v>
+      </c>
+      <c r="L100" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="M100" t="inlineStr">
+        <is>
+          <t>3666</t>
         </is>
       </c>
     </row>
@@ -4579,9 +5139,15 @@
       <c r="J101" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K101" t="inlineStr">
-        <is>
-          <t>2305</t>
+      <c r="K101" t="n">
+        <v>2305</v>
+      </c>
+      <c r="L101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M101" t="inlineStr">
+        <is>
+          <t>2317</t>
         </is>
       </c>
     </row>
@@ -4622,9 +5188,15 @@
       <c r="J102" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K102" t="inlineStr">
-        <is>
-          <t>4376</t>
+      <c r="K102" t="n">
+        <v>4376</v>
+      </c>
+      <c r="L102" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>4635</t>
         </is>
       </c>
     </row>
@@ -4665,9 +5237,15 @@
       <c r="J103" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K103" t="inlineStr">
-        <is>
-          <t>3928</t>
+      <c r="K103" t="n">
+        <v>3928</v>
+      </c>
+      <c r="L103" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M103" t="inlineStr">
+        <is>
+          <t>4169</t>
         </is>
       </c>
     </row>
@@ -4708,9 +5286,15 @@
       <c r="J104" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K104" t="inlineStr">
-        <is>
-          <t>4017</t>
+      <c r="K104" t="n">
+        <v>4017</v>
+      </c>
+      <c r="L104" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M104" t="inlineStr">
+        <is>
+          <t>4189</t>
         </is>
       </c>
     </row>
@@ -4751,9 +5335,15 @@
       <c r="J105" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="K105" t="inlineStr">
-        <is>
-          <t>4268</t>
+      <c r="K105" t="n">
+        <v>4268</v>
+      </c>
+      <c r="L105" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M105" t="inlineStr">
+        <is>
+          <t>4460</t>
         </is>
       </c>
     </row>
@@ -4794,9 +5384,15 @@
       <c r="J106" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="K106" t="inlineStr">
-        <is>
-          <t>4068</t>
+      <c r="K106" t="n">
+        <v>4068</v>
+      </c>
+      <c r="L106" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="M106" t="inlineStr">
+        <is>
+          <t>4196</t>
         </is>
       </c>
     </row>
@@ -4837,9 +5433,15 @@
       <c r="J107" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="K107" t="inlineStr">
-        <is>
-          <t>4048</t>
+      <c r="K107" t="n">
+        <v>4048</v>
+      </c>
+      <c r="L107" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="M107" t="inlineStr">
+        <is>
+          <t>4265</t>
         </is>
       </c>
     </row>
@@ -4880,7 +5482,13 @@
       <c r="J108" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K108" t="inlineStr">
+      <c r="K108" t="n">
+        <v>0</v>
+      </c>
+      <c r="L108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4923,9 +5531,15 @@
       <c r="J109" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K109" t="inlineStr">
-        <is>
-          <t>2859</t>
+      <c r="K109" t="n">
+        <v>2859</v>
+      </c>
+      <c r="L109" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="M109" t="inlineStr">
+        <is>
+          <t>2993</t>
         </is>
       </c>
     </row>
@@ -4966,7 +5580,13 @@
       <c r="J110" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K110" t="inlineStr">
+      <c r="K110" t="n">
+        <v>0</v>
+      </c>
+      <c r="L110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M110" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5009,9 +5629,15 @@
       <c r="J111" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="K111" t="inlineStr">
-        <is>
-          <t>3827</t>
+      <c r="K111" t="n">
+        <v>3827</v>
+      </c>
+      <c r="L111" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M111" t="inlineStr">
+        <is>
+          <t>3894</t>
         </is>
       </c>
     </row>
@@ -5052,9 +5678,15 @@
       <c r="J112" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K112" t="inlineStr">
-        <is>
-          <t>4003</t>
+      <c r="K112" t="n">
+        <v>4003</v>
+      </c>
+      <c r="L112" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>4187</t>
         </is>
       </c>
     </row>
@@ -5095,9 +5727,15 @@
       <c r="J113" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K113" t="inlineStr">
-        <is>
-          <t>3640</t>
+      <c r="K113" t="n">
+        <v>3640</v>
+      </c>
+      <c r="L113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>3624</t>
         </is>
       </c>
     </row>
@@ -5138,9 +5776,15 @@
       <c r="J114" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K114" t="inlineStr">
-        <is>
-          <t>2552</t>
+      <c r="K114" t="n">
+        <v>2552</v>
+      </c>
+      <c r="L114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M114" t="inlineStr">
+        <is>
+          <t>2547</t>
         </is>
       </c>
     </row>
@@ -5181,9 +5825,15 @@
       <c r="J115" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K115" t="inlineStr">
-        <is>
-          <t>3563</t>
+      <c r="K115" t="n">
+        <v>3563</v>
+      </c>
+      <c r="L115" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>3874</t>
         </is>
       </c>
     </row>
@@ -5224,9 +5874,15 @@
       <c r="J116" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K116" t="inlineStr">
-        <is>
-          <t>3055</t>
+      <c r="K116" t="n">
+        <v>3055</v>
+      </c>
+      <c r="L116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>3094</t>
         </is>
       </c>
     </row>
@@ -5267,9 +5923,15 @@
       <c r="J117" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K117" t="inlineStr">
-        <is>
-          <t>2397</t>
+      <c r="K117" t="n">
+        <v>2397</v>
+      </c>
+      <c r="L117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M117" t="inlineStr">
+        <is>
+          <t>2393</t>
         </is>
       </c>
     </row>
@@ -5310,9 +5972,15 @@
       <c r="J118" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="K118" t="inlineStr">
-        <is>
-          <t>3024</t>
+      <c r="K118" t="n">
+        <v>3024</v>
+      </c>
+      <c r="L118" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="M118" t="inlineStr">
+        <is>
+          <t>3080</t>
         </is>
       </c>
     </row>
@@ -5353,9 +6021,15 @@
       <c r="J119" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K119" t="inlineStr">
-        <is>
-          <t>4021</t>
+      <c r="K119" t="n">
+        <v>4021</v>
+      </c>
+      <c r="L119" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M119" t="inlineStr">
+        <is>
+          <t>4232</t>
         </is>
       </c>
     </row>
@@ -5396,9 +6070,15 @@
       <c r="J120" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K120" t="inlineStr">
-        <is>
-          <t>2585</t>
+      <c r="K120" t="n">
+        <v>2585</v>
+      </c>
+      <c r="L120" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>2623</t>
         </is>
       </c>
     </row>
@@ -5439,9 +6119,15 @@
       <c r="J121" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K121" t="inlineStr">
-        <is>
-          <t>1574</t>
+      <c r="K121" t="n">
+        <v>1574</v>
+      </c>
+      <c r="L121" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="M121" t="inlineStr">
+        <is>
+          <t>1601</t>
         </is>
       </c>
     </row>
@@ -5482,9 +6168,15 @@
       <c r="J122" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="K122" t="inlineStr">
-        <is>
-          <t>2694</t>
+      <c r="K122" t="n">
+        <v>2694</v>
+      </c>
+      <c r="L122" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>3007</t>
         </is>
       </c>
     </row>
@@ -5525,9 +6217,15 @@
       <c r="J123" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="K123" t="inlineStr">
-        <is>
-          <t>4029</t>
+      <c r="K123" t="n">
+        <v>4029</v>
+      </c>
+      <c r="L123" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="M123" t="inlineStr">
+        <is>
+          <t>4193</t>
         </is>
       </c>
     </row>
@@ -5568,7 +6266,13 @@
       <c r="J124" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K124" t="inlineStr">
+      <c r="K124" t="n">
+        <v>0</v>
+      </c>
+      <c r="L124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M124" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5611,9 +6315,15 @@
       <c r="J125" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K125" t="inlineStr">
-        <is>
-          <t>3807</t>
+      <c r="K125" t="n">
+        <v>3807</v>
+      </c>
+      <c r="L125" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M125" t="inlineStr">
+        <is>
+          <t>3991</t>
         </is>
       </c>
     </row>
@@ -5654,9 +6364,15 @@
       <c r="J126" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="K126" t="inlineStr">
-        <is>
-          <t>3646</t>
+      <c r="K126" t="n">
+        <v>3646</v>
+      </c>
+      <c r="L126" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="M126" t="inlineStr">
+        <is>
+          <t>3720</t>
         </is>
       </c>
     </row>
@@ -5697,9 +6413,15 @@
       <c r="J127" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K127" t="inlineStr">
-        <is>
-          <t>3301</t>
+      <c r="K127" t="n">
+        <v>3301</v>
+      </c>
+      <c r="L127" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M127" t="inlineStr">
+        <is>
+          <t>3329</t>
         </is>
       </c>
     </row>
@@ -5740,9 +6462,15 @@
       <c r="J128" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K128" t="inlineStr">
-        <is>
-          <t>3980</t>
+      <c r="K128" t="n">
+        <v>3980</v>
+      </c>
+      <c r="L128" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="M128" t="inlineStr">
+        <is>
+          <t>3991</t>
         </is>
       </c>
     </row>
@@ -5783,9 +6511,15 @@
       <c r="J129" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K129" t="inlineStr">
-        <is>
-          <t>2021</t>
+      <c r="K129" t="n">
+        <v>2021</v>
+      </c>
+      <c r="L129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M129" t="inlineStr">
+        <is>
+          <t>2017</t>
         </is>
       </c>
     </row>
@@ -5826,7 +6560,13 @@
       <c r="J130" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K130" t="inlineStr">
+      <c r="K130" t="n">
+        <v>0</v>
+      </c>
+      <c r="L130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5869,7 +6609,13 @@
       <c r="J131" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K131" t="inlineStr">
+      <c r="K131" t="n">
+        <v>0</v>
+      </c>
+      <c r="L131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5912,9 +6658,15 @@
       <c r="J132" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K132" t="inlineStr">
-        <is>
-          <t>3663</t>
+      <c r="K132" t="n">
+        <v>3663</v>
+      </c>
+      <c r="L132" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M132" t="inlineStr">
+        <is>
+          <t>3778</t>
         </is>
       </c>
     </row>
@@ -5955,7 +6707,13 @@
       <c r="J133" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K133" t="inlineStr">
+      <c r="K133" t="n">
+        <v>0</v>
+      </c>
+      <c r="L133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5998,9 +6756,15 @@
       <c r="J134" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K134" t="inlineStr">
-        <is>
-          <t>3104</t>
+      <c r="K134" t="n">
+        <v>3104</v>
+      </c>
+      <c r="L134" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M134" t="inlineStr">
+        <is>
+          <t>3192</t>
         </is>
       </c>
     </row>
@@ -6041,9 +6805,15 @@
       <c r="J135" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="K135" t="inlineStr">
-        <is>
-          <t>3991</t>
+      <c r="K135" t="n">
+        <v>3991</v>
+      </c>
+      <c r="L135" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M135" t="inlineStr">
+        <is>
+          <t>3992</t>
         </is>
       </c>
     </row>
@@ -6084,9 +6854,15 @@
       <c r="J136" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K136" t="inlineStr">
-        <is>
-          <t>3913</t>
+      <c r="K136" t="n">
+        <v>3913</v>
+      </c>
+      <c r="L136" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t>4016</t>
         </is>
       </c>
     </row>
@@ -6127,7 +6903,13 @@
       <c r="J137" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K137" t="inlineStr">
+      <c r="K137" t="n">
+        <v>0</v>
+      </c>
+      <c r="L137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6170,7 +6952,13 @@
       <c r="J138" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K138" t="inlineStr">
+      <c r="K138" t="n">
+        <v>0</v>
+      </c>
+      <c r="L138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M138" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6213,9 +7001,15 @@
       <c r="J139" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K139" t="inlineStr">
-        <is>
-          <t>3072</t>
+      <c r="K139" t="n">
+        <v>3072</v>
+      </c>
+      <c r="L139" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="M139" t="inlineStr">
+        <is>
+          <t>3094</t>
         </is>
       </c>
     </row>
@@ -6256,7 +7050,13 @@
       <c r="J140" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K140" t="inlineStr">
+      <c r="K140" t="n">
+        <v>0</v>
+      </c>
+      <c r="L140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6299,7 +7099,13 @@
       <c r="J141" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K141" t="inlineStr">
+      <c r="K141" t="n">
+        <v>0</v>
+      </c>
+      <c r="L141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6342,9 +7148,15 @@
       <c r="J142" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K142" t="inlineStr">
-        <is>
-          <t>3147</t>
+      <c r="K142" t="n">
+        <v>3147</v>
+      </c>
+      <c r="L142" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="M142" t="inlineStr">
+        <is>
+          <t>3139</t>
         </is>
       </c>
     </row>
@@ -6385,7 +7197,13 @@
       <c r="J143" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K143" t="inlineStr">
+      <c r="K143" t="n">
+        <v>0</v>
+      </c>
+      <c r="L143" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6428,9 +7246,15 @@
       <c r="J144" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K144" t="inlineStr">
-        <is>
-          <t>3232</t>
+      <c r="K144" t="n">
+        <v>3232</v>
+      </c>
+      <c r="L144" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="M144" t="inlineStr">
+        <is>
+          <t>3314</t>
         </is>
       </c>
     </row>
@@ -6471,7 +7295,13 @@
       <c r="J145" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K145" t="inlineStr">
+      <c r="K145" t="n">
+        <v>0</v>
+      </c>
+      <c r="L145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6514,7 +7344,13 @@
       <c r="J146" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K146" t="inlineStr">
+      <c r="K146" t="n">
+        <v>0</v>
+      </c>
+      <c r="L146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6557,9 +7393,15 @@
       <c r="J147" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="K147" t="inlineStr">
-        <is>
-          <t>2051</t>
+      <c r="K147" t="n">
+        <v>2051</v>
+      </c>
+      <c r="L147" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M147" t="inlineStr">
+        <is>
+          <t>2074</t>
         </is>
       </c>
     </row>
@@ -6600,7 +7442,13 @@
       <c r="J148" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K148" t="inlineStr">
+      <c r="K148" t="n">
+        <v>0</v>
+      </c>
+      <c r="L148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6643,7 +7491,13 @@
       <c r="J149" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K149" t="inlineStr">
+      <c r="K149" t="n">
+        <v>0</v>
+      </c>
+      <c r="L149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6686,9 +7540,15 @@
       <c r="J150" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K150" t="inlineStr">
-        <is>
-          <t>2530</t>
+      <c r="K150" t="n">
+        <v>2530</v>
+      </c>
+      <c r="L150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M150" t="inlineStr">
+        <is>
+          <t>2556</t>
         </is>
       </c>
     </row>
@@ -6729,7 +7589,13 @@
       <c r="J151" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K151" t="inlineStr">
+      <c r="K151" t="n">
+        <v>0</v>
+      </c>
+      <c r="L151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6772,7 +7638,13 @@
       <c r="J152" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K152" t="inlineStr">
+      <c r="K152" t="n">
+        <v>0</v>
+      </c>
+      <c r="L152" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6815,7 +7687,13 @@
       <c r="J153" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K153" t="inlineStr">
+      <c r="K153" t="n">
+        <v>0</v>
+      </c>
+      <c r="L153" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6858,9 +7736,15 @@
       <c r="J154" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="K154" t="inlineStr">
-        <is>
-          <t>2926</t>
+      <c r="K154" t="n">
+        <v>2926</v>
+      </c>
+      <c r="L154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M154" t="inlineStr">
+        <is>
+          <t>2916</t>
         </is>
       </c>
     </row>
@@ -6901,7 +7785,13 @@
       <c r="J155" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K155" t="inlineStr">
+      <c r="K155" t="n">
+        <v>0</v>
+      </c>
+      <c r="L155" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6944,7 +7834,13 @@
       <c r="J156" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K156" t="inlineStr">
+      <c r="K156" t="n">
+        <v>0</v>
+      </c>
+      <c r="L156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6987,7 +7883,13 @@
       <c r="J157" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K157" t="inlineStr">
+      <c r="K157" t="n">
+        <v>0</v>
+      </c>
+      <c r="L157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7030,9 +7932,15 @@
       <c r="J158" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K158" t="inlineStr">
-        <is>
-          <t>2884</t>
+      <c r="K158" t="n">
+        <v>2884</v>
+      </c>
+      <c r="L158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M158" t="inlineStr">
+        <is>
+          <t>2929</t>
         </is>
       </c>
     </row>
@@ -7067,11 +7975,11 @@
       <c r="J159" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K159" t="inlineStr">
-        <is>
-          <t>2739</t>
-        </is>
-      </c>
+      <c r="K159" t="n">
+        <v>2739</v>
+      </c>
+      <c r="L159" s="2" t="inlineStr"/>
+      <c r="M159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="n">
@@ -7104,9 +8012,15 @@
       <c r="J160" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K160" t="inlineStr">
-        <is>
-          <t>4220</t>
+      <c r="K160" t="n">
+        <v>4220</v>
+      </c>
+      <c r="L160" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M160" t="inlineStr">
+        <is>
+          <t>4314</t>
         </is>
       </c>
     </row>
@@ -7136,6 +8050,8 @@
       <c r="I161" t="inlineStr"/>
       <c r="J161" s="2" t="inlineStr"/>
       <c r="K161" t="inlineStr"/>
+      <c r="L161" s="2" t="inlineStr"/>
+      <c r="M161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="n">
@@ -7168,9 +8084,15 @@
       <c r="J162" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K162" t="inlineStr">
-        <is>
-          <t>3240</t>
+      <c r="K162" t="n">
+        <v>3240</v>
+      </c>
+      <c r="L162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M162" t="inlineStr">
+        <is>
+          <t>3451</t>
         </is>
       </c>
     </row>
@@ -7205,9 +8127,15 @@
       <c r="J163" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K163" t="inlineStr">
-        <is>
-          <t>2619</t>
+      <c r="K163" t="n">
+        <v>2619</v>
+      </c>
+      <c r="L163" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="M163" t="inlineStr">
+        <is>
+          <t>2713</t>
         </is>
       </c>
     </row>
@@ -7238,9 +8166,15 @@
       <c r="J164" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="K164" t="inlineStr">
-        <is>
-          <t>2910</t>
+      <c r="K164" t="n">
+        <v>2910</v>
+      </c>
+      <c r="L164" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="M164" t="inlineStr">
+        <is>
+          <t>2901</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-20 11:30:51
</commit_message>
<xml_diff>
--- a/Season_Attack/86.xlsx
+++ b/Season_Attack/86.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M164"/>
+  <dimension ref="A1:O164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,16 @@
           <t>03-18_0</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>03-19_A</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>03-19_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -500,9 +510,15 @@
       <c r="L2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>3042</t>
+      <c r="M2" t="n">
+        <v>3042</v>
+      </c>
+      <c r="N2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>3070</t>
         </is>
       </c>
     </row>
@@ -544,6 +560,8 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" s="2" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
+      <c r="N3" s="2" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -588,9 +606,15 @@
       <c r="L4" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>5190</t>
+      <c r="M4" t="n">
+        <v>5190</v>
+      </c>
+      <c r="N4" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>5391</t>
         </is>
       </c>
     </row>
@@ -637,9 +661,15 @@
       <c r="L5" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>5082</t>
+      <c r="M5" t="n">
+        <v>5082</v>
+      </c>
+      <c r="N5" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>5510</t>
         </is>
       </c>
     </row>
@@ -686,9 +716,15 @@
       <c r="L6" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>4962</t>
+      <c r="M6" t="n">
+        <v>4962</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>5256</t>
         </is>
       </c>
     </row>
@@ -735,9 +771,15 @@
       <c r="L7" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>5278</t>
+      <c r="M7" t="n">
+        <v>5278</v>
+      </c>
+      <c r="N7" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>5649</t>
         </is>
       </c>
     </row>
@@ -784,9 +826,15 @@
       <c r="L8" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>4694</t>
+      <c r="M8" t="n">
+        <v>4694</v>
+      </c>
+      <c r="N8" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>4972</t>
         </is>
       </c>
     </row>
@@ -809,7 +857,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F9" s="4" t="n">
@@ -833,9 +881,15 @@
       <c r="L9" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>4952</t>
+      <c r="M9" t="n">
+        <v>4952</v>
+      </c>
+      <c r="N9" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>5097</t>
         </is>
       </c>
     </row>
@@ -882,9 +936,15 @@
       <c r="L10" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>5027</t>
+      <c r="M10" t="n">
+        <v>5027</v>
+      </c>
+      <c r="N10" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>5190</t>
         </is>
       </c>
     </row>
@@ -926,6 +986,8 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" s="2" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
+      <c r="N11" s="2" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -970,7 +1032,13 @@
       <c r="L12" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="M12" t="n">
+        <v>3304</v>
+      </c>
+      <c r="N12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="inlineStr">
         <is>
           <t>3304</t>
         </is>
@@ -1019,9 +1087,15 @@
       <c r="L13" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>5648</t>
+      <c r="M13" t="n">
+        <v>5648</v>
+      </c>
+      <c r="N13" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>6012</t>
         </is>
       </c>
     </row>
@@ -1068,9 +1142,15 @@
       <c r="L14" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>4905</t>
+      <c r="M14" t="n">
+        <v>4905</v>
+      </c>
+      <c r="N14" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>5185</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1171,11 @@
       <c r="D15" t="n">
         <v>6558</v>
       </c>
-      <c r="E15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
       <c r="F15" s="2" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" s="2" t="inlineStr"/>
@@ -1100,6 +1184,14 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" s="2" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
+      <c r="N15" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>5472</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1144,9 +1236,15 @@
       <c r="L16" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>4462</t>
+      <c r="M16" t="n">
+        <v>4462</v>
+      </c>
+      <c r="N16" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>4608</t>
         </is>
       </c>
     </row>
@@ -1193,9 +1291,15 @@
       <c r="L17" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>4447</t>
+      <c r="M17" t="n">
+        <v>4447</v>
+      </c>
+      <c r="N17" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>4710</t>
         </is>
       </c>
     </row>
@@ -1242,9 +1346,15 @@
       <c r="L18" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>4806</t>
+      <c r="M18" t="n">
+        <v>4806</v>
+      </c>
+      <c r="N18" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>5137</t>
         </is>
       </c>
     </row>
@@ -1265,7 +1375,11 @@
       <c r="D19" t="n">
         <v>7464</v>
       </c>
-      <c r="E19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
       <c r="F19" s="2" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" s="2" t="inlineStr"/>
@@ -1274,6 +1388,14 @@
       <c r="K19" t="inlineStr"/>
       <c r="L19" s="2" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
+      <c r="N19" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>5984</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1318,9 +1440,15 @@
       <c r="L20" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>4102</t>
+      <c r="M20" t="n">
+        <v>4102</v>
+      </c>
+      <c r="N20" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>4426</t>
         </is>
       </c>
     </row>
@@ -1367,9 +1495,15 @@
       <c r="L21" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>5190</t>
+      <c r="M21" t="n">
+        <v>5190</v>
+      </c>
+      <c r="N21" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>5405</t>
         </is>
       </c>
     </row>
@@ -1416,9 +1550,15 @@
       <c r="L22" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>4053</t>
+      <c r="M22" t="n">
+        <v>4053</v>
+      </c>
+      <c r="N22" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>4107</t>
         </is>
       </c>
     </row>
@@ -1441,7 +1581,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F23" s="4" t="n">
@@ -1465,9 +1605,15 @@
       <c r="L23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>5152</t>
+      <c r="M23" t="n">
+        <v>5152</v>
+      </c>
+      <c r="N23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>5431</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1660,13 @@
       <c r="L24" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M24" t="inlineStr">
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1563,7 +1715,13 @@
       <c r="L25" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M25" t="inlineStr">
+      <c r="M25" t="n">
+        <v>2609</v>
+      </c>
+      <c r="N25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="inlineStr">
         <is>
           <t>2609</t>
         </is>
@@ -1595,6 +1753,8 @@
       <c r="K26" t="inlineStr"/>
       <c r="L26" s="2" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
+      <c r="N26" s="2" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1622,6 +1782,8 @@
       <c r="K27" t="inlineStr"/>
       <c r="L27" s="2" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
+      <c r="N27" s="2" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1666,9 +1828,15 @@
       <c r="L28" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>5301</t>
+      <c r="M28" t="n">
+        <v>5301</v>
+      </c>
+      <c r="N28" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>5594</t>
         </is>
       </c>
     </row>
@@ -1698,6 +1866,8 @@
       <c r="K29" t="inlineStr"/>
       <c r="L29" s="2" t="inlineStr"/>
       <c r="M29" t="inlineStr"/>
+      <c r="N29" s="2" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1742,9 +1912,15 @@
       <c r="L30" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>4266</t>
+      <c r="M30" t="n">
+        <v>4266</v>
+      </c>
+      <c r="N30" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>4516</t>
         </is>
       </c>
     </row>
@@ -1791,9 +1967,15 @@
       <c r="L31" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>5551</t>
+      <c r="M31" t="n">
+        <v>5551</v>
+      </c>
+      <c r="N31" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>5715</t>
         </is>
       </c>
     </row>
@@ -1835,6 +2017,8 @@
       <c r="K32" t="inlineStr"/>
       <c r="L32" s="2" t="inlineStr"/>
       <c r="M32" t="inlineStr"/>
+      <c r="N32" s="2" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1879,9 +2063,15 @@
       <c r="L33" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M33" t="inlineStr">
-        <is>
-          <t>4816</t>
+      <c r="M33" t="n">
+        <v>4816</v>
+      </c>
+      <c r="N33" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>5147</t>
         </is>
       </c>
     </row>
@@ -1928,9 +2118,15 @@
       <c r="L34" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="M34" t="inlineStr">
-        <is>
-          <t>5328</t>
+      <c r="M34" t="n">
+        <v>5328</v>
+      </c>
+      <c r="N34" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>5727</t>
         </is>
       </c>
     </row>
@@ -1977,9 +2173,15 @@
       <c r="L35" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>4768</t>
+      <c r="M35" t="n">
+        <v>4768</v>
+      </c>
+      <c r="N35" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>5141</t>
         </is>
       </c>
     </row>
@@ -2009,6 +2211,8 @@
       <c r="K36" t="inlineStr"/>
       <c r="L36" s="2" t="inlineStr"/>
       <c r="M36" t="inlineStr"/>
+      <c r="N36" s="2" t="inlineStr"/>
+      <c r="O36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2053,9 +2257,15 @@
       <c r="L37" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>5117</t>
+      <c r="M37" t="n">
+        <v>5117</v>
+      </c>
+      <c r="N37" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>5347</t>
         </is>
       </c>
     </row>
@@ -2102,9 +2312,15 @@
       <c r="L38" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>4921</t>
+      <c r="M38" t="n">
+        <v>4921</v>
+      </c>
+      <c r="N38" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>5203</t>
         </is>
       </c>
     </row>
@@ -2151,9 +2367,15 @@
       <c r="L39" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>5229</t>
+      <c r="M39" t="n">
+        <v>5229</v>
+      </c>
+      <c r="N39" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>5556</t>
         </is>
       </c>
     </row>
@@ -2200,9 +2422,15 @@
       <c r="L40" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>5547</t>
+      <c r="M40" t="n">
+        <v>5547</v>
+      </c>
+      <c r="N40" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>6003</t>
         </is>
       </c>
     </row>
@@ -2249,9 +2477,15 @@
       <c r="L41" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>5237</t>
+      <c r="M41" t="n">
+        <v>5237</v>
+      </c>
+      <c r="N41" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>5504</t>
         </is>
       </c>
     </row>
@@ -2298,9 +2532,15 @@
       <c r="L42" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>4918</t>
+      <c r="M42" t="n">
+        <v>4918</v>
+      </c>
+      <c r="N42" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>5238</t>
         </is>
       </c>
     </row>
@@ -2347,9 +2587,15 @@
       <c r="L43" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="M43" t="inlineStr">
-        <is>
-          <t>4626</t>
+      <c r="M43" t="n">
+        <v>4626</v>
+      </c>
+      <c r="N43" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>4883</t>
         </is>
       </c>
     </row>
@@ -2396,9 +2642,15 @@
       <c r="L44" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>4772</t>
+      <c r="M44" t="n">
+        <v>4772</v>
+      </c>
+      <c r="N44" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>4977</t>
         </is>
       </c>
     </row>
@@ -2445,9 +2697,15 @@
       <c r="L45" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>4391</t>
+      <c r="M45" t="n">
+        <v>4391</v>
+      </c>
+      <c r="N45" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>4511</t>
         </is>
       </c>
     </row>
@@ -2494,9 +2752,15 @@
       <c r="L46" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>5297</t>
+      <c r="M46" t="n">
+        <v>5297</v>
+      </c>
+      <c r="N46" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>5589</t>
         </is>
       </c>
     </row>
@@ -2543,9 +2807,15 @@
       <c r="L47" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>4270</t>
+      <c r="M47" t="n">
+        <v>4270</v>
+      </c>
+      <c r="N47" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>4528</t>
         </is>
       </c>
     </row>
@@ -2592,7 +2862,13 @@
       <c r="L48" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M48" t="inlineStr">
+      <c r="M48" t="n">
+        <v>2516</v>
+      </c>
+      <c r="N48" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O48" t="inlineStr">
         <is>
           <t>2516</t>
         </is>
@@ -2624,6 +2900,8 @@
       <c r="K49" t="inlineStr"/>
       <c r="L49" s="2" t="inlineStr"/>
       <c r="M49" t="inlineStr"/>
+      <c r="N49" s="2" t="inlineStr"/>
+      <c r="O49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -2668,7 +2946,13 @@
       <c r="L50" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M50" t="inlineStr">
+      <c r="M50" t="n">
+        <v>0</v>
+      </c>
+      <c r="N50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O50" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2717,9 +3001,15 @@
       <c r="L51" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>2592</t>
+      <c r="M51" t="n">
+        <v>2592</v>
+      </c>
+      <c r="N51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>2728</t>
         </is>
       </c>
     </row>
@@ -2766,9 +3056,15 @@
       <c r="L52" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>3170</t>
+      <c r="M52" t="n">
+        <v>3170</v>
+      </c>
+      <c r="N52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>3168</t>
         </is>
       </c>
     </row>
@@ -2815,9 +3111,15 @@
       <c r="L53" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>4981</t>
+      <c r="M53" t="n">
+        <v>4981</v>
+      </c>
+      <c r="N53" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>5243</t>
         </is>
       </c>
     </row>
@@ -2864,9 +3166,15 @@
       <c r="L54" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M54" t="inlineStr">
-        <is>
-          <t>4321</t>
+      <c r="M54" t="n">
+        <v>4321</v>
+      </c>
+      <c r="N54" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>4503</t>
         </is>
       </c>
     </row>
@@ -2913,9 +3221,15 @@
       <c r="L55" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>4387</t>
+      <c r="M55" t="n">
+        <v>4387</v>
+      </c>
+      <c r="N55" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>4596</t>
         </is>
       </c>
     </row>
@@ -2962,9 +3276,15 @@
       <c r="L56" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>4765</t>
+      <c r="M56" t="n">
+        <v>4765</v>
+      </c>
+      <c r="N56" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>4950</t>
         </is>
       </c>
     </row>
@@ -3011,9 +3331,15 @@
       <c r="L57" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>4477</t>
+      <c r="M57" t="n">
+        <v>4477</v>
+      </c>
+      <c r="N57" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>4594</t>
         </is>
       </c>
     </row>
@@ -3060,9 +3386,15 @@
       <c r="L58" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M58" t="inlineStr">
-        <is>
-          <t>4067</t>
+      <c r="M58" t="n">
+        <v>4067</v>
+      </c>
+      <c r="N58" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>4522</t>
         </is>
       </c>
     </row>
@@ -3109,7 +3441,13 @@
       <c r="L59" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M59" t="inlineStr">
+      <c r="M59" t="n">
+        <v>0</v>
+      </c>
+      <c r="N59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O59" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3158,9 +3496,15 @@
       <c r="L60" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="M60" t="inlineStr">
-        <is>
-          <t>4991</t>
+      <c r="M60" t="n">
+        <v>4991</v>
+      </c>
+      <c r="N60" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>5277</t>
         </is>
       </c>
     </row>
@@ -3207,7 +3551,13 @@
       <c r="L61" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M61" t="inlineStr">
+      <c r="M61" t="n">
+        <v>2742</v>
+      </c>
+      <c r="N61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O61" t="inlineStr">
         <is>
           <t>2742</t>
         </is>
@@ -3256,9 +3606,15 @@
       <c r="L62" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M62" t="inlineStr">
-        <is>
-          <t>3229</t>
+      <c r="M62" t="n">
+        <v>3229</v>
+      </c>
+      <c r="N62" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>3253</t>
         </is>
       </c>
     </row>
@@ -3305,9 +3661,15 @@
       <c r="L63" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="M63" t="inlineStr">
-        <is>
-          <t>4701</t>
+      <c r="M63" t="n">
+        <v>4701</v>
+      </c>
+      <c r="N63" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>4948</t>
         </is>
       </c>
     </row>
@@ -3354,9 +3716,15 @@
       <c r="L64" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="M64" t="inlineStr">
-        <is>
-          <t>5030</t>
+      <c r="M64" t="n">
+        <v>5030</v>
+      </c>
+      <c r="N64" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>5283</t>
         </is>
       </c>
     </row>
@@ -3403,9 +3771,15 @@
       <c r="L65" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M65" t="inlineStr">
-        <is>
-          <t>2947</t>
+      <c r="M65" t="n">
+        <v>2947</v>
+      </c>
+      <c r="N65" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>2957</t>
         </is>
       </c>
     </row>
@@ -3452,9 +3826,15 @@
       <c r="L66" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="M66" t="inlineStr">
-        <is>
-          <t>4465</t>
+      <c r="M66" t="n">
+        <v>4465</v>
+      </c>
+      <c r="N66" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>4635</t>
         </is>
       </c>
     </row>
@@ -3501,9 +3881,15 @@
       <c r="L67" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="M67" t="inlineStr">
-        <is>
-          <t>2833</t>
+      <c r="M67" t="n">
+        <v>2833</v>
+      </c>
+      <c r="N67" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>2996</t>
         </is>
       </c>
     </row>
@@ -3550,7 +3936,13 @@
       <c r="L68" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M68" t="inlineStr">
+      <c r="M68" t="n">
+        <v>0</v>
+      </c>
+      <c r="N68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3599,9 +3991,15 @@
       <c r="L69" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="M69" t="inlineStr">
-        <is>
-          <t>4133</t>
+      <c r="M69" t="n">
+        <v>4133</v>
+      </c>
+      <c r="N69" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>4161</t>
         </is>
       </c>
     </row>
@@ -3648,9 +4046,15 @@
       <c r="L70" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M70" t="inlineStr">
-        <is>
-          <t>4399</t>
+      <c r="M70" t="n">
+        <v>4399</v>
+      </c>
+      <c r="N70" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>4506</t>
         </is>
       </c>
     </row>
@@ -3697,9 +4101,15 @@
       <c r="L71" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M71" t="inlineStr">
-        <is>
-          <t>2869</t>
+      <c r="M71" t="n">
+        <v>2869</v>
+      </c>
+      <c r="N71" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>2896</t>
         </is>
       </c>
     </row>
@@ -3746,9 +4156,15 @@
       <c r="L72" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M72" t="inlineStr">
-        <is>
-          <t>4283</t>
+      <c r="M72" t="n">
+        <v>4283</v>
+      </c>
+      <c r="N72" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>4408</t>
         </is>
       </c>
     </row>
@@ -3795,9 +4211,15 @@
       <c r="L73" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M73" t="inlineStr">
-        <is>
-          <t>4735</t>
+      <c r="M73" t="n">
+        <v>4735</v>
+      </c>
+      <c r="N73" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>4986</t>
         </is>
       </c>
     </row>
@@ -3844,7 +4266,13 @@
       <c r="L74" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M74" t="inlineStr">
+      <c r="M74" t="n">
+        <v>0</v>
+      </c>
+      <c r="N74" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3893,7 +4321,13 @@
       <c r="L75" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M75" t="inlineStr">
+      <c r="M75" t="n">
+        <v>0</v>
+      </c>
+      <c r="N75" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3942,9 +4376,15 @@
       <c r="L76" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M76" t="inlineStr">
-        <is>
-          <t>4844</t>
+      <c r="M76" t="n">
+        <v>4844</v>
+      </c>
+      <c r="N76" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>5024</t>
         </is>
       </c>
     </row>
@@ -3991,7 +4431,13 @@
       <c r="L77" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M77" t="inlineStr">
+      <c r="M77" t="n">
+        <v>0</v>
+      </c>
+      <c r="N77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4040,9 +4486,15 @@
       <c r="L78" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="M78" t="inlineStr">
-        <is>
-          <t>4592</t>
+      <c r="M78" t="n">
+        <v>4592</v>
+      </c>
+      <c r="N78" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>4869</t>
         </is>
       </c>
     </row>
@@ -4089,9 +4541,15 @@
       <c r="L79" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="M79" t="inlineStr">
-        <is>
-          <t>3182</t>
+      <c r="M79" t="n">
+        <v>3182</v>
+      </c>
+      <c r="N79" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>3164</t>
         </is>
       </c>
     </row>
@@ -4121,6 +4579,8 @@
       <c r="K80" t="inlineStr"/>
       <c r="L80" s="2" t="inlineStr"/>
       <c r="M80" t="inlineStr"/>
+      <c r="N80" s="2" t="inlineStr"/>
+      <c r="O80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -4165,9 +4625,15 @@
       <c r="L81" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M81" t="inlineStr">
-        <is>
-          <t>4658</t>
+      <c r="M81" t="n">
+        <v>4658</v>
+      </c>
+      <c r="N81" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>4991</t>
         </is>
       </c>
     </row>
@@ -4214,9 +4680,15 @@
       <c r="L82" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="M82" t="inlineStr">
-        <is>
-          <t>4676</t>
+      <c r="M82" t="n">
+        <v>4676</v>
+      </c>
+      <c r="N82" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>4852</t>
         </is>
       </c>
     </row>
@@ -4263,9 +4735,15 @@
       <c r="L83" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="M83" t="inlineStr">
-        <is>
-          <t>4414</t>
+      <c r="M83" t="n">
+        <v>4414</v>
+      </c>
+      <c r="N83" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>4562</t>
         </is>
       </c>
     </row>
@@ -4312,9 +4790,15 @@
       <c r="L84" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M84" t="inlineStr">
-        <is>
-          <t>4288</t>
+      <c r="M84" t="n">
+        <v>4288</v>
+      </c>
+      <c r="N84" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>4394</t>
         </is>
       </c>
     </row>
@@ -4361,9 +4845,15 @@
       <c r="L85" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M85" t="inlineStr">
-        <is>
-          <t>4236</t>
+      <c r="M85" t="n">
+        <v>4236</v>
+      </c>
+      <c r="N85" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>4341</t>
         </is>
       </c>
     </row>
@@ -4410,9 +4900,15 @@
       <c r="L86" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M86" t="inlineStr">
-        <is>
-          <t>3206</t>
+      <c r="M86" t="n">
+        <v>3206</v>
+      </c>
+      <c r="N86" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>3633</t>
         </is>
       </c>
     </row>
@@ -4459,9 +4955,15 @@
       <c r="L87" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M87" t="inlineStr">
-        <is>
-          <t>4510</t>
+      <c r="M87" t="n">
+        <v>4510</v>
+      </c>
+      <c r="N87" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>4705</t>
         </is>
       </c>
     </row>
@@ -4508,9 +5010,15 @@
       <c r="L88" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M88" t="inlineStr">
-        <is>
-          <t>3301</t>
+      <c r="M88" t="n">
+        <v>3301</v>
+      </c>
+      <c r="N88" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>3414</t>
         </is>
       </c>
     </row>
@@ -4557,9 +5065,15 @@
       <c r="L89" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="M89" t="inlineStr">
-        <is>
-          <t>3893</t>
+      <c r="M89" t="n">
+        <v>3893</v>
+      </c>
+      <c r="N89" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>4027</t>
         </is>
       </c>
     </row>
@@ -4606,9 +5120,15 @@
       <c r="L90" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M90" t="inlineStr">
-        <is>
-          <t>2853</t>
+      <c r="M90" t="n">
+        <v>2853</v>
+      </c>
+      <c r="N90" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>2864</t>
         </is>
       </c>
     </row>
@@ -4655,9 +5175,15 @@
       <c r="L91" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M91" t="inlineStr">
-        <is>
-          <t>3568</t>
+      <c r="M91" t="n">
+        <v>3568</v>
+      </c>
+      <c r="N91" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>3693</t>
         </is>
       </c>
     </row>
@@ -4704,7 +5230,13 @@
       <c r="L92" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M92" t="inlineStr">
+      <c r="M92" t="n">
+        <v>0</v>
+      </c>
+      <c r="N92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4753,9 +5285,15 @@
       <c r="L93" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="M93" t="inlineStr">
-        <is>
-          <t>3530</t>
+      <c r="M93" t="n">
+        <v>3530</v>
+      </c>
+      <c r="N93" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>3799</t>
         </is>
       </c>
     </row>
@@ -4802,9 +5340,15 @@
       <c r="L94" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M94" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M94" t="n">
+        <v>0</v>
+      </c>
+      <c r="N94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -4851,9 +5395,15 @@
       <c r="L95" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="M95" t="inlineStr">
-        <is>
-          <t>3986</t>
+      <c r="M95" t="n">
+        <v>3986</v>
+      </c>
+      <c r="N95" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>4034</t>
         </is>
       </c>
     </row>
@@ -4900,9 +5450,15 @@
       <c r="L96" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M96" t="inlineStr">
-        <is>
-          <t>2557</t>
+      <c r="M96" t="n">
+        <v>2557</v>
+      </c>
+      <c r="N96" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>2570</t>
         </is>
       </c>
     </row>
@@ -4949,9 +5505,15 @@
       <c r="L97" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M97" t="inlineStr">
-        <is>
-          <t>2187</t>
+      <c r="M97" t="n">
+        <v>2187</v>
+      </c>
+      <c r="N97" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>2186</t>
         </is>
       </c>
     </row>
@@ -4998,9 +5560,15 @@
       <c r="L98" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="M98" t="inlineStr">
-        <is>
-          <t>3326</t>
+      <c r="M98" t="n">
+        <v>3326</v>
+      </c>
+      <c r="N98" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>3357</t>
         </is>
       </c>
     </row>
@@ -5047,9 +5615,15 @@
       <c r="L99" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M99" t="inlineStr">
-        <is>
-          <t>2511</t>
+      <c r="M99" t="n">
+        <v>2511</v>
+      </c>
+      <c r="N99" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>2502</t>
         </is>
       </c>
     </row>
@@ -5096,9 +5670,15 @@
       <c r="L100" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="M100" t="inlineStr">
-        <is>
-          <t>3666</t>
+      <c r="M100" t="n">
+        <v>3666</v>
+      </c>
+      <c r="N100" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>3920</t>
         </is>
       </c>
     </row>
@@ -5145,9 +5725,15 @@
       <c r="L101" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M101" t="inlineStr">
-        <is>
-          <t>2317</t>
+      <c r="M101" t="n">
+        <v>2317</v>
+      </c>
+      <c r="N101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>2333</t>
         </is>
       </c>
     </row>
@@ -5194,9 +5780,15 @@
       <c r="L102" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M102" t="inlineStr">
-        <is>
-          <t>4635</t>
+      <c r="M102" t="n">
+        <v>4635</v>
+      </c>
+      <c r="N102" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>4814</t>
         </is>
       </c>
     </row>
@@ -5243,9 +5835,15 @@
       <c r="L103" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M103" t="inlineStr">
-        <is>
-          <t>4169</t>
+      <c r="M103" t="n">
+        <v>4169</v>
+      </c>
+      <c r="N103" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>4422</t>
         </is>
       </c>
     </row>
@@ -5292,9 +5890,15 @@
       <c r="L104" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M104" t="inlineStr">
-        <is>
-          <t>4189</t>
+      <c r="M104" t="n">
+        <v>4189</v>
+      </c>
+      <c r="N104" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>4278</t>
         </is>
       </c>
     </row>
@@ -5341,9 +5945,15 @@
       <c r="L105" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M105" t="inlineStr">
-        <is>
-          <t>4460</t>
+      <c r="M105" t="n">
+        <v>4460</v>
+      </c>
+      <c r="N105" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>4645</t>
         </is>
       </c>
     </row>
@@ -5390,9 +6000,15 @@
       <c r="L106" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="M106" t="inlineStr">
-        <is>
-          <t>4196</t>
+      <c r="M106" t="n">
+        <v>4196</v>
+      </c>
+      <c r="N106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>4241</t>
         </is>
       </c>
     </row>
@@ -5439,9 +6055,15 @@
       <c r="L107" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="M107" t="inlineStr">
-        <is>
-          <t>4265</t>
+      <c r="M107" t="n">
+        <v>4265</v>
+      </c>
+      <c r="N107" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>4519</t>
         </is>
       </c>
     </row>
@@ -5488,7 +6110,13 @@
       <c r="L108" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M108" t="inlineStr">
+      <c r="M108" t="n">
+        <v>0</v>
+      </c>
+      <c r="N108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5537,9 +6165,15 @@
       <c r="L109" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="M109" t="inlineStr">
-        <is>
-          <t>2993</t>
+      <c r="M109" t="n">
+        <v>2993</v>
+      </c>
+      <c r="N109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>2990</t>
         </is>
       </c>
     </row>
@@ -5586,7 +6220,13 @@
       <c r="L110" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M110" t="inlineStr">
+      <c r="M110" t="n">
+        <v>0</v>
+      </c>
+      <c r="N110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O110" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5635,9 +6275,15 @@
       <c r="L111" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M111" t="inlineStr">
-        <is>
-          <t>3894</t>
+      <c r="M111" t="n">
+        <v>3894</v>
+      </c>
+      <c r="N111" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="O111" t="inlineStr">
+        <is>
+          <t>4308</t>
         </is>
       </c>
     </row>
@@ -5684,9 +6330,15 @@
       <c r="L112" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M112" t="inlineStr">
-        <is>
-          <t>4187</t>
+      <c r="M112" t="n">
+        <v>4187</v>
+      </c>
+      <c r="N112" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>4311</t>
         </is>
       </c>
     </row>
@@ -5733,9 +6385,15 @@
       <c r="L113" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M113" t="inlineStr">
-        <is>
-          <t>3624</t>
+      <c r="M113" t="n">
+        <v>3624</v>
+      </c>
+      <c r="N113" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>3904</t>
         </is>
       </c>
     </row>
@@ -5782,9 +6440,15 @@
       <c r="L114" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M114" t="inlineStr">
-        <is>
-          <t>2547</t>
+      <c r="M114" t="n">
+        <v>2547</v>
+      </c>
+      <c r="N114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>2551</t>
         </is>
       </c>
     </row>
@@ -5831,9 +6495,15 @@
       <c r="L115" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="M115" t="inlineStr">
-        <is>
-          <t>3874</t>
+      <c r="M115" t="n">
+        <v>3874</v>
+      </c>
+      <c r="N115" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="O115" t="inlineStr">
+        <is>
+          <t>4159</t>
         </is>
       </c>
     </row>
@@ -5880,9 +6550,15 @@
       <c r="L116" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M116" t="inlineStr">
-        <is>
-          <t>3094</t>
+      <c r="M116" t="n">
+        <v>3094</v>
+      </c>
+      <c r="N116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O116" t="inlineStr">
+        <is>
+          <t>3109</t>
         </is>
       </c>
     </row>
@@ -5929,9 +6605,15 @@
       <c r="L117" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M117" t="inlineStr">
-        <is>
-          <t>2393</t>
+      <c r="M117" t="n">
+        <v>2393</v>
+      </c>
+      <c r="N117" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>2451</t>
         </is>
       </c>
     </row>
@@ -5978,9 +6660,15 @@
       <c r="L118" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="M118" t="inlineStr">
-        <is>
-          <t>3080</t>
+      <c r="M118" t="n">
+        <v>3080</v>
+      </c>
+      <c r="N118" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="O118" t="inlineStr">
+        <is>
+          <t>3189</t>
         </is>
       </c>
     </row>
@@ -6027,9 +6715,15 @@
       <c r="L119" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M119" t="inlineStr">
-        <is>
-          <t>4232</t>
+      <c r="M119" t="n">
+        <v>4232</v>
+      </c>
+      <c r="N119" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O119" t="inlineStr">
+        <is>
+          <t>4413</t>
         </is>
       </c>
     </row>
@@ -6076,9 +6770,15 @@
       <c r="L120" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M120" t="inlineStr">
-        <is>
-          <t>2623</t>
+      <c r="M120" t="n">
+        <v>2623</v>
+      </c>
+      <c r="N120" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O120" t="inlineStr">
+        <is>
+          <t>2742</t>
         </is>
       </c>
     </row>
@@ -6125,7 +6825,13 @@
       <c r="L121" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="M121" t="inlineStr">
+      <c r="M121" t="n">
+        <v>1601</v>
+      </c>
+      <c r="N121" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O121" t="inlineStr">
         <is>
           <t>1601</t>
         </is>
@@ -6174,9 +6880,15 @@
       <c r="L122" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M122" t="inlineStr">
-        <is>
-          <t>3007</t>
+      <c r="M122" t="n">
+        <v>3007</v>
+      </c>
+      <c r="N122" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O122" t="inlineStr">
+        <is>
+          <t>3224</t>
         </is>
       </c>
     </row>
@@ -6223,9 +6935,15 @@
       <c r="L123" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="M123" t="inlineStr">
-        <is>
-          <t>4193</t>
+      <c r="M123" t="n">
+        <v>4193</v>
+      </c>
+      <c r="N123" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="O123" t="inlineStr">
+        <is>
+          <t>4185</t>
         </is>
       </c>
     </row>
@@ -6272,7 +6990,13 @@
       <c r="L124" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M124" t="inlineStr">
+      <c r="M124" t="n">
+        <v>0</v>
+      </c>
+      <c r="N124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O124" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6321,9 +7045,15 @@
       <c r="L125" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M125" t="inlineStr">
-        <is>
-          <t>3991</t>
+      <c r="M125" t="n">
+        <v>3991</v>
+      </c>
+      <c r="N125" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O125" t="inlineStr">
+        <is>
+          <t>3997</t>
         </is>
       </c>
     </row>
@@ -6370,9 +7100,15 @@
       <c r="L126" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="M126" t="inlineStr">
-        <is>
-          <t>3720</t>
+      <c r="M126" t="n">
+        <v>3720</v>
+      </c>
+      <c r="N126" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="O126" t="inlineStr">
+        <is>
+          <t>3994</t>
         </is>
       </c>
     </row>
@@ -6419,9 +7155,15 @@
       <c r="L127" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M127" t="inlineStr">
-        <is>
-          <t>3329</t>
+      <c r="M127" t="n">
+        <v>3329</v>
+      </c>
+      <c r="N127" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O127" t="inlineStr">
+        <is>
+          <t>3378</t>
         </is>
       </c>
     </row>
@@ -6468,9 +7210,15 @@
       <c r="L128" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="M128" t="inlineStr">
-        <is>
-          <t>3991</t>
+      <c r="M128" t="n">
+        <v>3991</v>
+      </c>
+      <c r="N128" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O128" t="inlineStr">
+        <is>
+          <t>4071</t>
         </is>
       </c>
     </row>
@@ -6517,9 +7265,15 @@
       <c r="L129" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M129" t="inlineStr">
-        <is>
-          <t>2017</t>
+      <c r="M129" t="n">
+        <v>2017</v>
+      </c>
+      <c r="N129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O129" t="inlineStr">
+        <is>
+          <t>2025</t>
         </is>
       </c>
     </row>
@@ -6566,7 +7320,13 @@
       <c r="L130" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M130" t="inlineStr">
+      <c r="M130" t="n">
+        <v>0</v>
+      </c>
+      <c r="N130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6615,7 +7375,13 @@
       <c r="L131" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M131" t="inlineStr">
+      <c r="M131" t="n">
+        <v>0</v>
+      </c>
+      <c r="N131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6664,9 +7430,15 @@
       <c r="L132" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M132" t="inlineStr">
-        <is>
-          <t>3778</t>
+      <c r="M132" t="n">
+        <v>3778</v>
+      </c>
+      <c r="N132" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O132" t="inlineStr">
+        <is>
+          <t>3932</t>
         </is>
       </c>
     </row>
@@ -6713,7 +7485,13 @@
       <c r="L133" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M133" t="inlineStr">
+      <c r="M133" t="n">
+        <v>0</v>
+      </c>
+      <c r="N133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6762,9 +7540,15 @@
       <c r="L134" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M134" t="inlineStr">
-        <is>
-          <t>3192</t>
+      <c r="M134" t="n">
+        <v>3192</v>
+      </c>
+      <c r="N134" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O134" t="inlineStr">
+        <is>
+          <t>3321</t>
         </is>
       </c>
     </row>
@@ -6811,9 +7595,15 @@
       <c r="L135" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M135" t="inlineStr">
-        <is>
-          <t>3992</t>
+      <c r="M135" t="n">
+        <v>3992</v>
+      </c>
+      <c r="N135" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O135" t="inlineStr">
+        <is>
+          <t>3993</t>
         </is>
       </c>
     </row>
@@ -6860,9 +7650,15 @@
       <c r="L136" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M136" t="inlineStr">
-        <is>
-          <t>4016</t>
+      <c r="M136" t="n">
+        <v>4016</v>
+      </c>
+      <c r="N136" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O136" t="inlineStr">
+        <is>
+          <t>4048</t>
         </is>
       </c>
     </row>
@@ -6909,7 +7705,13 @@
       <c r="L137" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M137" t="inlineStr">
+      <c r="M137" t="n">
+        <v>0</v>
+      </c>
+      <c r="N137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6958,7 +7760,13 @@
       <c r="L138" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M138" t="inlineStr">
+      <c r="M138" t="n">
+        <v>0</v>
+      </c>
+      <c r="N138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O138" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7007,9 +7815,15 @@
       <c r="L139" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="M139" t="inlineStr">
-        <is>
-          <t>3094</t>
+      <c r="M139" t="n">
+        <v>3094</v>
+      </c>
+      <c r="N139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O139" t="inlineStr">
+        <is>
+          <t>3108</t>
         </is>
       </c>
     </row>
@@ -7056,7 +7870,13 @@
       <c r="L140" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M140" t="inlineStr">
+      <c r="M140" t="n">
+        <v>0</v>
+      </c>
+      <c r="N140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7105,7 +7925,13 @@
       <c r="L141" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M141" t="inlineStr">
+      <c r="M141" t="n">
+        <v>0</v>
+      </c>
+      <c r="N141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7154,9 +7980,15 @@
       <c r="L142" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="M142" t="inlineStr">
-        <is>
-          <t>3139</t>
+      <c r="M142" t="n">
+        <v>3139</v>
+      </c>
+      <c r="N142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O142" t="inlineStr">
+        <is>
+          <t>3124</t>
         </is>
       </c>
     </row>
@@ -7203,7 +8035,13 @@
       <c r="L143" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M143" t="inlineStr">
+      <c r="M143" t="n">
+        <v>0</v>
+      </c>
+      <c r="N143" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7252,9 +8090,15 @@
       <c r="L144" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="M144" t="inlineStr">
-        <is>
-          <t>3314</t>
+      <c r="M144" t="n">
+        <v>3314</v>
+      </c>
+      <c r="N144" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O144" t="inlineStr">
+        <is>
+          <t>3291</t>
         </is>
       </c>
     </row>
@@ -7301,7 +8145,13 @@
       <c r="L145" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M145" t="inlineStr">
+      <c r="M145" t="n">
+        <v>0</v>
+      </c>
+      <c r="N145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7350,7 +8200,13 @@
       <c r="L146" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M146" t="inlineStr">
+      <c r="M146" t="n">
+        <v>0</v>
+      </c>
+      <c r="N146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7399,9 +8255,15 @@
       <c r="L147" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M147" t="inlineStr">
-        <is>
-          <t>2074</t>
+      <c r="M147" t="n">
+        <v>2074</v>
+      </c>
+      <c r="N147" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O147" t="inlineStr">
+        <is>
+          <t>2070</t>
         </is>
       </c>
     </row>
@@ -7448,7 +8310,13 @@
       <c r="L148" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M148" t="inlineStr">
+      <c r="M148" t="n">
+        <v>0</v>
+      </c>
+      <c r="N148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7497,7 +8365,13 @@
       <c r="L149" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M149" t="inlineStr">
+      <c r="M149" t="n">
+        <v>0</v>
+      </c>
+      <c r="N149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7546,7 +8420,13 @@
       <c r="L150" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M150" t="inlineStr">
+      <c r="M150" t="n">
+        <v>2556</v>
+      </c>
+      <c r="N150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O150" t="inlineStr">
         <is>
           <t>2556</t>
         </is>
@@ -7595,7 +8475,13 @@
       <c r="L151" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M151" t="inlineStr">
+      <c r="M151" t="n">
+        <v>0</v>
+      </c>
+      <c r="N151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7644,7 +8530,13 @@
       <c r="L152" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M152" t="inlineStr">
+      <c r="M152" t="n">
+        <v>0</v>
+      </c>
+      <c r="N152" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7693,7 +8585,13 @@
       <c r="L153" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M153" t="inlineStr">
+      <c r="M153" t="n">
+        <v>0</v>
+      </c>
+      <c r="N153" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7742,9 +8640,15 @@
       <c r="L154" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M154" t="inlineStr">
-        <is>
-          <t>2916</t>
+      <c r="M154" t="n">
+        <v>2916</v>
+      </c>
+      <c r="N154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O154" t="inlineStr">
+        <is>
+          <t>2910</t>
         </is>
       </c>
     </row>
@@ -7791,7 +8695,13 @@
       <c r="L155" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M155" t="inlineStr">
+      <c r="M155" t="n">
+        <v>0</v>
+      </c>
+      <c r="N155" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7840,7 +8750,13 @@
       <c r="L156" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M156" t="inlineStr">
+      <c r="M156" t="n">
+        <v>0</v>
+      </c>
+      <c r="N156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7889,7 +8805,13 @@
       <c r="L157" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M157" t="inlineStr">
+      <c r="M157" t="n">
+        <v>0</v>
+      </c>
+      <c r="N157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7938,9 +8860,15 @@
       <c r="L158" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M158" t="inlineStr">
-        <is>
-          <t>2929</t>
+      <c r="M158" t="n">
+        <v>2929</v>
+      </c>
+      <c r="N158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O158" t="inlineStr">
+        <is>
+          <t>2952</t>
         </is>
       </c>
     </row>
@@ -7980,6 +8908,8 @@
       </c>
       <c r="L159" s="2" t="inlineStr"/>
       <c r="M159" t="inlineStr"/>
+      <c r="N159" s="2" t="inlineStr"/>
+      <c r="O159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="n">
@@ -8018,9 +8948,15 @@
       <c r="L160" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M160" t="inlineStr">
-        <is>
-          <t>4314</t>
+      <c r="M160" t="n">
+        <v>4314</v>
+      </c>
+      <c r="N160" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O160" t="inlineStr">
+        <is>
+          <t>4464</t>
         </is>
       </c>
     </row>
@@ -8052,6 +8988,8 @@
       <c r="K161" t="inlineStr"/>
       <c r="L161" s="2" t="inlineStr"/>
       <c r="M161" t="inlineStr"/>
+      <c r="N161" s="2" t="inlineStr"/>
+      <c r="O161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="n">
@@ -8090,9 +9028,15 @@
       <c r="L162" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M162" t="inlineStr">
-        <is>
-          <t>3451</t>
+      <c r="M162" t="n">
+        <v>3451</v>
+      </c>
+      <c r="N162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O162" t="inlineStr">
+        <is>
+          <t>3518</t>
         </is>
       </c>
     </row>
@@ -8133,9 +9077,15 @@
       <c r="L163" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="M163" t="inlineStr">
-        <is>
-          <t>2713</t>
+      <c r="M163" t="n">
+        <v>2713</v>
+      </c>
+      <c r="N163" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="O163" t="inlineStr">
+        <is>
+          <t>2751</t>
         </is>
       </c>
     </row>
@@ -8172,9 +9122,15 @@
       <c r="L164" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="M164" t="inlineStr">
-        <is>
-          <t>2901</t>
+      <c r="M164" t="n">
+        <v>2901</v>
+      </c>
+      <c r="N164" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="O164" t="inlineStr">
+        <is>
+          <t>3029</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-21 11:30:55
</commit_message>
<xml_diff>
--- a/Season_Attack/86.xlsx
+++ b/Season_Attack/86.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O164"/>
+  <dimension ref="A1:Q164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,16 @@
           <t>03-19_0</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>03-20_A</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>03-20_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -516,9 +526,15 @@
       <c r="N2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>3070</t>
+      <c r="O2" t="n">
+        <v>3070</v>
+      </c>
+      <c r="P2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>3067</t>
         </is>
       </c>
     </row>
@@ -562,6 +578,14 @@
       <c r="M3" t="inlineStr"/>
       <c r="N3" s="2" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
+      <c r="P3" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>5812</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -612,9 +636,15 @@
       <c r="N4" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>5391</t>
+      <c r="O4" t="n">
+        <v>5391</v>
+      </c>
+      <c r="P4" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>5752</t>
         </is>
       </c>
     </row>
@@ -637,7 +667,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F5" s="2" t="n">
@@ -667,9 +697,15 @@
       <c r="N5" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>5510</t>
+      <c r="O5" t="n">
+        <v>5510</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>5808</t>
         </is>
       </c>
     </row>
@@ -722,9 +758,15 @@
       <c r="N6" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>5256</t>
+      <c r="O6" t="n">
+        <v>5256</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>5489</t>
         </is>
       </c>
     </row>
@@ -747,7 +789,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F7" s="4" t="n">
@@ -777,9 +819,15 @@
       <c r="N7" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>5649</t>
+      <c r="O7" t="n">
+        <v>5649</v>
+      </c>
+      <c r="P7" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>6070</t>
         </is>
       </c>
     </row>
@@ -832,9 +880,15 @@
       <c r="N8" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>4972</t>
+      <c r="O8" t="n">
+        <v>4972</v>
+      </c>
+      <c r="P8" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>5138</t>
         </is>
       </c>
     </row>
@@ -887,9 +941,15 @@
       <c r="N9" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>5097</t>
+      <c r="O9" t="n">
+        <v>5097</v>
+      </c>
+      <c r="P9" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>5543</t>
         </is>
       </c>
     </row>
@@ -942,9 +1002,15 @@
       <c r="N10" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>5190</t>
+      <c r="O10" t="n">
+        <v>5190</v>
+      </c>
+      <c r="P10" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>5679</t>
         </is>
       </c>
     </row>
@@ -988,6 +1054,8 @@
       <c r="M11" t="inlineStr"/>
       <c r="N11" s="2" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
+      <c r="P11" s="2" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1038,9 +1106,15 @@
       <c r="N12" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>3304</t>
+      <c r="O12" t="n">
+        <v>3304</v>
+      </c>
+      <c r="P12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>3336</t>
         </is>
       </c>
     </row>
@@ -1093,9 +1167,15 @@
       <c r="N13" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>6012</t>
+      <c r="O13" t="n">
+        <v>6012</v>
+      </c>
+      <c r="P13" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>6269</t>
         </is>
       </c>
     </row>
@@ -1148,9 +1228,15 @@
       <c r="N14" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>5185</t>
+      <c r="O14" t="n">
+        <v>5185</v>
+      </c>
+      <c r="P14" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>5366</t>
         </is>
       </c>
     </row>
@@ -1187,9 +1273,15 @@
       <c r="N15" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>5472</t>
+      <c r="O15" t="n">
+        <v>5472</v>
+      </c>
+      <c r="P15" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>5662</t>
         </is>
       </c>
     </row>
@@ -1242,9 +1334,15 @@
       <c r="N16" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>4608</t>
+      <c r="O16" t="n">
+        <v>4608</v>
+      </c>
+      <c r="P16" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>4708</t>
         </is>
       </c>
     </row>
@@ -1297,9 +1395,15 @@
       <c r="N17" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>4710</t>
+      <c r="O17" t="n">
+        <v>4710</v>
+      </c>
+      <c r="P17" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>4827</t>
         </is>
       </c>
     </row>
@@ -1352,9 +1456,15 @@
       <c r="N18" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>5137</t>
+      <c r="O18" t="n">
+        <v>5137</v>
+      </c>
+      <c r="P18" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>5459</t>
         </is>
       </c>
     </row>
@@ -1391,9 +1501,15 @@
       <c r="N19" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>5984</t>
+      <c r="O19" t="n">
+        <v>5984</v>
+      </c>
+      <c r="P19" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>6297</t>
         </is>
       </c>
     </row>
@@ -1446,7 +1562,13 @@
       <c r="N20" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O20" t="inlineStr">
+      <c r="O20" t="n">
+        <v>4426</v>
+      </c>
+      <c r="P20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="inlineStr">
         <is>
           <t>4426</t>
         </is>
@@ -1501,9 +1623,15 @@
       <c r="N21" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>5405</t>
+      <c r="O21" t="n">
+        <v>5405</v>
+      </c>
+      <c r="P21" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>5651</t>
         </is>
       </c>
     </row>
@@ -1556,9 +1684,15 @@
       <c r="N22" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>4107</t>
+      <c r="O22" t="n">
+        <v>4107</v>
+      </c>
+      <c r="P22" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>4803</t>
         </is>
       </c>
     </row>
@@ -1611,9 +1745,15 @@
       <c r="N23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>5431</t>
+      <c r="O23" t="n">
+        <v>5431</v>
+      </c>
+      <c r="P23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>5590</t>
         </is>
       </c>
     </row>
@@ -1666,7 +1806,13 @@
       <c r="N24" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O24" t="inlineStr">
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1721,7 +1867,13 @@
       <c r="N25" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O25" t="inlineStr">
+      <c r="O25" t="n">
+        <v>2609</v>
+      </c>
+      <c r="P25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="inlineStr">
         <is>
           <t>2609</t>
         </is>
@@ -1744,7 +1896,11 @@
       <c r="D26" t="n">
         <v>6592</v>
       </c>
-      <c r="E26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
       <c r="F26" s="2" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
       <c r="H26" s="2" t="inlineStr"/>
@@ -1755,6 +1911,14 @@
       <c r="M26" t="inlineStr"/>
       <c r="N26" s="2" t="inlineStr"/>
       <c r="O26" t="inlineStr"/>
+      <c r="P26" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>5755</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1773,7 +1937,11 @@
       <c r="D27" t="n">
         <v>6148</v>
       </c>
-      <c r="E27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
       <c r="F27" s="2" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
       <c r="H27" s="2" t="inlineStr"/>
@@ -1784,6 +1952,14 @@
       <c r="M27" t="inlineStr"/>
       <c r="N27" s="2" t="inlineStr"/>
       <c r="O27" t="inlineStr"/>
+      <c r="P27" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>4641</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1834,9 +2010,15 @@
       <c r="N28" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>5594</t>
+      <c r="O28" t="n">
+        <v>5594</v>
+      </c>
+      <c r="P28" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>5956</t>
         </is>
       </c>
     </row>
@@ -1857,7 +2039,11 @@
       <c r="D29" t="n">
         <v>6444</v>
       </c>
-      <c r="E29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
       <c r="F29" s="2" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
       <c r="H29" s="2" t="inlineStr"/>
@@ -1868,6 +2054,14 @@
       <c r="M29" t="inlineStr"/>
       <c r="N29" s="2" t="inlineStr"/>
       <c r="O29" t="inlineStr"/>
+      <c r="P29" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>5112</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1918,9 +2112,15 @@
       <c r="N30" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>4516</t>
+      <c r="O30" t="n">
+        <v>4516</v>
+      </c>
+      <c r="P30" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>4802</t>
         </is>
       </c>
     </row>
@@ -1973,9 +2173,15 @@
       <c r="N31" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>5715</t>
+      <c r="O31" t="n">
+        <v>5715</v>
+      </c>
+      <c r="P31" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>6184</t>
         </is>
       </c>
     </row>
@@ -2019,6 +2225,8 @@
       <c r="M32" t="inlineStr"/>
       <c r="N32" s="2" t="inlineStr"/>
       <c r="O32" t="inlineStr"/>
+      <c r="P32" s="2" t="inlineStr"/>
+      <c r="Q32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2069,9 +2277,15 @@
       <c r="N33" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O33" t="inlineStr">
-        <is>
-          <t>5147</t>
+      <c r="O33" t="n">
+        <v>5147</v>
+      </c>
+      <c r="P33" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>5389</t>
         </is>
       </c>
     </row>
@@ -2124,9 +2338,15 @@
       <c r="N34" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="O34" t="inlineStr">
-        <is>
-          <t>5727</t>
+      <c r="O34" t="n">
+        <v>5727</v>
+      </c>
+      <c r="P34" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>5975</t>
         </is>
       </c>
     </row>
@@ -2179,9 +2399,15 @@
       <c r="N35" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>5141</t>
+      <c r="O35" t="n">
+        <v>5141</v>
+      </c>
+      <c r="P35" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>5392</t>
         </is>
       </c>
     </row>
@@ -2202,7 +2428,11 @@
       <c r="D36" t="n">
         <v>4600</v>
       </c>
-      <c r="E36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
       <c r="F36" s="2" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
       <c r="H36" s="2" t="inlineStr"/>
@@ -2213,6 +2443,14 @@
       <c r="M36" t="inlineStr"/>
       <c r="N36" s="2" t="inlineStr"/>
       <c r="O36" t="inlineStr"/>
+      <c r="P36" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>4867</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2263,9 +2501,15 @@
       <c r="N37" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>5347</t>
+      <c r="O37" t="n">
+        <v>5347</v>
+      </c>
+      <c r="P37" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>5584</t>
         </is>
       </c>
     </row>
@@ -2318,9 +2562,15 @@
       <c r="N38" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>5203</t>
+      <c r="O38" t="n">
+        <v>5203</v>
+      </c>
+      <c r="P38" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>5334</t>
         </is>
       </c>
     </row>
@@ -2373,9 +2623,15 @@
       <c r="N39" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>5556</t>
+      <c r="O39" t="n">
+        <v>5556</v>
+      </c>
+      <c r="P39" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>5781</t>
         </is>
       </c>
     </row>
@@ -2428,9 +2684,15 @@
       <c r="N40" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>6003</t>
+      <c r="O40" t="n">
+        <v>6003</v>
+      </c>
+      <c r="P40" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>6233</t>
         </is>
       </c>
     </row>
@@ -2453,7 +2715,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F41" s="4" t="n">
@@ -2483,9 +2745,15 @@
       <c r="N41" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>5504</t>
+      <c r="O41" t="n">
+        <v>5504</v>
+      </c>
+      <c r="P41" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>5622</t>
         </is>
       </c>
     </row>
@@ -2538,9 +2806,15 @@
       <c r="N42" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>5238</t>
+      <c r="O42" t="n">
+        <v>5238</v>
+      </c>
+      <c r="P42" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>5273</t>
         </is>
       </c>
     </row>
@@ -2593,9 +2867,15 @@
       <c r="N43" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>4883</t>
+      <c r="O43" t="n">
+        <v>4883</v>
+      </c>
+      <c r="P43" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>5054</t>
         </is>
       </c>
     </row>
@@ -2648,9 +2928,15 @@
       <c r="N44" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>4977</t>
+      <c r="O44" t="n">
+        <v>4977</v>
+      </c>
+      <c r="P44" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>5281</t>
         </is>
       </c>
     </row>
@@ -2703,9 +2989,15 @@
       <c r="N45" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>4511</t>
+      <c r="O45" t="n">
+        <v>4511</v>
+      </c>
+      <c r="P45" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>4752</t>
         </is>
       </c>
     </row>
@@ -2758,9 +3050,15 @@
       <c r="N46" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>5589</t>
+      <c r="O46" t="n">
+        <v>5589</v>
+      </c>
+      <c r="P46" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>5899</t>
         </is>
       </c>
     </row>
@@ -2813,9 +3111,15 @@
       <c r="N47" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>4528</t>
+      <c r="O47" t="n">
+        <v>4528</v>
+      </c>
+      <c r="P47" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>4856</t>
         </is>
       </c>
     </row>
@@ -2868,7 +3172,13 @@
       <c r="N48" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O48" t="inlineStr">
+      <c r="O48" t="n">
+        <v>2516</v>
+      </c>
+      <c r="P48" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q48" t="inlineStr">
         <is>
           <t>2516</t>
         </is>
@@ -2902,6 +3212,8 @@
       <c r="M49" t="inlineStr"/>
       <c r="N49" s="2" t="inlineStr"/>
       <c r="O49" t="inlineStr"/>
+      <c r="P49" s="2" t="inlineStr"/>
+      <c r="Q49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -2952,7 +3264,13 @@
       <c r="N50" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O50" t="inlineStr">
+      <c r="O50" t="n">
+        <v>0</v>
+      </c>
+      <c r="P50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q50" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3007,9 +3325,15 @@
       <c r="N51" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>2728</t>
+      <c r="O51" t="n">
+        <v>2728</v>
+      </c>
+      <c r="P51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>2726</t>
         </is>
       </c>
     </row>
@@ -3062,7 +3386,13 @@
       <c r="N52" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O52" t="inlineStr">
+      <c r="O52" t="n">
+        <v>3168</v>
+      </c>
+      <c r="P52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q52" t="inlineStr">
         <is>
           <t>3168</t>
         </is>
@@ -3117,9 +3447,15 @@
       <c r="N53" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>5243</t>
+      <c r="O53" t="n">
+        <v>5243</v>
+      </c>
+      <c r="P53" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>5476</t>
         </is>
       </c>
     </row>
@@ -3172,9 +3508,15 @@
       <c r="N54" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t>4503</t>
+      <c r="O54" t="n">
+        <v>4503</v>
+      </c>
+      <c r="P54" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>4670</t>
         </is>
       </c>
     </row>
@@ -3227,9 +3569,15 @@
       <c r="N55" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>4596</t>
+      <c r="O55" t="n">
+        <v>4596</v>
+      </c>
+      <c r="P55" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>4782</t>
         </is>
       </c>
     </row>
@@ -3282,9 +3630,15 @@
       <c r="N56" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>4950</t>
+      <c r="O56" t="n">
+        <v>4950</v>
+      </c>
+      <c r="P56" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>5243</t>
         </is>
       </c>
     </row>
@@ -3337,9 +3691,15 @@
       <c r="N57" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>4594</t>
+      <c r="O57" t="n">
+        <v>4594</v>
+      </c>
+      <c r="P57" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>4773</t>
         </is>
       </c>
     </row>
@@ -3392,9 +3752,15 @@
       <c r="N58" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>4522</t>
+      <c r="O58" t="n">
+        <v>4522</v>
+      </c>
+      <c r="P58" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>4573</t>
         </is>
       </c>
     </row>
@@ -3447,7 +3813,13 @@
       <c r="N59" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O59" t="inlineStr">
+      <c r="O59" t="n">
+        <v>0</v>
+      </c>
+      <c r="P59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q59" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3502,9 +3874,15 @@
       <c r="N60" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="O60" t="inlineStr">
-        <is>
-          <t>5277</t>
+      <c r="O60" t="n">
+        <v>5277</v>
+      </c>
+      <c r="P60" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>5452</t>
         </is>
       </c>
     </row>
@@ -3557,9 +3935,15 @@
       <c r="N61" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>2742</t>
+      <c r="O61" t="n">
+        <v>2742</v>
+      </c>
+      <c r="P61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>2758</t>
         </is>
       </c>
     </row>
@@ -3612,9 +3996,15 @@
       <c r="N62" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>3253</t>
+      <c r="O62" t="n">
+        <v>3253</v>
+      </c>
+      <c r="P62" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>3246</t>
         </is>
       </c>
     </row>
@@ -3667,9 +4057,15 @@
       <c r="N63" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>4948</t>
+      <c r="O63" t="n">
+        <v>4948</v>
+      </c>
+      <c r="P63" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>5115</t>
         </is>
       </c>
     </row>
@@ -3722,9 +4118,15 @@
       <c r="N64" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>5283</t>
+      <c r="O64" t="n">
+        <v>5283</v>
+      </c>
+      <c r="P64" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>5700</t>
         </is>
       </c>
     </row>
@@ -3777,9 +4179,15 @@
       <c r="N65" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O65" t="inlineStr">
-        <is>
-          <t>2957</t>
+      <c r="O65" t="n">
+        <v>2957</v>
+      </c>
+      <c r="P65" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>2952</t>
         </is>
       </c>
     </row>
@@ -3832,9 +4240,15 @@
       <c r="N66" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>4635</t>
+      <c r="O66" t="n">
+        <v>4635</v>
+      </c>
+      <c r="P66" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>4808</t>
         </is>
       </c>
     </row>
@@ -3887,9 +4301,15 @@
       <c r="N67" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="O67" t="inlineStr">
-        <is>
-          <t>2996</t>
+      <c r="O67" t="n">
+        <v>2996</v>
+      </c>
+      <c r="P67" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>3389</t>
         </is>
       </c>
     </row>
@@ -3942,7 +4362,13 @@
       <c r="N68" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O68" t="inlineStr">
+      <c r="O68" t="n">
+        <v>0</v>
+      </c>
+      <c r="P68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3997,9 +4423,15 @@
       <c r="N69" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="O69" t="inlineStr">
-        <is>
-          <t>4161</t>
+      <c r="O69" t="n">
+        <v>4161</v>
+      </c>
+      <c r="P69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>4130</t>
         </is>
       </c>
     </row>
@@ -4052,9 +4484,15 @@
       <c r="N70" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O70" t="inlineStr">
-        <is>
-          <t>4506</t>
+      <c r="O70" t="n">
+        <v>4506</v>
+      </c>
+      <c r="P70" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>4709</t>
         </is>
       </c>
     </row>
@@ -4107,9 +4545,15 @@
       <c r="N71" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O71" t="inlineStr">
-        <is>
-          <t>2896</t>
+      <c r="O71" t="n">
+        <v>2896</v>
+      </c>
+      <c r="P71" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>3198</t>
         </is>
       </c>
     </row>
@@ -4162,9 +4606,15 @@
       <c r="N72" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O72" t="inlineStr">
-        <is>
-          <t>4408</t>
+      <c r="O72" t="n">
+        <v>4408</v>
+      </c>
+      <c r="P72" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>4513</t>
         </is>
       </c>
     </row>
@@ -4217,9 +4667,15 @@
       <c r="N73" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O73" t="inlineStr">
-        <is>
-          <t>4986</t>
+      <c r="O73" t="n">
+        <v>4986</v>
+      </c>
+      <c r="P73" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>5174</t>
         </is>
       </c>
     </row>
@@ -4272,7 +4728,13 @@
       <c r="N74" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O74" t="inlineStr">
+      <c r="O74" t="n">
+        <v>0</v>
+      </c>
+      <c r="P74" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4327,7 +4789,13 @@
       <c r="N75" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O75" t="inlineStr">
+      <c r="O75" t="n">
+        <v>0</v>
+      </c>
+      <c r="P75" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4382,9 +4850,15 @@
       <c r="N76" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O76" t="inlineStr">
-        <is>
-          <t>5024</t>
+      <c r="O76" t="n">
+        <v>5024</v>
+      </c>
+      <c r="P76" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>5121</t>
         </is>
       </c>
     </row>
@@ -4437,7 +4911,13 @@
       <c r="N77" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O77" t="inlineStr">
+      <c r="O77" t="n">
+        <v>0</v>
+      </c>
+      <c r="P77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4492,9 +4972,15 @@
       <c r="N78" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="O78" t="inlineStr">
-        <is>
-          <t>4869</t>
+      <c r="O78" t="n">
+        <v>4869</v>
+      </c>
+      <c r="P78" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>4951</t>
         </is>
       </c>
     </row>
@@ -4547,9 +5033,15 @@
       <c r="N79" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>3164</t>
+      <c r="O79" t="n">
+        <v>3164</v>
+      </c>
+      <c r="P79" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>3344</t>
         </is>
       </c>
     </row>
@@ -4581,6 +5073,8 @@
       <c r="M80" t="inlineStr"/>
       <c r="N80" s="2" t="inlineStr"/>
       <c r="O80" t="inlineStr"/>
+      <c r="P80" s="2" t="inlineStr"/>
+      <c r="Q80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -4631,9 +5125,15 @@
       <c r="N81" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>4991</t>
+      <c r="O81" t="n">
+        <v>4991</v>
+      </c>
+      <c r="P81" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>5127</t>
         </is>
       </c>
     </row>
@@ -4686,9 +5186,15 @@
       <c r="N82" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>4852</t>
+      <c r="O82" t="n">
+        <v>4852</v>
+      </c>
+      <c r="P82" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>4888</t>
         </is>
       </c>
     </row>
@@ -4741,9 +5247,15 @@
       <c r="N83" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="O83" t="inlineStr">
-        <is>
-          <t>4562</t>
+      <c r="O83" t="n">
+        <v>4562</v>
+      </c>
+      <c r="P83" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>4660</t>
         </is>
       </c>
     </row>
@@ -4796,9 +5308,15 @@
       <c r="N84" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>4394</t>
+      <c r="O84" t="n">
+        <v>4394</v>
+      </c>
+      <c r="P84" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>4514</t>
         </is>
       </c>
     </row>
@@ -4851,9 +5369,15 @@
       <c r="N85" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>4341</t>
+      <c r="O85" t="n">
+        <v>4341</v>
+      </c>
+      <c r="P85" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q85" t="inlineStr">
+        <is>
+          <t>4558</t>
         </is>
       </c>
     </row>
@@ -4906,9 +5430,15 @@
       <c r="N86" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O86" t="inlineStr">
-        <is>
-          <t>3633</t>
+      <c r="O86" t="n">
+        <v>3633</v>
+      </c>
+      <c r="P86" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q86" t="inlineStr">
+        <is>
+          <t>3643</t>
         </is>
       </c>
     </row>
@@ -4961,9 +5491,15 @@
       <c r="N87" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O87" t="inlineStr">
-        <is>
-          <t>4705</t>
+      <c r="O87" t="n">
+        <v>4705</v>
+      </c>
+      <c r="P87" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q87" t="inlineStr">
+        <is>
+          <t>5027</t>
         </is>
       </c>
     </row>
@@ -5016,9 +5552,15 @@
       <c r="N88" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O88" t="inlineStr">
-        <is>
-          <t>3414</t>
+      <c r="O88" t="n">
+        <v>3414</v>
+      </c>
+      <c r="P88" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q88" t="inlineStr">
+        <is>
+          <t>3497</t>
         </is>
       </c>
     </row>
@@ -5071,9 +5613,15 @@
       <c r="N89" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="O89" t="inlineStr">
-        <is>
-          <t>4027</t>
+      <c r="O89" t="n">
+        <v>4027</v>
+      </c>
+      <c r="P89" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q89" t="inlineStr">
+        <is>
+          <t>4046</t>
         </is>
       </c>
     </row>
@@ -5126,9 +5674,15 @@
       <c r="N90" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O90" t="inlineStr">
-        <is>
-          <t>2864</t>
+      <c r="O90" t="n">
+        <v>2864</v>
+      </c>
+      <c r="P90" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>2869</t>
         </is>
       </c>
     </row>
@@ -5181,9 +5735,15 @@
       <c r="N91" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O91" t="inlineStr">
-        <is>
-          <t>3693</t>
+      <c r="O91" t="n">
+        <v>3693</v>
+      </c>
+      <c r="P91" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q91" t="inlineStr">
+        <is>
+          <t>3883</t>
         </is>
       </c>
     </row>
@@ -5236,7 +5796,13 @@
       <c r="N92" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O92" t="inlineStr">
+      <c r="O92" t="n">
+        <v>0</v>
+      </c>
+      <c r="P92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5291,9 +5857,15 @@
       <c r="N93" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O93" t="inlineStr">
-        <is>
-          <t>3799</t>
+      <c r="O93" t="n">
+        <v>3799</v>
+      </c>
+      <c r="P93" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q93" t="inlineStr">
+        <is>
+          <t>3754</t>
         </is>
       </c>
     </row>
@@ -5346,9 +5918,15 @@
       <c r="N94" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O94" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="O94" t="n">
+        <v>2499</v>
+      </c>
+      <c r="P94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q94" t="inlineStr">
+        <is>
+          <t>2530</t>
         </is>
       </c>
     </row>
@@ -5401,9 +5979,15 @@
       <c r="N95" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O95" t="inlineStr">
-        <is>
-          <t>4034</t>
+      <c r="O95" t="n">
+        <v>4034</v>
+      </c>
+      <c r="P95" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q95" t="inlineStr">
+        <is>
+          <t>4102</t>
         </is>
       </c>
     </row>
@@ -5456,9 +6040,15 @@
       <c r="N96" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>2570</t>
+      <c r="O96" t="n">
+        <v>2570</v>
+      </c>
+      <c r="P96" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q96" t="inlineStr">
+        <is>
+          <t>2563</t>
         </is>
       </c>
     </row>
@@ -5511,9 +6101,15 @@
       <c r="N97" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O97" t="inlineStr">
-        <is>
-          <t>2186</t>
+      <c r="O97" t="n">
+        <v>2186</v>
+      </c>
+      <c r="P97" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q97" t="inlineStr">
+        <is>
+          <t>2183</t>
         </is>
       </c>
     </row>
@@ -5566,9 +6162,15 @@
       <c r="N98" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="O98" t="inlineStr">
-        <is>
-          <t>3357</t>
+      <c r="O98" t="n">
+        <v>3357</v>
+      </c>
+      <c r="P98" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q98" t="inlineStr">
+        <is>
+          <t>3356</t>
         </is>
       </c>
     </row>
@@ -5621,9 +6223,15 @@
       <c r="N99" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O99" t="inlineStr">
-        <is>
-          <t>2502</t>
+      <c r="O99" t="n">
+        <v>2502</v>
+      </c>
+      <c r="P99" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q99" t="inlineStr">
+        <is>
+          <t>2495</t>
         </is>
       </c>
     </row>
@@ -5676,9 +6284,15 @@
       <c r="N100" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="O100" t="inlineStr">
-        <is>
-          <t>3920</t>
+      <c r="O100" t="n">
+        <v>3920</v>
+      </c>
+      <c r="P100" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q100" t="inlineStr">
+        <is>
+          <t>4082</t>
         </is>
       </c>
     </row>
@@ -5731,9 +6345,15 @@
       <c r="N101" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O101" t="inlineStr">
-        <is>
-          <t>2333</t>
+      <c r="O101" t="n">
+        <v>2333</v>
+      </c>
+      <c r="P101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q101" t="inlineStr">
+        <is>
+          <t>2362</t>
         </is>
       </c>
     </row>
@@ -5786,9 +6406,15 @@
       <c r="N102" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O102" t="inlineStr">
-        <is>
-          <t>4814</t>
+      <c r="O102" t="n">
+        <v>4814</v>
+      </c>
+      <c r="P102" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q102" t="inlineStr">
+        <is>
+          <t>4974</t>
         </is>
       </c>
     </row>
@@ -5841,9 +6467,15 @@
       <c r="N103" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O103" t="inlineStr">
-        <is>
-          <t>4422</t>
+      <c r="O103" t="n">
+        <v>4422</v>
+      </c>
+      <c r="P103" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q103" t="inlineStr">
+        <is>
+          <t>4529</t>
         </is>
       </c>
     </row>
@@ -5896,9 +6528,15 @@
       <c r="N104" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="O104" t="inlineStr">
-        <is>
-          <t>4278</t>
+      <c r="O104" t="n">
+        <v>4278</v>
+      </c>
+      <c r="P104" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q104" t="inlineStr">
+        <is>
+          <t>4436</t>
         </is>
       </c>
     </row>
@@ -5951,9 +6589,15 @@
       <c r="N105" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="O105" t="inlineStr">
-        <is>
-          <t>4645</t>
+      <c r="O105" t="n">
+        <v>4645</v>
+      </c>
+      <c r="P105" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q105" t="inlineStr">
+        <is>
+          <t>4837</t>
         </is>
       </c>
     </row>
@@ -6006,9 +6650,15 @@
       <c r="N106" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O106" t="inlineStr">
-        <is>
-          <t>4241</t>
+      <c r="O106" t="n">
+        <v>4241</v>
+      </c>
+      <c r="P106" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q106" t="inlineStr">
+        <is>
+          <t>4452</t>
         </is>
       </c>
     </row>
@@ -6061,9 +6711,15 @@
       <c r="N107" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="O107" t="inlineStr">
-        <is>
-          <t>4519</t>
+      <c r="O107" t="n">
+        <v>4519</v>
+      </c>
+      <c r="P107" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q107" t="inlineStr">
+        <is>
+          <t>4828</t>
         </is>
       </c>
     </row>
@@ -6116,7 +6772,13 @@
       <c r="N108" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O108" t="inlineStr">
+      <c r="O108" t="n">
+        <v>0</v>
+      </c>
+      <c r="P108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6171,9 +6833,15 @@
       <c r="N109" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O109" t="inlineStr">
-        <is>
-          <t>2990</t>
+      <c r="O109" t="n">
+        <v>2990</v>
+      </c>
+      <c r="P109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q109" t="inlineStr">
+        <is>
+          <t>2997</t>
         </is>
       </c>
     </row>
@@ -6226,7 +6894,13 @@
       <c r="N110" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O110" t="inlineStr">
+      <c r="O110" t="n">
+        <v>0</v>
+      </c>
+      <c r="P110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q110" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6281,9 +6955,15 @@
       <c r="N111" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="O111" t="inlineStr">
-        <is>
-          <t>4308</t>
+      <c r="O111" t="n">
+        <v>4308</v>
+      </c>
+      <c r="P111" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q111" t="inlineStr">
+        <is>
+          <t>4407</t>
         </is>
       </c>
     </row>
@@ -6336,9 +7016,15 @@
       <c r="N112" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O112" t="inlineStr">
-        <is>
-          <t>4311</t>
+      <c r="O112" t="n">
+        <v>4311</v>
+      </c>
+      <c r="P112" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q112" t="inlineStr">
+        <is>
+          <t>4559</t>
         </is>
       </c>
     </row>
@@ -6391,9 +7077,15 @@
       <c r="N113" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O113" t="inlineStr">
-        <is>
-          <t>3904</t>
+      <c r="O113" t="n">
+        <v>3904</v>
+      </c>
+      <c r="P113" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q113" t="inlineStr">
+        <is>
+          <t>4088</t>
         </is>
       </c>
     </row>
@@ -6446,9 +7138,15 @@
       <c r="N114" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O114" t="inlineStr">
-        <is>
-          <t>2551</t>
+      <c r="O114" t="n">
+        <v>2551</v>
+      </c>
+      <c r="P114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q114" t="inlineStr">
+        <is>
+          <t>2606</t>
         </is>
       </c>
     </row>
@@ -6501,9 +7199,15 @@
       <c r="N115" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="O115" t="inlineStr">
-        <is>
-          <t>4159</t>
+      <c r="O115" t="n">
+        <v>4159</v>
+      </c>
+      <c r="P115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q115" t="inlineStr">
+        <is>
+          <t>4201</t>
         </is>
       </c>
     </row>
@@ -6556,9 +7260,15 @@
       <c r="N116" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O116" t="inlineStr">
-        <is>
-          <t>3109</t>
+      <c r="O116" t="n">
+        <v>3109</v>
+      </c>
+      <c r="P116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q116" t="inlineStr">
+        <is>
+          <t>3164</t>
         </is>
       </c>
     </row>
@@ -6611,9 +7321,15 @@
       <c r="N117" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="O117" t="inlineStr">
-        <is>
-          <t>2451</t>
+      <c r="O117" t="n">
+        <v>2451</v>
+      </c>
+      <c r="P117" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q117" t="inlineStr">
+        <is>
+          <t>2507</t>
         </is>
       </c>
     </row>
@@ -6666,9 +7382,15 @@
       <c r="N118" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="O118" t="inlineStr">
-        <is>
-          <t>3189</t>
+      <c r="O118" t="n">
+        <v>3189</v>
+      </c>
+      <c r="P118" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q118" t="inlineStr">
+        <is>
+          <t>3303</t>
         </is>
       </c>
     </row>
@@ -6691,7 +7413,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F119" s="2" t="n">
@@ -6721,9 +7443,15 @@
       <c r="N119" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O119" t="inlineStr">
-        <is>
-          <t>4413</t>
+      <c r="O119" t="n">
+        <v>4413</v>
+      </c>
+      <c r="P119" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q119" t="inlineStr">
+        <is>
+          <t>4511</t>
         </is>
       </c>
     </row>
@@ -6776,9 +7504,15 @@
       <c r="N120" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O120" t="inlineStr">
-        <is>
-          <t>2742</t>
+      <c r="O120" t="n">
+        <v>2742</v>
+      </c>
+      <c r="P120" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q120" t="inlineStr">
+        <is>
+          <t>2873</t>
         </is>
       </c>
     </row>
@@ -6831,9 +7565,15 @@
       <c r="N121" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O121" t="inlineStr">
-        <is>
-          <t>1601</t>
+      <c r="O121" t="n">
+        <v>1601</v>
+      </c>
+      <c r="P121" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q121" t="inlineStr">
+        <is>
+          <t>1654</t>
         </is>
       </c>
     </row>
@@ -6886,9 +7626,15 @@
       <c r="N122" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O122" t="inlineStr">
-        <is>
-          <t>3224</t>
+      <c r="O122" t="n">
+        <v>3224</v>
+      </c>
+      <c r="P122" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q122" t="inlineStr">
+        <is>
+          <t>3490</t>
         </is>
       </c>
     </row>
@@ -6941,9 +7687,15 @@
       <c r="N123" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="O123" t="inlineStr">
-        <is>
-          <t>4185</t>
+      <c r="O123" t="n">
+        <v>4185</v>
+      </c>
+      <c r="P123" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q123" t="inlineStr">
+        <is>
+          <t>4300</t>
         </is>
       </c>
     </row>
@@ -6996,7 +7748,13 @@
       <c r="N124" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O124" t="inlineStr">
+      <c r="O124" t="n">
+        <v>0</v>
+      </c>
+      <c r="P124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q124" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7051,9 +7809,15 @@
       <c r="N125" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O125" t="inlineStr">
-        <is>
-          <t>3997</t>
+      <c r="O125" t="n">
+        <v>3997</v>
+      </c>
+      <c r="P125" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q125" t="inlineStr">
+        <is>
+          <t>4021</t>
         </is>
       </c>
     </row>
@@ -7106,9 +7870,15 @@
       <c r="N126" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="O126" t="inlineStr">
-        <is>
-          <t>3994</t>
+      <c r="O126" t="n">
+        <v>3994</v>
+      </c>
+      <c r="P126" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q126" t="inlineStr">
+        <is>
+          <t>4023</t>
         </is>
       </c>
     </row>
@@ -7161,9 +7931,15 @@
       <c r="N127" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O127" t="inlineStr">
-        <is>
-          <t>3378</t>
+      <c r="O127" t="n">
+        <v>3378</v>
+      </c>
+      <c r="P127" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q127" t="inlineStr">
+        <is>
+          <t>3400</t>
         </is>
       </c>
     </row>
@@ -7216,9 +7992,15 @@
       <c r="N128" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O128" t="inlineStr">
-        <is>
-          <t>4071</t>
+      <c r="O128" t="n">
+        <v>4071</v>
+      </c>
+      <c r="P128" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q128" t="inlineStr">
+        <is>
+          <t>4149</t>
         </is>
       </c>
     </row>
@@ -7271,9 +8053,15 @@
       <c r="N129" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O129" t="inlineStr">
-        <is>
-          <t>2025</t>
+      <c r="O129" t="n">
+        <v>2025</v>
+      </c>
+      <c r="P129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q129" t="inlineStr">
+        <is>
+          <t>2016</t>
         </is>
       </c>
     </row>
@@ -7326,7 +8114,13 @@
       <c r="N130" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O130" t="inlineStr">
+      <c r="O130" t="n">
+        <v>0</v>
+      </c>
+      <c r="P130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7381,7 +8175,13 @@
       <c r="N131" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O131" t="inlineStr">
+      <c r="O131" t="n">
+        <v>0</v>
+      </c>
+      <c r="P131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7436,9 +8236,15 @@
       <c r="N132" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O132" t="inlineStr">
-        <is>
-          <t>3932</t>
+      <c r="O132" t="n">
+        <v>3932</v>
+      </c>
+      <c r="P132" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q132" t="inlineStr">
+        <is>
+          <t>3992</t>
         </is>
       </c>
     </row>
@@ -7491,7 +8297,13 @@
       <c r="N133" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O133" t="inlineStr">
+      <c r="O133" t="n">
+        <v>0</v>
+      </c>
+      <c r="P133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7546,9 +8358,15 @@
       <c r="N134" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O134" t="inlineStr">
-        <is>
-          <t>3321</t>
+      <c r="O134" t="n">
+        <v>3321</v>
+      </c>
+      <c r="P134" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q134" t="inlineStr">
+        <is>
+          <t>3370</t>
         </is>
       </c>
     </row>
@@ -7601,9 +8419,15 @@
       <c r="N135" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O135" t="inlineStr">
-        <is>
-          <t>3993</t>
+      <c r="O135" t="n">
+        <v>3993</v>
+      </c>
+      <c r="P135" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q135" t="inlineStr">
+        <is>
+          <t>4089</t>
         </is>
       </c>
     </row>
@@ -7656,9 +8480,15 @@
       <c r="N136" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O136" t="inlineStr">
-        <is>
-          <t>4048</t>
+      <c r="O136" t="n">
+        <v>4048</v>
+      </c>
+      <c r="P136" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q136" t="inlineStr">
+        <is>
+          <t>4093</t>
         </is>
       </c>
     </row>
@@ -7711,7 +8541,13 @@
       <c r="N137" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O137" t="inlineStr">
+      <c r="O137" t="n">
+        <v>0</v>
+      </c>
+      <c r="P137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7766,7 +8602,13 @@
       <c r="N138" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O138" t="inlineStr">
+      <c r="O138" t="n">
+        <v>0</v>
+      </c>
+      <c r="P138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q138" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7821,9 +8663,15 @@
       <c r="N139" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O139" t="inlineStr">
-        <is>
-          <t>3108</t>
+      <c r="O139" t="n">
+        <v>3108</v>
+      </c>
+      <c r="P139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q139" t="inlineStr">
+        <is>
+          <t>3117</t>
         </is>
       </c>
     </row>
@@ -7876,7 +8724,13 @@
       <c r="N140" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O140" t="inlineStr">
+      <c r="O140" t="n">
+        <v>0</v>
+      </c>
+      <c r="P140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7931,7 +8785,13 @@
       <c r="N141" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O141" t="inlineStr">
+      <c r="O141" t="n">
+        <v>0</v>
+      </c>
+      <c r="P141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7986,9 +8846,15 @@
       <c r="N142" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O142" t="inlineStr">
-        <is>
-          <t>3124</t>
+      <c r="O142" t="n">
+        <v>3124</v>
+      </c>
+      <c r="P142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q142" t="inlineStr">
+        <is>
+          <t>3116</t>
         </is>
       </c>
     </row>
@@ -8041,7 +8907,13 @@
       <c r="N143" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O143" t="inlineStr">
+      <c r="O143" t="n">
+        <v>0</v>
+      </c>
+      <c r="P143" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8096,9 +8968,15 @@
       <c r="N144" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O144" t="inlineStr">
-        <is>
-          <t>3291</t>
+      <c r="O144" t="n">
+        <v>3291</v>
+      </c>
+      <c r="P144" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q144" t="inlineStr">
+        <is>
+          <t>3551</t>
         </is>
       </c>
     </row>
@@ -8151,7 +9029,13 @@
       <c r="N145" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O145" t="inlineStr">
+      <c r="O145" t="n">
+        <v>0</v>
+      </c>
+      <c r="P145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8206,7 +9090,13 @@
       <c r="N146" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O146" t="inlineStr">
+      <c r="O146" t="n">
+        <v>0</v>
+      </c>
+      <c r="P146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8261,9 +9151,15 @@
       <c r="N147" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O147" t="inlineStr">
-        <is>
-          <t>2070</t>
+      <c r="O147" t="n">
+        <v>2070</v>
+      </c>
+      <c r="P147" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q147" t="inlineStr">
+        <is>
+          <t>2128</t>
         </is>
       </c>
     </row>
@@ -8316,7 +9212,13 @@
       <c r="N148" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O148" t="inlineStr">
+      <c r="O148" t="n">
+        <v>0</v>
+      </c>
+      <c r="P148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8371,7 +9273,13 @@
       <c r="N149" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O149" t="inlineStr">
+      <c r="O149" t="n">
+        <v>0</v>
+      </c>
+      <c r="P149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8426,9 +9334,15 @@
       <c r="N150" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O150" t="inlineStr">
-        <is>
-          <t>2556</t>
+      <c r="O150" t="n">
+        <v>2556</v>
+      </c>
+      <c r="P150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q150" t="inlineStr">
+        <is>
+          <t>2604</t>
         </is>
       </c>
     </row>
@@ -8481,7 +9395,13 @@
       <c r="N151" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O151" t="inlineStr">
+      <c r="O151" t="n">
+        <v>0</v>
+      </c>
+      <c r="P151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8536,7 +9456,13 @@
       <c r="N152" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O152" t="inlineStr">
+      <c r="O152" t="n">
+        <v>0</v>
+      </c>
+      <c r="P152" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8591,7 +9517,13 @@
       <c r="N153" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O153" t="inlineStr">
+      <c r="O153" t="n">
+        <v>0</v>
+      </c>
+      <c r="P153" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8646,9 +9578,15 @@
       <c r="N154" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O154" t="inlineStr">
-        <is>
-          <t>2910</t>
+      <c r="O154" t="n">
+        <v>2910</v>
+      </c>
+      <c r="P154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q154" t="inlineStr">
+        <is>
+          <t>2923</t>
         </is>
       </c>
     </row>
@@ -8701,7 +9639,13 @@
       <c r="N155" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O155" t="inlineStr">
+      <c r="O155" t="n">
+        <v>0</v>
+      </c>
+      <c r="P155" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8756,7 +9700,13 @@
       <c r="N156" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O156" t="inlineStr">
+      <c r="O156" t="n">
+        <v>0</v>
+      </c>
+      <c r="P156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8811,7 +9761,13 @@
       <c r="N157" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O157" t="inlineStr">
+      <c r="O157" t="n">
+        <v>0</v>
+      </c>
+      <c r="P157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8866,9 +9822,15 @@
       <c r="N158" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O158" t="inlineStr">
-        <is>
-          <t>2952</t>
+      <c r="O158" t="n">
+        <v>2952</v>
+      </c>
+      <c r="P158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q158" t="inlineStr">
+        <is>
+          <t>3014</t>
         </is>
       </c>
     </row>
@@ -8910,6 +9872,8 @@
       <c r="M159" t="inlineStr"/>
       <c r="N159" s="2" t="inlineStr"/>
       <c r="O159" t="inlineStr"/>
+      <c r="P159" s="2" t="inlineStr"/>
+      <c r="Q159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="n">
@@ -8954,9 +9918,15 @@
       <c r="N160" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O160" t="inlineStr">
-        <is>
-          <t>4464</t>
+      <c r="O160" t="n">
+        <v>4464</v>
+      </c>
+      <c r="P160" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q160" t="inlineStr">
+        <is>
+          <t>4558</t>
         </is>
       </c>
     </row>
@@ -8990,6 +9960,8 @@
       <c r="M161" t="inlineStr"/>
       <c r="N161" s="2" t="inlineStr"/>
       <c r="O161" t="inlineStr"/>
+      <c r="P161" s="2" t="inlineStr"/>
+      <c r="Q161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="n">
@@ -9034,9 +10006,15 @@
       <c r="N162" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O162" t="inlineStr">
-        <is>
-          <t>3518</t>
+      <c r="O162" t="n">
+        <v>3518</v>
+      </c>
+      <c r="P162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q162" t="inlineStr">
+        <is>
+          <t>3635</t>
         </is>
       </c>
     </row>
@@ -9083,9 +10061,15 @@
       <c r="N163" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="O163" t="inlineStr">
-        <is>
-          <t>2751</t>
+      <c r="O163" t="n">
+        <v>2751</v>
+      </c>
+      <c r="P163" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q163" t="inlineStr">
+        <is>
+          <t>2841</t>
         </is>
       </c>
     </row>
@@ -9128,9 +10112,15 @@
       <c r="N164" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="O164" t="inlineStr">
-        <is>
-          <t>3029</t>
+      <c r="O164" t="n">
+        <v>3029</v>
+      </c>
+      <c r="P164" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q164" t="inlineStr">
+        <is>
+          <t>3229</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-22 11:30:52
</commit_message>
<xml_diff>
--- a/Season_Attack/86.xlsx
+++ b/Season_Attack/86.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q164"/>
+  <dimension ref="A1:S166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,16 @@
           <t>03-20_0</t>
         </is>
       </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>03-21_A</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>03-21_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -532,9 +542,15 @@
       <c r="P2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>3067</t>
+      <c r="Q2" t="n">
+        <v>3067</v>
+      </c>
+      <c r="R2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>3120</t>
         </is>
       </c>
     </row>
@@ -581,9 +597,15 @@
       <c r="P3" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>5812</t>
+      <c r="Q3" t="n">
+        <v>5812</v>
+      </c>
+      <c r="R3" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>6131</t>
         </is>
       </c>
     </row>
@@ -642,9 +664,15 @@
       <c r="P4" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>5752</t>
+      <c r="Q4" t="n">
+        <v>5752</v>
+      </c>
+      <c r="R4" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>6079</t>
         </is>
       </c>
     </row>
@@ -703,9 +731,15 @@
       <c r="P5" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>5808</t>
+      <c r="Q5" t="n">
+        <v>5808</v>
+      </c>
+      <c r="R5" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>6189</t>
         </is>
       </c>
     </row>
@@ -764,9 +798,15 @@
       <c r="P6" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>5489</t>
+      <c r="Q6" t="n">
+        <v>5489</v>
+      </c>
+      <c r="R6" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>5714</t>
         </is>
       </c>
     </row>
@@ -825,9 +865,15 @@
       <c r="P7" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>6070</t>
+      <c r="Q7" t="n">
+        <v>6070</v>
+      </c>
+      <c r="R7" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>6351</t>
         </is>
       </c>
     </row>
@@ -886,9 +932,15 @@
       <c r="P8" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>5138</t>
+      <c r="Q8" t="n">
+        <v>5138</v>
+      </c>
+      <c r="R8" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>5368</t>
         </is>
       </c>
     </row>
@@ -947,9 +999,15 @@
       <c r="P9" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>5543</t>
+      <c r="Q9" t="n">
+        <v>5543</v>
+      </c>
+      <c r="R9" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>5703</t>
         </is>
       </c>
     </row>
@@ -1008,9 +1066,15 @@
       <c r="P10" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>5679</t>
+      <c r="Q10" t="n">
+        <v>5679</v>
+      </c>
+      <c r="R10" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>6186</t>
         </is>
       </c>
     </row>
@@ -1056,6 +1120,14 @@
       <c r="O11" t="inlineStr"/>
       <c r="P11" s="2" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
+      <c r="R11" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>5736</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1112,7 +1184,13 @@
       <c r="P12" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Q12" t="inlineStr">
+      <c r="Q12" t="n">
+        <v>3336</v>
+      </c>
+      <c r="R12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="inlineStr">
         <is>
           <t>3336</t>
         </is>
@@ -1173,9 +1251,15 @@
       <c r="P13" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>6269</t>
+      <c r="Q13" t="n">
+        <v>6269</v>
+      </c>
+      <c r="R13" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>6448</t>
         </is>
       </c>
     </row>
@@ -1234,9 +1318,15 @@
       <c r="P14" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>5366</t>
+      <c r="Q14" t="n">
+        <v>5366</v>
+      </c>
+      <c r="R14" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>5622</t>
         </is>
       </c>
     </row>
@@ -1279,9 +1369,15 @@
       <c r="P15" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>5662</t>
+      <c r="Q15" t="n">
+        <v>5662</v>
+      </c>
+      <c r="R15" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>5912</t>
         </is>
       </c>
     </row>
@@ -1340,9 +1436,15 @@
       <c r="P16" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>4708</t>
+      <c r="Q16" t="n">
+        <v>4708</v>
+      </c>
+      <c r="R16" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>4942</t>
         </is>
       </c>
     </row>
@@ -1401,9 +1503,15 @@
       <c r="P17" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>4827</t>
+      <c r="Q17" t="n">
+        <v>4827</v>
+      </c>
+      <c r="R17" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>5126</t>
         </is>
       </c>
     </row>
@@ -1462,9 +1570,15 @@
       <c r="P18" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>5459</t>
+      <c r="Q18" t="n">
+        <v>5459</v>
+      </c>
+      <c r="R18" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>5784</t>
         </is>
       </c>
     </row>
@@ -1507,9 +1621,15 @@
       <c r="P19" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>6297</t>
+      <c r="Q19" t="n">
+        <v>6297</v>
+      </c>
+      <c r="R19" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>6605</t>
         </is>
       </c>
     </row>
@@ -1568,9 +1688,15 @@
       <c r="P20" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>4426</t>
+      <c r="Q20" t="n">
+        <v>4426</v>
+      </c>
+      <c r="R20" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>4932</t>
         </is>
       </c>
     </row>
@@ -1629,9 +1755,15 @@
       <c r="P21" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>5651</t>
+      <c r="Q21" t="n">
+        <v>5651</v>
+      </c>
+      <c r="R21" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>5989</t>
         </is>
       </c>
     </row>
@@ -1690,9 +1822,15 @@
       <c r="P22" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>4803</t>
+      <c r="Q22" t="n">
+        <v>4803</v>
+      </c>
+      <c r="R22" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>5338</t>
         </is>
       </c>
     </row>
@@ -1751,9 +1889,15 @@
       <c r="P23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>5590</t>
+      <c r="Q23" t="n">
+        <v>5590</v>
+      </c>
+      <c r="R23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>5821</t>
         </is>
       </c>
     </row>
@@ -1812,7 +1956,13 @@
       <c r="P24" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q24" t="inlineStr">
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1873,9 +2023,15 @@
       <c r="P25" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>2609</t>
+      <c r="Q25" t="n">
+        <v>2609</v>
+      </c>
+      <c r="R25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>2641</t>
         </is>
       </c>
     </row>
@@ -1914,9 +2070,15 @@
       <c r="P26" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>5755</t>
+      <c r="Q26" t="n">
+        <v>5755</v>
+      </c>
+      <c r="R26" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>6054</t>
         </is>
       </c>
     </row>
@@ -1955,9 +2117,15 @@
       <c r="P27" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>4641</t>
+      <c r="Q27" t="n">
+        <v>4641</v>
+      </c>
+      <c r="R27" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>5200</t>
         </is>
       </c>
     </row>
@@ -2016,9 +2184,15 @@
       <c r="P28" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>5956</t>
+      <c r="Q28" t="n">
+        <v>5956</v>
+      </c>
+      <c r="R28" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>6274</t>
         </is>
       </c>
     </row>
@@ -2028,7 +2202,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>kusipao</t>
+          <t>何苦僧ai</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2057,9 +2231,15 @@
       <c r="P29" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>5112</t>
+      <c r="Q29" t="n">
+        <v>5112</v>
+      </c>
+      <c r="R29" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>5511</t>
         </is>
       </c>
     </row>
@@ -2118,9 +2298,15 @@
       <c r="P30" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>4802</t>
+      <c r="Q30" t="n">
+        <v>4802</v>
+      </c>
+      <c r="R30" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>5058</t>
         </is>
       </c>
     </row>
@@ -2179,9 +2365,15 @@
       <c r="P31" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>6184</t>
+      <c r="Q31" t="n">
+        <v>6184</v>
+      </c>
+      <c r="R31" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>6482</t>
         </is>
       </c>
     </row>
@@ -2227,6 +2419,14 @@
       <c r="O32" t="inlineStr"/>
       <c r="P32" s="2" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
+      <c r="R32" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>4344</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2283,9 +2483,15 @@
       <c r="P33" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="Q33" t="inlineStr">
-        <is>
-          <t>5389</t>
+      <c r="Q33" t="n">
+        <v>5389</v>
+      </c>
+      <c r="R33" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>5775</t>
         </is>
       </c>
     </row>
@@ -2344,9 +2550,15 @@
       <c r="P34" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="Q34" t="inlineStr">
-        <is>
-          <t>5975</t>
+      <c r="Q34" t="n">
+        <v>5975</v>
+      </c>
+      <c r="R34" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>6255</t>
         </is>
       </c>
     </row>
@@ -2405,9 +2617,15 @@
       <c r="P35" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>5392</t>
+      <c r="Q35" t="n">
+        <v>5392</v>
+      </c>
+      <c r="R35" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>5650</t>
         </is>
       </c>
     </row>
@@ -2446,9 +2664,15 @@
       <c r="P36" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="Q36" t="inlineStr">
-        <is>
-          <t>4867</t>
+      <c r="Q36" t="n">
+        <v>4867</v>
+      </c>
+      <c r="R36" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>4955</t>
         </is>
       </c>
     </row>
@@ -2507,9 +2731,15 @@
       <c r="P37" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>5584</t>
+      <c r="Q37" t="n">
+        <v>5584</v>
+      </c>
+      <c r="R37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>5808</t>
         </is>
       </c>
     </row>
@@ -2568,9 +2798,15 @@
       <c r="P38" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>5334</t>
+      <c r="Q38" t="n">
+        <v>5334</v>
+      </c>
+      <c r="R38" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>5524</t>
         </is>
       </c>
     </row>
@@ -2629,9 +2865,15 @@
       <c r="P39" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>5781</t>
+      <c r="Q39" t="n">
+        <v>5781</v>
+      </c>
+      <c r="R39" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>6135</t>
         </is>
       </c>
     </row>
@@ -2690,9 +2932,15 @@
       <c r="P40" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="Q40" t="inlineStr">
-        <is>
-          <t>6233</t>
+      <c r="Q40" t="n">
+        <v>6233</v>
+      </c>
+      <c r="R40" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>6540</t>
         </is>
       </c>
     </row>
@@ -2751,9 +2999,15 @@
       <c r="P41" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q41" t="inlineStr">
-        <is>
-          <t>5622</t>
+      <c r="Q41" t="n">
+        <v>5622</v>
+      </c>
+      <c r="R41" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>5877</t>
         </is>
       </c>
     </row>
@@ -2812,9 +3066,15 @@
       <c r="P42" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>5273</t>
+      <c r="Q42" t="n">
+        <v>5273</v>
+      </c>
+      <c r="R42" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>5818</t>
         </is>
       </c>
     </row>
@@ -2873,9 +3133,15 @@
       <c r="P43" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="Q43" t="inlineStr">
-        <is>
-          <t>5054</t>
+      <c r="Q43" t="n">
+        <v>5054</v>
+      </c>
+      <c r="R43" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>5289</t>
         </is>
       </c>
     </row>
@@ -2934,9 +3200,15 @@
       <c r="P44" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q44" t="inlineStr">
-        <is>
-          <t>5281</t>
+      <c r="Q44" t="n">
+        <v>5281</v>
+      </c>
+      <c r="R44" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>5511</t>
         </is>
       </c>
     </row>
@@ -2995,9 +3267,15 @@
       <c r="P45" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q45" t="inlineStr">
-        <is>
-          <t>4752</t>
+      <c r="Q45" t="n">
+        <v>4752</v>
+      </c>
+      <c r="R45" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>4992</t>
         </is>
       </c>
     </row>
@@ -3056,9 +3334,15 @@
       <c r="P46" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="Q46" t="inlineStr">
-        <is>
-          <t>5899</t>
+      <c r="Q46" t="n">
+        <v>5899</v>
+      </c>
+      <c r="R46" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>6156</t>
         </is>
       </c>
     </row>
@@ -3117,9 +3401,15 @@
       <c r="P47" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="Q47" t="inlineStr">
-        <is>
-          <t>4856</t>
+      <c r="Q47" t="n">
+        <v>4856</v>
+      </c>
+      <c r="R47" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>5096</t>
         </is>
       </c>
     </row>
@@ -3178,9 +3468,15 @@
       <c r="P48" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q48" t="inlineStr">
-        <is>
-          <t>2516</t>
+      <c r="Q48" t="n">
+        <v>2516</v>
+      </c>
+      <c r="R48" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S48" t="inlineStr">
+        <is>
+          <t>2548</t>
         </is>
       </c>
     </row>
@@ -3214,6 +3510,8 @@
       <c r="O49" t="inlineStr"/>
       <c r="P49" s="2" t="inlineStr"/>
       <c r="Q49" t="inlineStr"/>
+      <c r="R49" s="2" t="inlineStr"/>
+      <c r="S49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -3270,7 +3568,13 @@
       <c r="P50" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q50" t="inlineStr">
+      <c r="Q50" t="n">
+        <v>0</v>
+      </c>
+      <c r="R50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S50" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3331,9 +3635,15 @@
       <c r="P51" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q51" t="inlineStr">
-        <is>
-          <t>2726</t>
+      <c r="Q51" t="n">
+        <v>2726</v>
+      </c>
+      <c r="R51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>2819</t>
         </is>
       </c>
     </row>
@@ -3392,9 +3702,15 @@
       <c r="P52" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q52" t="inlineStr">
-        <is>
-          <t>3168</t>
+      <c r="Q52" t="n">
+        <v>3168</v>
+      </c>
+      <c r="R52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>3184</t>
         </is>
       </c>
     </row>
@@ -3453,9 +3769,15 @@
       <c r="P53" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="Q53" t="inlineStr">
-        <is>
-          <t>5476</t>
+      <c r="Q53" t="n">
+        <v>5476</v>
+      </c>
+      <c r="R53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>5457</t>
         </is>
       </c>
     </row>
@@ -3514,9 +3836,15 @@
       <c r="P54" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Q54" t="inlineStr">
-        <is>
-          <t>4670</t>
+      <c r="Q54" t="n">
+        <v>4670</v>
+      </c>
+      <c r="R54" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>4753</t>
         </is>
       </c>
     </row>
@@ -3575,9 +3903,15 @@
       <c r="P55" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="Q55" t="inlineStr">
-        <is>
-          <t>4782</t>
+      <c r="Q55" t="n">
+        <v>4782</v>
+      </c>
+      <c r="R55" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>4941</t>
         </is>
       </c>
     </row>
@@ -3636,9 +3970,15 @@
       <c r="P56" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="Q56" t="inlineStr">
-        <is>
-          <t>5243</t>
+      <c r="Q56" t="n">
+        <v>5243</v>
+      </c>
+      <c r="R56" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>5455</t>
         </is>
       </c>
     </row>
@@ -3697,9 +4037,15 @@
       <c r="P57" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q57" t="inlineStr">
-        <is>
-          <t>4773</t>
+      <c r="Q57" t="n">
+        <v>4773</v>
+      </c>
+      <c r="R57" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>4922</t>
         </is>
       </c>
     </row>
@@ -3758,9 +4104,15 @@
       <c r="P58" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="Q58" t="inlineStr">
-        <is>
-          <t>4573</t>
+      <c r="Q58" t="n">
+        <v>4573</v>
+      </c>
+      <c r="R58" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="S58" t="inlineStr">
+        <is>
+          <t>4624</t>
         </is>
       </c>
     </row>
@@ -3819,7 +4171,13 @@
       <c r="P59" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q59" t="inlineStr">
+      <c r="Q59" t="n">
+        <v>0</v>
+      </c>
+      <c r="R59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S59" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3880,9 +4238,15 @@
       <c r="P60" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="Q60" t="inlineStr">
-        <is>
-          <t>5452</t>
+      <c r="Q60" t="n">
+        <v>5452</v>
+      </c>
+      <c r="R60" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="S60" t="inlineStr">
+        <is>
+          <t>5658</t>
         </is>
       </c>
     </row>
@@ -3941,7 +4305,13 @@
       <c r="P61" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q61" t="inlineStr">
+      <c r="Q61" t="n">
+        <v>2758</v>
+      </c>
+      <c r="R61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S61" t="inlineStr">
         <is>
           <t>2758</t>
         </is>
@@ -4002,9 +4372,15 @@
       <c r="P62" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q62" t="inlineStr">
-        <is>
-          <t>3246</t>
+      <c r="Q62" t="n">
+        <v>3246</v>
+      </c>
+      <c r="R62" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>3241</t>
         </is>
       </c>
     </row>
@@ -4063,9 +4439,15 @@
       <c r="P63" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="Q63" t="inlineStr">
-        <is>
-          <t>5115</t>
+      <c r="Q63" t="n">
+        <v>5115</v>
+      </c>
+      <c r="R63" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>5272</t>
         </is>
       </c>
     </row>
@@ -4124,9 +4506,15 @@
       <c r="P64" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="Q64" t="inlineStr">
-        <is>
-          <t>5700</t>
+      <c r="Q64" t="n">
+        <v>5700</v>
+      </c>
+      <c r="R64" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="S64" t="inlineStr">
+        <is>
+          <t>6017</t>
         </is>
       </c>
     </row>
@@ -4185,9 +4573,15 @@
       <c r="P65" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q65" t="inlineStr">
-        <is>
-          <t>2952</t>
+      <c r="Q65" t="n">
+        <v>2952</v>
+      </c>
+      <c r="R65" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S65" t="inlineStr">
+        <is>
+          <t>3298</t>
         </is>
       </c>
     </row>
@@ -4246,9 +4640,15 @@
       <c r="P66" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="Q66" t="inlineStr">
-        <is>
-          <t>4808</t>
+      <c r="Q66" t="n">
+        <v>4808</v>
+      </c>
+      <c r="R66" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="S66" t="inlineStr">
+        <is>
+          <t>4903</t>
         </is>
       </c>
     </row>
@@ -4307,9 +4707,15 @@
       <c r="P67" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q67" t="inlineStr">
-        <is>
-          <t>3389</t>
+      <c r="Q67" t="n">
+        <v>3389</v>
+      </c>
+      <c r="R67" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>3405</t>
         </is>
       </c>
     </row>
@@ -4368,7 +4774,13 @@
       <c r="P68" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q68" t="inlineStr">
+      <c r="Q68" t="n">
+        <v>0</v>
+      </c>
+      <c r="R68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4429,9 +4841,15 @@
       <c r="P69" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q69" t="inlineStr">
-        <is>
-          <t>4130</t>
+      <c r="Q69" t="n">
+        <v>4130</v>
+      </c>
+      <c r="R69" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="S69" t="inlineStr">
+        <is>
+          <t>4327</t>
         </is>
       </c>
     </row>
@@ -4490,9 +4908,15 @@
       <c r="P70" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q70" t="inlineStr">
-        <is>
-          <t>4709</t>
+      <c r="Q70" t="n">
+        <v>4709</v>
+      </c>
+      <c r="R70" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S70" t="inlineStr">
+        <is>
+          <t>4813</t>
         </is>
       </c>
     </row>
@@ -4551,9 +4975,15 @@
       <c r="P71" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q71" t="inlineStr">
-        <is>
-          <t>3198</t>
+      <c r="Q71" t="n">
+        <v>3198</v>
+      </c>
+      <c r="R71" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S71" t="inlineStr">
+        <is>
+          <t>3225</t>
         </is>
       </c>
     </row>
@@ -4612,9 +5042,15 @@
       <c r="P72" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="Q72" t="inlineStr">
-        <is>
-          <t>4513</t>
+      <c r="Q72" t="n">
+        <v>4513</v>
+      </c>
+      <c r="R72" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="S72" t="inlineStr">
+        <is>
+          <t>4668</t>
         </is>
       </c>
     </row>
@@ -4673,9 +5109,15 @@
       <c r="P73" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q73" t="inlineStr">
-        <is>
-          <t>5174</t>
+      <c r="Q73" t="n">
+        <v>5174</v>
+      </c>
+      <c r="R73" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S73" t="inlineStr">
+        <is>
+          <t>5369</t>
         </is>
       </c>
     </row>
@@ -4734,7 +5176,13 @@
       <c r="P74" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q74" t="inlineStr">
+      <c r="Q74" t="n">
+        <v>0</v>
+      </c>
+      <c r="R74" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4795,7 +5243,13 @@
       <c r="P75" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q75" t="inlineStr">
+      <c r="Q75" t="n">
+        <v>0</v>
+      </c>
+      <c r="R75" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4856,9 +5310,15 @@
       <c r="P76" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="Q76" t="inlineStr">
-        <is>
-          <t>5121</t>
+      <c r="Q76" t="n">
+        <v>5121</v>
+      </c>
+      <c r="R76" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="S76" t="inlineStr">
+        <is>
+          <t>5342</t>
         </is>
       </c>
     </row>
@@ -4917,7 +5377,13 @@
       <c r="P77" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q77" t="inlineStr">
+      <c r="Q77" t="n">
+        <v>0</v>
+      </c>
+      <c r="R77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4978,9 +5444,15 @@
       <c r="P78" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="Q78" t="inlineStr">
-        <is>
-          <t>4951</t>
+      <c r="Q78" t="n">
+        <v>4951</v>
+      </c>
+      <c r="R78" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="S78" t="inlineStr">
+        <is>
+          <t>5178</t>
         </is>
       </c>
     </row>
@@ -5039,9 +5511,15 @@
       <c r="P79" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="Q79" t="inlineStr">
-        <is>
-          <t>3344</t>
+      <c r="Q79" t="n">
+        <v>3344</v>
+      </c>
+      <c r="R79" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S79" t="inlineStr">
+        <is>
+          <t>3331</t>
         </is>
       </c>
     </row>
@@ -5075,6 +5553,8 @@
       <c r="O80" t="inlineStr"/>
       <c r="P80" s="2" t="inlineStr"/>
       <c r="Q80" t="inlineStr"/>
+      <c r="R80" s="2" t="inlineStr"/>
+      <c r="S80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -5131,9 +5611,15 @@
       <c r="P81" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="Q81" t="inlineStr">
-        <is>
-          <t>5127</t>
+      <c r="Q81" t="n">
+        <v>5127</v>
+      </c>
+      <c r="R81" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S81" t="inlineStr">
+        <is>
+          <t>5270</t>
         </is>
       </c>
     </row>
@@ -5192,9 +5678,15 @@
       <c r="P82" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="Q82" t="inlineStr">
-        <is>
-          <t>4888</t>
+      <c r="Q82" t="n">
+        <v>4888</v>
+      </c>
+      <c r="R82" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S82" t="inlineStr">
+        <is>
+          <t>4982</t>
         </is>
       </c>
     </row>
@@ -5253,9 +5745,15 @@
       <c r="P83" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="Q83" t="inlineStr">
-        <is>
-          <t>4660</t>
+      <c r="Q83" t="n">
+        <v>4660</v>
+      </c>
+      <c r="R83" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="S83" t="inlineStr">
+        <is>
+          <t>4832</t>
         </is>
       </c>
     </row>
@@ -5314,9 +5812,15 @@
       <c r="P84" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q84" t="inlineStr">
-        <is>
-          <t>4514</t>
+      <c r="Q84" t="n">
+        <v>4514</v>
+      </c>
+      <c r="R84" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S84" t="inlineStr">
+        <is>
+          <t>4672</t>
         </is>
       </c>
     </row>
@@ -5375,9 +5879,15 @@
       <c r="P85" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q85" t="inlineStr">
-        <is>
-          <t>4558</t>
+      <c r="Q85" t="n">
+        <v>4558</v>
+      </c>
+      <c r="R85" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="S85" t="inlineStr">
+        <is>
+          <t>4663</t>
         </is>
       </c>
     </row>
@@ -5436,9 +5946,15 @@
       <c r="P86" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q86" t="inlineStr">
-        <is>
-          <t>3643</t>
+      <c r="Q86" t="n">
+        <v>3643</v>
+      </c>
+      <c r="R86" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S86" t="inlineStr">
+        <is>
+          <t>4064</t>
         </is>
       </c>
     </row>
@@ -5497,9 +6013,15 @@
       <c r="P87" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q87" t="inlineStr">
-        <is>
-          <t>5027</t>
+      <c r="Q87" t="n">
+        <v>5027</v>
+      </c>
+      <c r="R87" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="S87" t="inlineStr">
+        <is>
+          <t>4907</t>
         </is>
       </c>
     </row>
@@ -5558,9 +6080,15 @@
       <c r="P88" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q88" t="inlineStr">
-        <is>
-          <t>3497</t>
+      <c r="Q88" t="n">
+        <v>3497</v>
+      </c>
+      <c r="R88" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S88" t="inlineStr">
+        <is>
+          <t>3659</t>
         </is>
       </c>
     </row>
@@ -5619,9 +6147,15 @@
       <c r="P89" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="Q89" t="inlineStr">
-        <is>
-          <t>4046</t>
+      <c r="Q89" t="n">
+        <v>4046</v>
+      </c>
+      <c r="R89" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S89" t="inlineStr">
+        <is>
+          <t>4156</t>
         </is>
       </c>
     </row>
@@ -5680,9 +6214,15 @@
       <c r="P90" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q90" t="inlineStr">
-        <is>
-          <t>2869</t>
+      <c r="Q90" t="n">
+        <v>2869</v>
+      </c>
+      <c r="R90" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S90" t="inlineStr">
+        <is>
+          <t>2862</t>
         </is>
       </c>
     </row>
@@ -5741,9 +6281,15 @@
       <c r="P91" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="Q91" t="inlineStr">
-        <is>
-          <t>3883</t>
+      <c r="Q91" t="n">
+        <v>3883</v>
+      </c>
+      <c r="R91" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="S91" t="inlineStr">
+        <is>
+          <t>3988</t>
         </is>
       </c>
     </row>
@@ -5802,7 +6348,13 @@
       <c r="P92" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q92" t="inlineStr">
+      <c r="Q92" t="n">
+        <v>0</v>
+      </c>
+      <c r="R92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5863,9 +6415,15 @@
       <c r="P93" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q93" t="inlineStr">
-        <is>
-          <t>3754</t>
+      <c r="Q93" t="n">
+        <v>3754</v>
+      </c>
+      <c r="R93" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="S93" t="inlineStr">
+        <is>
+          <t>3998</t>
         </is>
       </c>
     </row>
@@ -5924,9 +6482,15 @@
       <c r="P94" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q94" t="inlineStr">
-        <is>
-          <t>2530</t>
+      <c r="Q94" t="n">
+        <v>2530</v>
+      </c>
+      <c r="R94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S94" t="inlineStr">
+        <is>
+          <t>2579</t>
         </is>
       </c>
     </row>
@@ -5936,7 +6500,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>"慶頴 謝"</t>
+          <t>Dj6106</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -5985,9 +6549,15 @@
       <c r="P95" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="Q95" t="inlineStr">
-        <is>
-          <t>4102</t>
+      <c r="Q95" t="n">
+        <v>4102</v>
+      </c>
+      <c r="R95" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="S95" t="inlineStr">
+        <is>
+          <t>4252</t>
         </is>
       </c>
     </row>
@@ -6046,9 +6616,15 @@
       <c r="P96" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q96" t="inlineStr">
-        <is>
-          <t>2563</t>
+      <c r="Q96" t="n">
+        <v>2563</v>
+      </c>
+      <c r="R96" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="S96" t="inlineStr">
+        <is>
+          <t>2624</t>
         </is>
       </c>
     </row>
@@ -6107,9 +6683,15 @@
       <c r="P97" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q97" t="inlineStr">
-        <is>
-          <t>2183</t>
+      <c r="Q97" t="n">
+        <v>2183</v>
+      </c>
+      <c r="R97" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S97" t="inlineStr">
+        <is>
+          <t>2193</t>
         </is>
       </c>
     </row>
@@ -6168,7 +6750,13 @@
       <c r="P98" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q98" t="inlineStr">
+      <c r="Q98" t="n">
+        <v>3356</v>
+      </c>
+      <c r="R98" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S98" t="inlineStr">
         <is>
           <t>3356</t>
         </is>
@@ -6229,9 +6817,15 @@
       <c r="P99" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q99" t="inlineStr">
-        <is>
-          <t>2495</t>
+      <c r="Q99" t="n">
+        <v>2495</v>
+      </c>
+      <c r="R99" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S99" t="inlineStr">
+        <is>
+          <t>2492</t>
         </is>
       </c>
     </row>
@@ -6290,9 +6884,15 @@
       <c r="P100" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="Q100" t="inlineStr">
-        <is>
-          <t>4082</t>
+      <c r="Q100" t="n">
+        <v>4082</v>
+      </c>
+      <c r="R100" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="S100" t="inlineStr">
+        <is>
+          <t>4139</t>
         </is>
       </c>
     </row>
@@ -6351,9 +6951,15 @@
       <c r="P101" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q101" t="inlineStr">
-        <is>
-          <t>2362</t>
+      <c r="Q101" t="n">
+        <v>2362</v>
+      </c>
+      <c r="R101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S101" t="inlineStr">
+        <is>
+          <t>2357</t>
         </is>
       </c>
     </row>
@@ -6412,9 +7018,15 @@
       <c r="P102" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="Q102" t="inlineStr">
-        <is>
-          <t>4974</t>
+      <c r="Q102" t="n">
+        <v>4974</v>
+      </c>
+      <c r="R102" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="S102" t="inlineStr">
+        <is>
+          <t>5132</t>
         </is>
       </c>
     </row>
@@ -6473,9 +7085,15 @@
       <c r="P103" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q103" t="inlineStr">
-        <is>
-          <t>4529</t>
+      <c r="Q103" t="n">
+        <v>4529</v>
+      </c>
+      <c r="R103" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S103" t="inlineStr">
+        <is>
+          <t>4601</t>
         </is>
       </c>
     </row>
@@ -6534,9 +7152,15 @@
       <c r="P104" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q104" t="inlineStr">
-        <is>
-          <t>4436</t>
+      <c r="Q104" t="n">
+        <v>4436</v>
+      </c>
+      <c r="R104" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S104" t="inlineStr">
+        <is>
+          <t>4621</t>
         </is>
       </c>
     </row>
@@ -6595,9 +7219,15 @@
       <c r="P105" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="Q105" t="inlineStr">
-        <is>
-          <t>4837</t>
+      <c r="Q105" t="n">
+        <v>4837</v>
+      </c>
+      <c r="R105" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="S105" t="inlineStr">
+        <is>
+          <t>4976</t>
         </is>
       </c>
     </row>
@@ -6656,9 +7286,15 @@
       <c r="P106" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="Q106" t="inlineStr">
-        <is>
-          <t>4452</t>
+      <c r="Q106" t="n">
+        <v>4452</v>
+      </c>
+      <c r="R106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S106" t="inlineStr">
+        <is>
+          <t>4604</t>
         </is>
       </c>
     </row>
@@ -6717,9 +7353,15 @@
       <c r="P107" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="Q107" t="inlineStr">
-        <is>
-          <t>4828</t>
+      <c r="Q107" t="n">
+        <v>4828</v>
+      </c>
+      <c r="R107" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="S107" t="inlineStr">
+        <is>
+          <t>5074</t>
         </is>
       </c>
     </row>
@@ -6778,7 +7420,13 @@
       <c r="P108" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q108" t="inlineStr">
+      <c r="Q108" t="n">
+        <v>0</v>
+      </c>
+      <c r="R108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6839,9 +7487,15 @@
       <c r="P109" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q109" t="inlineStr">
-        <is>
-          <t>2997</t>
+      <c r="Q109" t="n">
+        <v>2997</v>
+      </c>
+      <c r="R109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S109" t="inlineStr">
+        <is>
+          <t>3044</t>
         </is>
       </c>
     </row>
@@ -6900,7 +7554,13 @@
       <c r="P110" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q110" t="inlineStr">
+      <c r="Q110" t="n">
+        <v>0</v>
+      </c>
+      <c r="R110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S110" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6961,9 +7621,15 @@
       <c r="P111" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="Q111" t="inlineStr">
-        <is>
-          <t>4407</t>
+      <c r="Q111" t="n">
+        <v>4407</v>
+      </c>
+      <c r="R111" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="S111" t="inlineStr">
+        <is>
+          <t>4505</t>
         </is>
       </c>
     </row>
@@ -7022,9 +7688,15 @@
       <c r="P112" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="Q112" t="inlineStr">
-        <is>
-          <t>4559</t>
+      <c r="Q112" t="n">
+        <v>4559</v>
+      </c>
+      <c r="R112" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="S112" t="inlineStr">
+        <is>
+          <t>4623</t>
         </is>
       </c>
     </row>
@@ -7083,9 +7755,15 @@
       <c r="P113" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="Q113" t="inlineStr">
-        <is>
-          <t>4088</t>
+      <c r="Q113" t="n">
+        <v>4088</v>
+      </c>
+      <c r="R113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S113" t="inlineStr">
+        <is>
+          <t>4042</t>
         </is>
       </c>
     </row>
@@ -7144,9 +7822,15 @@
       <c r="P114" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q114" t="inlineStr">
-        <is>
-          <t>2606</t>
+      <c r="Q114" t="n">
+        <v>2606</v>
+      </c>
+      <c r="R114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S114" t="inlineStr">
+        <is>
+          <t>2631</t>
         </is>
       </c>
     </row>
@@ -7205,9 +7889,15 @@
       <c r="P115" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q115" t="inlineStr">
-        <is>
-          <t>4201</t>
+      <c r="Q115" t="n">
+        <v>4201</v>
+      </c>
+      <c r="R115" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="S115" t="inlineStr">
+        <is>
+          <t>4310</t>
         </is>
       </c>
     </row>
@@ -7266,9 +7956,15 @@
       <c r="P116" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q116" t="inlineStr">
-        <is>
-          <t>3164</t>
+      <c r="Q116" t="n">
+        <v>3164</v>
+      </c>
+      <c r="R116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S116" t="inlineStr">
+        <is>
+          <t>3285</t>
         </is>
       </c>
     </row>
@@ -7327,9 +8023,15 @@
       <c r="P117" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="Q117" t="inlineStr">
-        <is>
-          <t>2507</t>
+      <c r="Q117" t="n">
+        <v>2507</v>
+      </c>
+      <c r="R117" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="S117" t="inlineStr">
+        <is>
+          <t>2632</t>
         </is>
       </c>
     </row>
@@ -7388,9 +8090,15 @@
       <c r="P118" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="Q118" t="inlineStr">
-        <is>
-          <t>3303</t>
+      <c r="Q118" t="n">
+        <v>3303</v>
+      </c>
+      <c r="R118" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="S118" t="inlineStr">
+        <is>
+          <t>3434</t>
         </is>
       </c>
     </row>
@@ -7449,9 +8157,15 @@
       <c r="P119" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="Q119" t="inlineStr">
-        <is>
-          <t>4511</t>
+      <c r="Q119" t="n">
+        <v>4511</v>
+      </c>
+      <c r="R119" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="S119" t="inlineStr">
+        <is>
+          <t>4582</t>
         </is>
       </c>
     </row>
@@ -7510,9 +8224,15 @@
       <c r="P120" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q120" t="inlineStr">
-        <is>
-          <t>2873</t>
+      <c r="Q120" t="n">
+        <v>2873</v>
+      </c>
+      <c r="R120" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S120" t="inlineStr">
+        <is>
+          <t>2949</t>
         </is>
       </c>
     </row>
@@ -7571,9 +8291,15 @@
       <c r="P121" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="Q121" t="inlineStr">
-        <is>
-          <t>1654</t>
+      <c r="Q121" t="n">
+        <v>1654</v>
+      </c>
+      <c r="R121" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="S121" t="inlineStr">
+        <is>
+          <t>1686</t>
         </is>
       </c>
     </row>
@@ -7632,9 +8358,15 @@
       <c r="P122" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q122" t="inlineStr">
-        <is>
-          <t>3490</t>
+      <c r="Q122" t="n">
+        <v>3490</v>
+      </c>
+      <c r="R122" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S122" t="inlineStr">
+        <is>
+          <t>3722</t>
         </is>
       </c>
     </row>
@@ -7693,9 +8425,15 @@
       <c r="P123" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q123" t="inlineStr">
-        <is>
-          <t>4300</t>
+      <c r="Q123" t="n">
+        <v>4300</v>
+      </c>
+      <c r="R123" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="S123" t="inlineStr">
+        <is>
+          <t>4467</t>
         </is>
       </c>
     </row>
@@ -7754,7 +8492,13 @@
       <c r="P124" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q124" t="inlineStr">
+      <c r="Q124" t="n">
+        <v>0</v>
+      </c>
+      <c r="R124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S124" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7815,9 +8559,15 @@
       <c r="P125" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="Q125" t="inlineStr">
-        <is>
-          <t>4021</t>
+      <c r="Q125" t="n">
+        <v>4021</v>
+      </c>
+      <c r="R125" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S125" t="inlineStr">
+        <is>
+          <t>4137</t>
         </is>
       </c>
     </row>
@@ -7876,9 +8626,15 @@
       <c r="P126" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q126" t="inlineStr">
-        <is>
-          <t>4023</t>
+      <c r="Q126" t="n">
+        <v>4023</v>
+      </c>
+      <c r="R126" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="S126" t="inlineStr">
+        <is>
+          <t>4084</t>
         </is>
       </c>
     </row>
@@ -7937,9 +8693,15 @@
       <c r="P127" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q127" t="inlineStr">
-        <is>
-          <t>3400</t>
+      <c r="Q127" t="n">
+        <v>3400</v>
+      </c>
+      <c r="R127" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S127" t="inlineStr">
+        <is>
+          <t>3423</t>
         </is>
       </c>
     </row>
@@ -7998,9 +8760,15 @@
       <c r="P128" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="Q128" t="inlineStr">
-        <is>
-          <t>4149</t>
+      <c r="Q128" t="n">
+        <v>4149</v>
+      </c>
+      <c r="R128" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="S128" t="inlineStr">
+        <is>
+          <t>4172</t>
         </is>
       </c>
     </row>
@@ -8059,9 +8827,15 @@
       <c r="P129" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q129" t="inlineStr">
-        <is>
-          <t>2016</t>
+      <c r="Q129" t="n">
+        <v>2016</v>
+      </c>
+      <c r="R129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S129" t="inlineStr">
+        <is>
+          <t>2011</t>
         </is>
       </c>
     </row>
@@ -8120,7 +8894,13 @@
       <c r="P130" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q130" t="inlineStr">
+      <c r="Q130" t="n">
+        <v>0</v>
+      </c>
+      <c r="R130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8181,7 +8961,13 @@
       <c r="P131" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q131" t="inlineStr">
+      <c r="Q131" t="n">
+        <v>0</v>
+      </c>
+      <c r="R131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8242,9 +9028,15 @@
       <c r="P132" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q132" t="inlineStr">
-        <is>
-          <t>3992</t>
+      <c r="Q132" t="n">
+        <v>3992</v>
+      </c>
+      <c r="R132" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S132" t="inlineStr">
+        <is>
+          <t>3984</t>
         </is>
       </c>
     </row>
@@ -8303,7 +9095,13 @@
       <c r="P133" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q133" t="inlineStr">
+      <c r="Q133" t="n">
+        <v>0</v>
+      </c>
+      <c r="R133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8364,9 +9162,15 @@
       <c r="P134" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q134" t="inlineStr">
-        <is>
-          <t>3370</t>
+      <c r="Q134" t="n">
+        <v>3370</v>
+      </c>
+      <c r="R134" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S134" t="inlineStr">
+        <is>
+          <t>3402</t>
         </is>
       </c>
     </row>
@@ -8425,9 +9229,15 @@
       <c r="P135" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Q135" t="inlineStr">
-        <is>
-          <t>4089</t>
+      <c r="Q135" t="n">
+        <v>4089</v>
+      </c>
+      <c r="R135" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S135" t="inlineStr">
+        <is>
+          <t>4198</t>
         </is>
       </c>
     </row>
@@ -8486,9 +9296,15 @@
       <c r="P136" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q136" t="inlineStr">
-        <is>
-          <t>4093</t>
+      <c r="Q136" t="n">
+        <v>4093</v>
+      </c>
+      <c r="R136" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S136" t="inlineStr">
+        <is>
+          <t>4075</t>
         </is>
       </c>
     </row>
@@ -8547,7 +9363,13 @@
       <c r="P137" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q137" t="inlineStr">
+      <c r="Q137" t="n">
+        <v>0</v>
+      </c>
+      <c r="R137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8608,9 +9430,15 @@
       <c r="P138" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q138" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="Q138" t="n">
+        <v>0</v>
+      </c>
+      <c r="R138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S138" t="inlineStr">
+        <is>
+          <t>1498</t>
         </is>
       </c>
     </row>
@@ -8669,9 +9497,15 @@
       <c r="P139" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q139" t="inlineStr">
-        <is>
-          <t>3117</t>
+      <c r="Q139" t="n">
+        <v>3117</v>
+      </c>
+      <c r="R139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S139" t="inlineStr">
+        <is>
+          <t>3142</t>
         </is>
       </c>
     </row>
@@ -8730,7 +9564,13 @@
       <c r="P140" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q140" t="inlineStr">
+      <c r="Q140" t="n">
+        <v>0</v>
+      </c>
+      <c r="R140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8791,7 +9631,13 @@
       <c r="P141" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q141" t="inlineStr">
+      <c r="Q141" t="n">
+        <v>0</v>
+      </c>
+      <c r="R141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8852,9 +9698,15 @@
       <c r="P142" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q142" t="inlineStr">
-        <is>
-          <t>3116</t>
+      <c r="Q142" t="n">
+        <v>3116</v>
+      </c>
+      <c r="R142" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="S142" t="inlineStr">
+        <is>
+          <t>3261</t>
         </is>
       </c>
     </row>
@@ -8913,7 +9765,13 @@
       <c r="P143" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q143" t="inlineStr">
+      <c r="Q143" t="n">
+        <v>0</v>
+      </c>
+      <c r="R143" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8974,9 +9832,15 @@
       <c r="P144" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="Q144" t="inlineStr">
-        <is>
-          <t>3551</t>
+      <c r="Q144" t="n">
+        <v>3551</v>
+      </c>
+      <c r="R144" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S144" t="inlineStr">
+        <is>
+          <t>3520</t>
         </is>
       </c>
     </row>
@@ -9035,7 +9899,13 @@
       <c r="P145" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q145" t="inlineStr">
+      <c r="Q145" t="n">
+        <v>0</v>
+      </c>
+      <c r="R145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9096,7 +9966,13 @@
       <c r="P146" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q146" t="inlineStr">
+      <c r="Q146" t="n">
+        <v>0</v>
+      </c>
+      <c r="R146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9157,9 +10033,15 @@
       <c r="P147" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="Q147" t="inlineStr">
-        <is>
-          <t>2128</t>
+      <c r="Q147" t="n">
+        <v>2128</v>
+      </c>
+      <c r="R147" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="S147" t="inlineStr">
+        <is>
+          <t>2148</t>
         </is>
       </c>
     </row>
@@ -9218,7 +10100,13 @@
       <c r="P148" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q148" t="inlineStr">
+      <c r="Q148" t="n">
+        <v>0</v>
+      </c>
+      <c r="R148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9279,7 +10167,13 @@
       <c r="P149" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q149" t="inlineStr">
+      <c r="Q149" t="n">
+        <v>0</v>
+      </c>
+      <c r="R149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9340,7 +10234,13 @@
       <c r="P150" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q150" t="inlineStr">
+      <c r="Q150" t="n">
+        <v>2604</v>
+      </c>
+      <c r="R150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S150" t="inlineStr">
         <is>
           <t>2604</t>
         </is>
@@ -9401,7 +10301,13 @@
       <c r="P151" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q151" t="inlineStr">
+      <c r="Q151" t="n">
+        <v>0</v>
+      </c>
+      <c r="R151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9462,7 +10368,13 @@
       <c r="P152" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q152" t="inlineStr">
+      <c r="Q152" t="n">
+        <v>0</v>
+      </c>
+      <c r="R152" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9523,7 +10435,13 @@
       <c r="P153" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q153" t="inlineStr">
+      <c r="Q153" t="n">
+        <v>0</v>
+      </c>
+      <c r="R153" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9584,9 +10502,15 @@
       <c r="P154" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q154" t="inlineStr">
-        <is>
-          <t>2923</t>
+      <c r="Q154" t="n">
+        <v>2923</v>
+      </c>
+      <c r="R154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S154" t="inlineStr">
+        <is>
+          <t>2921</t>
         </is>
       </c>
     </row>
@@ -9645,7 +10569,13 @@
       <c r="P155" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q155" t="inlineStr">
+      <c r="Q155" t="n">
+        <v>0</v>
+      </c>
+      <c r="R155" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9706,7 +10636,13 @@
       <c r="P156" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q156" t="inlineStr">
+      <c r="Q156" t="n">
+        <v>0</v>
+      </c>
+      <c r="R156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9767,7 +10703,13 @@
       <c r="P157" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q157" t="inlineStr">
+      <c r="Q157" t="n">
+        <v>0</v>
+      </c>
+      <c r="R157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9828,9 +10770,15 @@
       <c r="P158" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q158" t="inlineStr">
-        <is>
-          <t>3014</t>
+      <c r="Q158" t="n">
+        <v>3014</v>
+      </c>
+      <c r="R158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S158" t="inlineStr">
+        <is>
+          <t>3103</t>
         </is>
       </c>
     </row>
@@ -9874,6 +10822,8 @@
       <c r="O159" t="inlineStr"/>
       <c r="P159" s="2" t="inlineStr"/>
       <c r="Q159" t="inlineStr"/>
+      <c r="R159" s="2" t="inlineStr"/>
+      <c r="S159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="n">
@@ -9924,9 +10874,15 @@
       <c r="P160" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="Q160" t="inlineStr">
-        <is>
-          <t>4558</t>
+      <c r="Q160" t="n">
+        <v>4558</v>
+      </c>
+      <c r="R160" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="S160" t="inlineStr">
+        <is>
+          <t>4687</t>
         </is>
       </c>
     </row>
@@ -9962,6 +10918,8 @@
       <c r="O161" t="inlineStr"/>
       <c r="P161" s="2" t="inlineStr"/>
       <c r="Q161" t="inlineStr"/>
+      <c r="R161" s="2" t="inlineStr"/>
+      <c r="S161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="n">
@@ -10012,9 +10970,15 @@
       <c r="P162" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="Q162" t="inlineStr">
-        <is>
-          <t>3635</t>
+      <c r="Q162" t="n">
+        <v>3635</v>
+      </c>
+      <c r="R162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S162" t="inlineStr">
+        <is>
+          <t>3774</t>
         </is>
       </c>
     </row>
@@ -10067,9 +11031,15 @@
       <c r="P163" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="Q163" t="inlineStr">
-        <is>
-          <t>2841</t>
+      <c r="Q163" t="n">
+        <v>2841</v>
+      </c>
+      <c r="R163" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="S163" t="inlineStr">
+        <is>
+          <t>2957</t>
         </is>
       </c>
     </row>
@@ -10118,9 +11088,93 @@
       <c r="P164" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="Q164" t="inlineStr">
-        <is>
-          <t>3229</t>
+      <c r="Q164" t="n">
+        <v>3229</v>
+      </c>
+      <c r="R164" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="S164" t="inlineStr">
+        <is>
+          <t>3521</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>138176</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Ze5kyphyr</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr"/>
+      <c r="D165" t="inlineStr"/>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F165" s="2" t="inlineStr"/>
+      <c r="G165" t="inlineStr"/>
+      <c r="H165" s="2" t="inlineStr"/>
+      <c r="I165" t="inlineStr"/>
+      <c r="J165" s="2" t="inlineStr"/>
+      <c r="K165" t="inlineStr"/>
+      <c r="L165" s="2" t="inlineStr"/>
+      <c r="M165" t="inlineStr"/>
+      <c r="N165" s="2" t="inlineStr"/>
+      <c r="O165" t="inlineStr"/>
+      <c r="P165" s="2" t="inlineStr"/>
+      <c r="Q165" t="inlineStr"/>
+      <c r="R165" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="S165" t="inlineStr">
+        <is>
+          <t>6773</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>32929656</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>"EIH Wilson Chu"</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr"/>
+      <c r="D166" t="inlineStr"/>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F166" s="2" t="inlineStr"/>
+      <c r="G166" t="inlineStr"/>
+      <c r="H166" s="2" t="inlineStr"/>
+      <c r="I166" t="inlineStr"/>
+      <c r="J166" s="2" t="inlineStr"/>
+      <c r="K166" t="inlineStr"/>
+      <c r="L166" s="2" t="inlineStr"/>
+      <c r="M166" t="inlineStr"/>
+      <c r="N166" s="2" t="inlineStr"/>
+      <c r="O166" t="inlineStr"/>
+      <c r="P166" s="2" t="inlineStr"/>
+      <c r="Q166" t="inlineStr"/>
+      <c r="R166" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="S166" t="inlineStr">
+        <is>
+          <t>4508</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-23 13:38:34
</commit_message>
<xml_diff>
--- a/Season_Attack/86.xlsx
+++ b/Season_Attack/86.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S166"/>
+  <dimension ref="A1:U169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,6 +486,16 @@
           <t>03-21_0</t>
         </is>
       </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>03-22_A</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>03-22_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -548,9 +558,15 @@
       <c r="R2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>3120</t>
+      <c r="S2" t="n">
+        <v>3120</v>
+      </c>
+      <c r="T2" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>3530</t>
         </is>
       </c>
     </row>
@@ -603,9 +619,15 @@
       <c r="R3" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>6131</t>
+      <c r="S3" t="n">
+        <v>6131</v>
+      </c>
+      <c r="T3" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>6514</t>
         </is>
       </c>
     </row>
@@ -670,9 +692,15 @@
       <c r="R4" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>6079</t>
+      <c r="S4" t="n">
+        <v>6079</v>
+      </c>
+      <c r="T4" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>6431</t>
         </is>
       </c>
     </row>
@@ -737,9 +765,15 @@
       <c r="R5" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>6189</t>
+      <c r="S5" t="n">
+        <v>6189</v>
+      </c>
+      <c r="T5" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>6509</t>
         </is>
       </c>
     </row>
@@ -804,9 +838,15 @@
       <c r="R6" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>5714</t>
+      <c r="S6" t="n">
+        <v>5714</v>
+      </c>
+      <c r="T6" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>5974</t>
         </is>
       </c>
     </row>
@@ -871,9 +911,15 @@
       <c r="R7" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>6351</t>
+      <c r="S7" t="n">
+        <v>6351</v>
+      </c>
+      <c r="T7" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>6671</t>
         </is>
       </c>
     </row>
@@ -938,9 +984,15 @@
       <c r="R8" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>5368</t>
+      <c r="S8" t="n">
+        <v>5368</v>
+      </c>
+      <c r="T8" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>5619</t>
         </is>
       </c>
     </row>
@@ -1005,9 +1057,15 @@
       <c r="R9" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>5703</t>
+      <c r="S9" t="n">
+        <v>5703</v>
+      </c>
+      <c r="T9" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>5809</t>
         </is>
       </c>
     </row>
@@ -1072,9 +1130,15 @@
       <c r="R10" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>6186</t>
+      <c r="S10" t="n">
+        <v>6186</v>
+      </c>
+      <c r="T10" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>6645</t>
         </is>
       </c>
     </row>
@@ -1123,9 +1187,15 @@
       <c r="R11" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>5736</t>
+      <c r="S11" t="n">
+        <v>5736</v>
+      </c>
+      <c r="T11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>5738</t>
         </is>
       </c>
     </row>
@@ -1190,7 +1260,13 @@
       <c r="R12" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S12" t="inlineStr">
+      <c r="S12" t="n">
+        <v>3336</v>
+      </c>
+      <c r="T12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="inlineStr">
         <is>
           <t>3336</t>
         </is>
@@ -1257,9 +1333,15 @@
       <c r="R13" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>6448</t>
+      <c r="S13" t="n">
+        <v>6448</v>
+      </c>
+      <c r="T13" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>6758</t>
         </is>
       </c>
     </row>
@@ -1324,9 +1406,15 @@
       <c r="R14" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>5622</t>
+      <c r="S14" t="n">
+        <v>5622</v>
+      </c>
+      <c r="T14" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>5870</t>
         </is>
       </c>
     </row>
@@ -1375,9 +1463,15 @@
       <c r="R15" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>5912</t>
+      <c r="S15" t="n">
+        <v>5912</v>
+      </c>
+      <c r="T15" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>6205</t>
         </is>
       </c>
     </row>
@@ -1442,9 +1536,15 @@
       <c r="R16" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>4942</t>
+      <c r="S16" t="n">
+        <v>4942</v>
+      </c>
+      <c r="T16" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>5151</t>
         </is>
       </c>
     </row>
@@ -1509,9 +1609,15 @@
       <c r="R17" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>5126</t>
+      <c r="S17" t="n">
+        <v>5126</v>
+      </c>
+      <c r="T17" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>5208</t>
         </is>
       </c>
     </row>
@@ -1576,9 +1682,15 @@
       <c r="R18" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>5784</t>
+      <c r="S18" t="n">
+        <v>5784</v>
+      </c>
+      <c r="T18" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>6072</t>
         </is>
       </c>
     </row>
@@ -1627,9 +1739,15 @@
       <c r="R19" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>6605</t>
+      <c r="S19" t="n">
+        <v>6605</v>
+      </c>
+      <c r="T19" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>6972</t>
         </is>
       </c>
     </row>
@@ -1694,7 +1812,13 @@
       <c r="R20" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="S20" t="inlineStr">
+      <c r="S20" t="n">
+        <v>4932</v>
+      </c>
+      <c r="T20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" t="inlineStr">
         <is>
           <t>4932</t>
         </is>
@@ -1761,9 +1885,15 @@
       <c r="R21" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>5989</t>
+      <c r="S21" t="n">
+        <v>5989</v>
+      </c>
+      <c r="T21" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>6282</t>
         </is>
       </c>
     </row>
@@ -1828,9 +1958,15 @@
       <c r="R22" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>5338</t>
+      <c r="S22" t="n">
+        <v>5338</v>
+      </c>
+      <c r="T22" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>5754</t>
         </is>
       </c>
     </row>
@@ -1895,9 +2031,15 @@
       <c r="R23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>5821</t>
+      <c r="S23" t="n">
+        <v>5821</v>
+      </c>
+      <c r="T23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>6101</t>
         </is>
       </c>
     </row>
@@ -1962,7 +2104,13 @@
       <c r="R24" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S24" t="inlineStr">
+      <c r="S24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2029,9 +2177,15 @@
       <c r="R25" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>2641</t>
+      <c r="S25" t="n">
+        <v>2641</v>
+      </c>
+      <c r="T25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>2673</t>
         </is>
       </c>
     </row>
@@ -2076,9 +2230,15 @@
       <c r="R26" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>6054</t>
+      <c r="S26" t="n">
+        <v>6054</v>
+      </c>
+      <c r="T26" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>6383</t>
         </is>
       </c>
     </row>
@@ -2088,7 +2248,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>꧁S.TIGRESS꧂ᶻᵍˣ</t>
+          <t>AOW全体工作人员吃屎交易大厅</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2123,9 +2283,15 @@
       <c r="R27" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>5200</t>
+      <c r="S27" t="n">
+        <v>5200</v>
+      </c>
+      <c r="T27" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>5660</t>
         </is>
       </c>
     </row>
@@ -2190,9 +2356,15 @@
       <c r="R28" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>6274</t>
+      <c r="S28" t="n">
+        <v>6274</v>
+      </c>
+      <c r="T28" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>6532</t>
         </is>
       </c>
     </row>
@@ -2237,9 +2409,15 @@
       <c r="R29" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S29" t="inlineStr">
-        <is>
-          <t>5511</t>
+      <c r="S29" t="n">
+        <v>5511</v>
+      </c>
+      <c r="T29" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>5568</t>
         </is>
       </c>
     </row>
@@ -2304,9 +2482,15 @@
       <c r="R30" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>5058</t>
+      <c r="S30" t="n">
+        <v>5058</v>
+      </c>
+      <c r="T30" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>5255</t>
         </is>
       </c>
     </row>
@@ -2371,9 +2555,15 @@
       <c r="R31" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="S31" t="inlineStr">
-        <is>
-          <t>6482</t>
+      <c r="S31" t="n">
+        <v>6482</v>
+      </c>
+      <c r="T31" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>6748</t>
         </is>
       </c>
     </row>
@@ -2422,9 +2612,15 @@
       <c r="R32" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="S32" t="inlineStr">
-        <is>
-          <t>4344</t>
+      <c r="S32" t="n">
+        <v>4344</v>
+      </c>
+      <c r="T32" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>4509</t>
         </is>
       </c>
     </row>
@@ -2489,9 +2685,15 @@
       <c r="R33" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="S33" t="inlineStr">
-        <is>
-          <t>5775</t>
+      <c r="S33" t="n">
+        <v>5775</v>
+      </c>
+      <c r="T33" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>5929</t>
         </is>
       </c>
     </row>
@@ -2556,9 +2758,15 @@
       <c r="R34" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="S34" t="inlineStr">
-        <is>
-          <t>6255</t>
+      <c r="S34" t="n">
+        <v>6255</v>
+      </c>
+      <c r="T34" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>6470</t>
         </is>
       </c>
     </row>
@@ -2623,9 +2831,15 @@
       <c r="R35" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S35" t="inlineStr">
-        <is>
-          <t>5650</t>
+      <c r="S35" t="n">
+        <v>5650</v>
+      </c>
+      <c r="T35" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>5921</t>
         </is>
       </c>
     </row>
@@ -2670,9 +2884,15 @@
       <c r="R36" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="S36" t="inlineStr">
-        <is>
-          <t>4955</t>
+      <c r="S36" t="n">
+        <v>4955</v>
+      </c>
+      <c r="T36" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>5087</t>
         </is>
       </c>
     </row>
@@ -2737,9 +2957,15 @@
       <c r="R37" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S37" t="inlineStr">
-        <is>
-          <t>5808</t>
+      <c r="S37" t="n">
+        <v>5808</v>
+      </c>
+      <c r="T37" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>6054</t>
         </is>
       </c>
     </row>
@@ -2804,9 +3030,15 @@
       <c r="R38" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="S38" t="inlineStr">
-        <is>
-          <t>5524</t>
+      <c r="S38" t="n">
+        <v>5524</v>
+      </c>
+      <c r="T38" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>5716</t>
         </is>
       </c>
     </row>
@@ -2871,9 +3103,15 @@
       <c r="R39" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="S39" t="inlineStr">
-        <is>
-          <t>6135</t>
+      <c r="S39" t="n">
+        <v>6135</v>
+      </c>
+      <c r="T39" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>6398</t>
         </is>
       </c>
     </row>
@@ -2938,9 +3176,15 @@
       <c r="R40" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="S40" t="inlineStr">
-        <is>
-          <t>6540</t>
+      <c r="S40" t="n">
+        <v>6540</v>
+      </c>
+      <c r="T40" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>6870</t>
         </is>
       </c>
     </row>
@@ -3005,9 +3249,15 @@
       <c r="R41" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="S41" t="inlineStr">
-        <is>
-          <t>5877</t>
+      <c r="S41" t="n">
+        <v>5877</v>
+      </c>
+      <c r="T41" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>6095</t>
         </is>
       </c>
     </row>
@@ -3072,9 +3322,15 @@
       <c r="R42" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S42" t="inlineStr">
-        <is>
-          <t>5818</t>
+      <c r="S42" t="n">
+        <v>5818</v>
+      </c>
+      <c r="T42" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>6044</t>
         </is>
       </c>
     </row>
@@ -3139,9 +3395,15 @@
       <c r="R43" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="S43" t="inlineStr">
-        <is>
-          <t>5289</t>
+      <c r="S43" t="n">
+        <v>5289</v>
+      </c>
+      <c r="T43" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>5417</t>
         </is>
       </c>
     </row>
@@ -3206,9 +3468,15 @@
       <c r="R44" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="S44" t="inlineStr">
-        <is>
-          <t>5511</t>
+      <c r="S44" t="n">
+        <v>5511</v>
+      </c>
+      <c r="T44" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>5597</t>
         </is>
       </c>
     </row>
@@ -3273,9 +3541,15 @@
       <c r="R45" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S45" t="inlineStr">
-        <is>
-          <t>4992</t>
+      <c r="S45" t="n">
+        <v>4992</v>
+      </c>
+      <c r="T45" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>5007</t>
         </is>
       </c>
     </row>
@@ -3340,9 +3614,15 @@
       <c r="R46" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="S46" t="inlineStr">
-        <is>
-          <t>6156</t>
+      <c r="S46" t="n">
+        <v>6156</v>
+      </c>
+      <c r="T46" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>6370</t>
         </is>
       </c>
     </row>
@@ -3407,9 +3687,15 @@
       <c r="R47" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="S47" t="inlineStr">
-        <is>
-          <t>5096</t>
+      <c r="S47" t="n">
+        <v>5096</v>
+      </c>
+      <c r="T47" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>5406</t>
         </is>
       </c>
     </row>
@@ -3474,7 +3760,13 @@
       <c r="R48" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S48" t="inlineStr">
+      <c r="S48" t="n">
+        <v>2548</v>
+      </c>
+      <c r="T48" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U48" t="inlineStr">
         <is>
           <t>2548</t>
         </is>
@@ -3512,6 +3804,8 @@
       <c r="Q49" t="inlineStr"/>
       <c r="R49" s="2" t="inlineStr"/>
       <c r="S49" t="inlineStr"/>
+      <c r="T49" s="2" t="inlineStr"/>
+      <c r="U49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -3574,7 +3868,13 @@
       <c r="R50" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S50" t="inlineStr">
+      <c r="S50" t="n">
+        <v>0</v>
+      </c>
+      <c r="T50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U50" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3641,9 +3941,15 @@
       <c r="R51" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S51" t="inlineStr">
-        <is>
-          <t>2819</t>
+      <c r="S51" t="n">
+        <v>2819</v>
+      </c>
+      <c r="T51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U51" t="inlineStr">
+        <is>
+          <t>2818</t>
         </is>
       </c>
     </row>
@@ -3708,7 +4014,13 @@
       <c r="R52" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S52" t="inlineStr">
+      <c r="S52" t="n">
+        <v>3184</v>
+      </c>
+      <c r="T52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U52" t="inlineStr">
         <is>
           <t>3184</t>
         </is>
@@ -3775,9 +4087,15 @@
       <c r="R53" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S53" t="inlineStr">
-        <is>
-          <t>5457</t>
+      <c r="S53" t="n">
+        <v>5457</v>
+      </c>
+      <c r="T53" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>5797</t>
         </is>
       </c>
     </row>
@@ -3842,9 +4160,15 @@
       <c r="R54" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S54" t="inlineStr">
-        <is>
-          <t>4753</t>
+      <c r="S54" t="n">
+        <v>4753</v>
+      </c>
+      <c r="T54" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U54" t="inlineStr">
+        <is>
+          <t>4993</t>
         </is>
       </c>
     </row>
@@ -3909,9 +4233,15 @@
       <c r="R55" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S55" t="inlineStr">
-        <is>
-          <t>4941</t>
+      <c r="S55" t="n">
+        <v>4941</v>
+      </c>
+      <c r="T55" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>5140</t>
         </is>
       </c>
     </row>
@@ -3976,9 +4306,15 @@
       <c r="R56" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S56" t="inlineStr">
-        <is>
-          <t>5455</t>
+      <c r="S56" t="n">
+        <v>5455</v>
+      </c>
+      <c r="T56" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U56" t="inlineStr">
+        <is>
+          <t>5728</t>
         </is>
       </c>
     </row>
@@ -4043,9 +4379,15 @@
       <c r="R57" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S57" t="inlineStr">
-        <is>
-          <t>4922</t>
+      <c r="S57" t="n">
+        <v>4922</v>
+      </c>
+      <c r="T57" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="U57" t="inlineStr">
+        <is>
+          <t>5062</t>
         </is>
       </c>
     </row>
@@ -4110,9 +4452,15 @@
       <c r="R58" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="S58" t="inlineStr">
-        <is>
-          <t>4624</t>
+      <c r="S58" t="n">
+        <v>4624</v>
+      </c>
+      <c r="T58" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="U58" t="inlineStr">
+        <is>
+          <t>4845</t>
         </is>
       </c>
     </row>
@@ -4177,7 +4525,13 @@
       <c r="R59" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S59" t="inlineStr">
+      <c r="S59" t="n">
+        <v>0</v>
+      </c>
+      <c r="T59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U59" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4244,9 +4598,15 @@
       <c r="R60" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="S60" t="inlineStr">
-        <is>
-          <t>5658</t>
+      <c r="S60" t="n">
+        <v>5658</v>
+      </c>
+      <c r="T60" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="U60" t="inlineStr">
+        <is>
+          <t>5878</t>
         </is>
       </c>
     </row>
@@ -4311,7 +4671,13 @@
       <c r="R61" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S61" t="inlineStr">
+      <c r="S61" t="n">
+        <v>2758</v>
+      </c>
+      <c r="T61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U61" t="inlineStr">
         <is>
           <t>2758</t>
         </is>
@@ -4378,9 +4744,15 @@
       <c r="R62" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S62" t="inlineStr">
-        <is>
-          <t>3241</t>
+      <c r="S62" t="n">
+        <v>3241</v>
+      </c>
+      <c r="T62" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U62" t="inlineStr">
+        <is>
+          <t>3237</t>
         </is>
       </c>
     </row>
@@ -4445,9 +4817,15 @@
       <c r="R63" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="S63" t="inlineStr">
-        <is>
-          <t>5272</t>
+      <c r="S63" t="n">
+        <v>5272</v>
+      </c>
+      <c r="T63" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>5476</t>
         </is>
       </c>
     </row>
@@ -4512,9 +4890,15 @@
       <c r="R64" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="S64" t="inlineStr">
-        <is>
-          <t>6017</t>
+      <c r="S64" t="n">
+        <v>6017</v>
+      </c>
+      <c r="T64" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="U64" t="inlineStr">
+        <is>
+          <t>6297</t>
         </is>
       </c>
     </row>
@@ -4579,9 +4963,15 @@
       <c r="R65" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S65" t="inlineStr">
-        <is>
-          <t>3298</t>
+      <c r="S65" t="n">
+        <v>3298</v>
+      </c>
+      <c r="T65" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="U65" t="inlineStr">
+        <is>
+          <t>3760</t>
         </is>
       </c>
     </row>
@@ -4646,9 +5036,15 @@
       <c r="R66" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="S66" t="inlineStr">
-        <is>
-          <t>4903</t>
+      <c r="S66" t="n">
+        <v>4903</v>
+      </c>
+      <c r="T66" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U66" t="inlineStr">
+        <is>
+          <t>5103</t>
         </is>
       </c>
     </row>
@@ -4713,9 +5109,15 @@
       <c r="R67" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="S67" t="inlineStr">
-        <is>
-          <t>3405</t>
+      <c r="S67" t="n">
+        <v>3405</v>
+      </c>
+      <c r="T67" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>3924</t>
         </is>
       </c>
     </row>
@@ -4780,7 +5182,13 @@
       <c r="R68" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S68" t="inlineStr">
+      <c r="S68" t="n">
+        <v>0</v>
+      </c>
+      <c r="T68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4847,9 +5255,15 @@
       <c r="R69" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="S69" t="inlineStr">
-        <is>
-          <t>4327</t>
+      <c r="S69" t="n">
+        <v>4327</v>
+      </c>
+      <c r="T69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U69" t="inlineStr">
+        <is>
+          <t>4297</t>
         </is>
       </c>
     </row>
@@ -4914,9 +5328,15 @@
       <c r="R70" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S70" t="inlineStr">
-        <is>
-          <t>4813</t>
+      <c r="S70" t="n">
+        <v>4813</v>
+      </c>
+      <c r="T70" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U70" t="inlineStr">
+        <is>
+          <t>4985</t>
         </is>
       </c>
     </row>
@@ -4981,9 +5401,15 @@
       <c r="R71" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S71" t="inlineStr">
-        <is>
-          <t>3225</t>
+      <c r="S71" t="n">
+        <v>3225</v>
+      </c>
+      <c r="T71" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U71" t="inlineStr">
+        <is>
+          <t>3709</t>
         </is>
       </c>
     </row>
@@ -5048,9 +5474,15 @@
       <c r="R72" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="S72" t="inlineStr">
-        <is>
-          <t>4668</t>
+      <c r="S72" t="n">
+        <v>4668</v>
+      </c>
+      <c r="T72" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="U72" t="inlineStr">
+        <is>
+          <t>4778</t>
         </is>
       </c>
     </row>
@@ -5115,9 +5547,15 @@
       <c r="R73" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S73" t="inlineStr">
-        <is>
-          <t>5369</t>
+      <c r="S73" t="n">
+        <v>5369</v>
+      </c>
+      <c r="T73" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U73" t="inlineStr">
+        <is>
+          <t>5589</t>
         </is>
       </c>
     </row>
@@ -5182,7 +5620,13 @@
       <c r="R74" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S74" t="inlineStr">
+      <c r="S74" t="n">
+        <v>0</v>
+      </c>
+      <c r="T74" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5249,7 +5693,13 @@
       <c r="R75" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S75" t="inlineStr">
+      <c r="S75" t="n">
+        <v>0</v>
+      </c>
+      <c r="T75" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5316,9 +5766,15 @@
       <c r="R76" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="S76" t="inlineStr">
-        <is>
-          <t>5342</t>
+      <c r="S76" t="n">
+        <v>5342</v>
+      </c>
+      <c r="T76" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="U76" t="inlineStr">
+        <is>
+          <t>5560</t>
         </is>
       </c>
     </row>
@@ -5383,7 +5839,13 @@
       <c r="R77" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S77" t="inlineStr">
+      <c r="S77" t="n">
+        <v>0</v>
+      </c>
+      <c r="T77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5450,9 +5912,15 @@
       <c r="R78" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="S78" t="inlineStr">
-        <is>
-          <t>5178</t>
+      <c r="S78" t="n">
+        <v>5178</v>
+      </c>
+      <c r="T78" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="U78" t="inlineStr">
+        <is>
+          <t>5303</t>
         </is>
       </c>
     </row>
@@ -5517,7 +5985,13 @@
       <c r="R79" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S79" t="inlineStr">
+      <c r="S79" t="n">
+        <v>3331</v>
+      </c>
+      <c r="T79" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U79" t="inlineStr">
         <is>
           <t>3331</t>
         </is>
@@ -5555,6 +6029,8 @@
       <c r="Q80" t="inlineStr"/>
       <c r="R80" s="2" t="inlineStr"/>
       <c r="S80" t="inlineStr"/>
+      <c r="T80" s="2" t="inlineStr"/>
+      <c r="U80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -5617,9 +6093,15 @@
       <c r="R81" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S81" t="inlineStr">
-        <is>
-          <t>5270</t>
+      <c r="S81" t="n">
+        <v>5270</v>
+      </c>
+      <c r="T81" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U81" t="inlineStr">
+        <is>
+          <t>5523</t>
         </is>
       </c>
     </row>
@@ -5684,9 +6166,15 @@
       <c r="R82" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S82" t="inlineStr">
-        <is>
-          <t>4982</t>
+      <c r="S82" t="n">
+        <v>4982</v>
+      </c>
+      <c r="T82" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="U82" t="inlineStr">
+        <is>
+          <t>5221</t>
         </is>
       </c>
     </row>
@@ -5751,9 +6239,15 @@
       <c r="R83" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="S83" t="inlineStr">
-        <is>
-          <t>4832</t>
+      <c r="S83" t="n">
+        <v>4832</v>
+      </c>
+      <c r="T83" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U83" t="inlineStr">
+        <is>
+          <t>5023</t>
         </is>
       </c>
     </row>
@@ -5818,9 +6312,15 @@
       <c r="R84" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S84" t="inlineStr">
-        <is>
-          <t>4672</t>
+      <c r="S84" t="n">
+        <v>4672</v>
+      </c>
+      <c r="T84" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U84" t="inlineStr">
+        <is>
+          <t>4776</t>
         </is>
       </c>
     </row>
@@ -5885,9 +6385,15 @@
       <c r="R85" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="S85" t="inlineStr">
-        <is>
-          <t>4663</t>
+      <c r="S85" t="n">
+        <v>4663</v>
+      </c>
+      <c r="T85" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U85" t="inlineStr">
+        <is>
+          <t>4725</t>
         </is>
       </c>
     </row>
@@ -5952,9 +6458,15 @@
       <c r="R86" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S86" t="inlineStr">
-        <is>
-          <t>4064</t>
+      <c r="S86" t="n">
+        <v>4064</v>
+      </c>
+      <c r="T86" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U86" t="inlineStr">
+        <is>
+          <t>4392</t>
         </is>
       </c>
     </row>
@@ -6019,9 +6531,15 @@
       <c r="R87" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="S87" t="inlineStr">
-        <is>
-          <t>4907</t>
+      <c r="S87" t="n">
+        <v>4907</v>
+      </c>
+      <c r="T87" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U87" t="inlineStr">
+        <is>
+          <t>5247</t>
         </is>
       </c>
     </row>
@@ -6086,9 +6604,15 @@
       <c r="R88" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S88" t="inlineStr">
-        <is>
-          <t>3659</t>
+      <c r="S88" t="n">
+        <v>3659</v>
+      </c>
+      <c r="T88" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U88" t="inlineStr">
+        <is>
+          <t>3804</t>
         </is>
       </c>
     </row>
@@ -6153,9 +6677,15 @@
       <c r="R89" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S89" t="inlineStr">
-        <is>
-          <t>4156</t>
+      <c r="S89" t="n">
+        <v>4156</v>
+      </c>
+      <c r="T89" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U89" t="inlineStr">
+        <is>
+          <t>4133</t>
         </is>
       </c>
     </row>
@@ -6220,9 +6750,15 @@
       <c r="R90" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S90" t="inlineStr">
-        <is>
-          <t>2862</t>
+      <c r="S90" t="n">
+        <v>2862</v>
+      </c>
+      <c r="T90" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U90" t="inlineStr">
+        <is>
+          <t>3127</t>
         </is>
       </c>
     </row>
@@ -6287,9 +6823,15 @@
       <c r="R91" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="S91" t="inlineStr">
-        <is>
-          <t>3988</t>
+      <c r="S91" t="n">
+        <v>3988</v>
+      </c>
+      <c r="T91" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="U91" t="inlineStr">
+        <is>
+          <t>4035</t>
         </is>
       </c>
     </row>
@@ -6354,7 +6896,13 @@
       <c r="R92" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S92" t="inlineStr">
+      <c r="S92" t="n">
+        <v>0</v>
+      </c>
+      <c r="T92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6421,9 +6969,15 @@
       <c r="R93" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="S93" t="inlineStr">
-        <is>
-          <t>3998</t>
+      <c r="S93" t="n">
+        <v>3998</v>
+      </c>
+      <c r="T93" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="U93" t="inlineStr">
+        <is>
+          <t>4095</t>
         </is>
       </c>
     </row>
@@ -6488,9 +7042,15 @@
       <c r="R94" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S94" t="inlineStr">
-        <is>
-          <t>2579</t>
+      <c r="S94" t="n">
+        <v>2579</v>
+      </c>
+      <c r="T94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U94" t="inlineStr">
+        <is>
+          <t>2592</t>
         </is>
       </c>
     </row>
@@ -6555,9 +7115,15 @@
       <c r="R95" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="S95" t="inlineStr">
-        <is>
-          <t>4252</t>
+      <c r="S95" t="n">
+        <v>4252</v>
+      </c>
+      <c r="T95" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U95" t="inlineStr">
+        <is>
+          <t>4317</t>
         </is>
       </c>
     </row>
@@ -6622,9 +7188,15 @@
       <c r="R96" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="S96" t="inlineStr">
-        <is>
-          <t>2624</t>
+      <c r="S96" t="n">
+        <v>2624</v>
+      </c>
+      <c r="T96" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U96" t="inlineStr">
+        <is>
+          <t>2623</t>
         </is>
       </c>
     </row>
@@ -6689,9 +7261,15 @@
       <c r="R97" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S97" t="inlineStr">
-        <is>
-          <t>2193</t>
+      <c r="S97" t="n">
+        <v>2193</v>
+      </c>
+      <c r="T97" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U97" t="inlineStr">
+        <is>
+          <t>2213</t>
         </is>
       </c>
     </row>
@@ -6756,7 +7334,13 @@
       <c r="R98" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S98" t="inlineStr">
+      <c r="S98" t="n">
+        <v>3356</v>
+      </c>
+      <c r="T98" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U98" t="inlineStr">
         <is>
           <t>3356</t>
         </is>
@@ -6823,9 +7407,15 @@
       <c r="R99" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S99" t="inlineStr">
-        <is>
-          <t>2492</t>
+      <c r="S99" t="n">
+        <v>2492</v>
+      </c>
+      <c r="T99" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U99" t="inlineStr">
+        <is>
+          <t>2507</t>
         </is>
       </c>
     </row>
@@ -6890,9 +7480,15 @@
       <c r="R100" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="S100" t="inlineStr">
-        <is>
-          <t>4139</t>
+      <c r="S100" t="n">
+        <v>4139</v>
+      </c>
+      <c r="T100" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U100" t="inlineStr">
+        <is>
+          <t>4181</t>
         </is>
       </c>
     </row>
@@ -6957,9 +7553,15 @@
       <c r="R101" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S101" t="inlineStr">
-        <is>
-          <t>2357</t>
+      <c r="S101" t="n">
+        <v>2357</v>
+      </c>
+      <c r="T101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U101" t="inlineStr">
+        <is>
+          <t>2356</t>
         </is>
       </c>
     </row>
@@ -7024,9 +7626,15 @@
       <c r="R102" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="S102" t="inlineStr">
-        <is>
-          <t>5132</t>
+      <c r="S102" t="n">
+        <v>5132</v>
+      </c>
+      <c r="T102" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="U102" t="inlineStr">
+        <is>
+          <t>5267</t>
         </is>
       </c>
     </row>
@@ -7091,9 +7699,15 @@
       <c r="R103" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S103" t="inlineStr">
-        <is>
-          <t>4601</t>
+      <c r="S103" t="n">
+        <v>4601</v>
+      </c>
+      <c r="T103" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U103" t="inlineStr">
+        <is>
+          <t>4665</t>
         </is>
       </c>
     </row>
@@ -7158,9 +7772,15 @@
       <c r="R104" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S104" t="inlineStr">
-        <is>
-          <t>4621</t>
+      <c r="S104" t="n">
+        <v>4621</v>
+      </c>
+      <c r="T104" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="U104" t="inlineStr">
+        <is>
+          <t>4654</t>
         </is>
       </c>
     </row>
@@ -7225,9 +7845,15 @@
       <c r="R105" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="S105" t="inlineStr">
-        <is>
-          <t>4976</t>
+      <c r="S105" t="n">
+        <v>4976</v>
+      </c>
+      <c r="T105" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="U105" t="inlineStr">
+        <is>
+          <t>5135</t>
         </is>
       </c>
     </row>
@@ -7292,9 +7918,15 @@
       <c r="R106" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S106" t="inlineStr">
-        <is>
-          <t>4604</t>
+      <c r="S106" t="n">
+        <v>4604</v>
+      </c>
+      <c r="T106" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="U106" t="inlineStr">
+        <is>
+          <t>4720</t>
         </is>
       </c>
     </row>
@@ -7359,9 +7991,15 @@
       <c r="R107" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="S107" t="inlineStr">
-        <is>
-          <t>5074</t>
+      <c r="S107" t="n">
+        <v>5074</v>
+      </c>
+      <c r="T107" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="U107" t="inlineStr">
+        <is>
+          <t>5272</t>
         </is>
       </c>
     </row>
@@ -7426,7 +8064,13 @@
       <c r="R108" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S108" t="inlineStr">
+      <c r="S108" t="n">
+        <v>0</v>
+      </c>
+      <c r="T108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7493,9 +8137,15 @@
       <c r="R109" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S109" t="inlineStr">
-        <is>
-          <t>3044</t>
+      <c r="S109" t="n">
+        <v>3044</v>
+      </c>
+      <c r="T109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U109" t="inlineStr">
+        <is>
+          <t>3061</t>
         </is>
       </c>
     </row>
@@ -7560,7 +8210,13 @@
       <c r="R110" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S110" t="inlineStr">
+      <c r="S110" t="n">
+        <v>0</v>
+      </c>
+      <c r="T110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U110" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7627,9 +8283,15 @@
       <c r="R111" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="S111" t="inlineStr">
-        <is>
-          <t>4505</t>
+      <c r="S111" t="n">
+        <v>4505</v>
+      </c>
+      <c r="T111" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="U111" t="inlineStr">
+        <is>
+          <t>4596</t>
         </is>
       </c>
     </row>
@@ -7694,9 +8356,15 @@
       <c r="R112" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="S112" t="inlineStr">
-        <is>
-          <t>4623</t>
+      <c r="S112" t="n">
+        <v>4623</v>
+      </c>
+      <c r="T112" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="U112" t="inlineStr">
+        <is>
+          <t>4710</t>
         </is>
       </c>
     </row>
@@ -7761,9 +8429,15 @@
       <c r="R113" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S113" t="inlineStr">
-        <is>
-          <t>4042</t>
+      <c r="S113" t="n">
+        <v>4042</v>
+      </c>
+      <c r="T113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U113" t="inlineStr">
+        <is>
+          <t>4024</t>
         </is>
       </c>
     </row>
@@ -7828,9 +8502,15 @@
       <c r="R114" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S114" t="inlineStr">
-        <is>
-          <t>2631</t>
+      <c r="S114" t="n">
+        <v>2631</v>
+      </c>
+      <c r="T114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U114" t="inlineStr">
+        <is>
+          <t>2660</t>
         </is>
       </c>
     </row>
@@ -7895,9 +8575,15 @@
       <c r="R115" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="S115" t="inlineStr">
-        <is>
-          <t>4310</t>
+      <c r="S115" t="n">
+        <v>4310</v>
+      </c>
+      <c r="T115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U115" t="inlineStr">
+        <is>
+          <t>4443</t>
         </is>
       </c>
     </row>
@@ -7962,9 +8648,15 @@
       <c r="R116" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S116" t="inlineStr">
-        <is>
-          <t>3285</t>
+      <c r="S116" t="n">
+        <v>3285</v>
+      </c>
+      <c r="T116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U116" t="inlineStr">
+        <is>
+          <t>3356</t>
         </is>
       </c>
     </row>
@@ -8029,9 +8721,15 @@
       <c r="R117" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="S117" t="inlineStr">
-        <is>
-          <t>2632</t>
+      <c r="S117" t="n">
+        <v>2632</v>
+      </c>
+      <c r="T117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U117" t="inlineStr">
+        <is>
+          <t>2629</t>
         </is>
       </c>
     </row>
@@ -8096,9 +8794,15 @@
       <c r="R118" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="S118" t="inlineStr">
-        <is>
-          <t>3434</t>
+      <c r="S118" t="n">
+        <v>3434</v>
+      </c>
+      <c r="T118" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="U118" t="inlineStr">
+        <is>
+          <t>3619</t>
         </is>
       </c>
     </row>
@@ -8163,9 +8867,15 @@
       <c r="R119" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="S119" t="inlineStr">
-        <is>
-          <t>4582</t>
+      <c r="S119" t="n">
+        <v>4582</v>
+      </c>
+      <c r="T119" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="U119" t="inlineStr">
+        <is>
+          <t>4743</t>
         </is>
       </c>
     </row>
@@ -8230,9 +8940,15 @@
       <c r="R120" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S120" t="inlineStr">
-        <is>
-          <t>2949</t>
+      <c r="S120" t="n">
+        <v>2949</v>
+      </c>
+      <c r="T120" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U120" t="inlineStr">
+        <is>
+          <t>2997</t>
         </is>
       </c>
     </row>
@@ -8297,9 +9013,15 @@
       <c r="R121" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="S121" t="inlineStr">
-        <is>
-          <t>1686</t>
+      <c r="S121" t="n">
+        <v>1686</v>
+      </c>
+      <c r="T121" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="U121" t="inlineStr">
+        <is>
+          <t>1728</t>
         </is>
       </c>
     </row>
@@ -8364,9 +9086,15 @@
       <c r="R122" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S122" t="inlineStr">
-        <is>
-          <t>3722</t>
+      <c r="S122" t="n">
+        <v>3722</v>
+      </c>
+      <c r="T122" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U122" t="inlineStr">
+        <is>
+          <t>3967</t>
         </is>
       </c>
     </row>
@@ -8431,9 +9159,15 @@
       <c r="R123" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="S123" t="inlineStr">
-        <is>
-          <t>4467</t>
+      <c r="S123" t="n">
+        <v>4467</v>
+      </c>
+      <c r="T123" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="U123" t="inlineStr">
+        <is>
+          <t>4633</t>
         </is>
       </c>
     </row>
@@ -8498,7 +9232,13 @@
       <c r="R124" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S124" t="inlineStr">
+      <c r="S124" t="n">
+        <v>0</v>
+      </c>
+      <c r="T124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U124" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8565,9 +9305,15 @@
       <c r="R125" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S125" t="inlineStr">
-        <is>
-          <t>4137</t>
+      <c r="S125" t="n">
+        <v>4137</v>
+      </c>
+      <c r="T125" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U125" t="inlineStr">
+        <is>
+          <t>4243</t>
         </is>
       </c>
     </row>
@@ -8632,9 +9378,15 @@
       <c r="R126" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="S126" t="inlineStr">
-        <is>
-          <t>4084</t>
+      <c r="S126" t="n">
+        <v>4084</v>
+      </c>
+      <c r="T126" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U126" t="inlineStr">
+        <is>
+          <t>4189</t>
         </is>
       </c>
     </row>
@@ -8699,9 +9451,15 @@
       <c r="R127" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S127" t="inlineStr">
-        <is>
-          <t>3423</t>
+      <c r="S127" t="n">
+        <v>3423</v>
+      </c>
+      <c r="T127" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U127" t="inlineStr">
+        <is>
+          <t>3421</t>
         </is>
       </c>
     </row>
@@ -8766,9 +9524,15 @@
       <c r="R128" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="S128" t="inlineStr">
-        <is>
-          <t>4172</t>
+      <c r="S128" t="n">
+        <v>4172</v>
+      </c>
+      <c r="T128" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="U128" t="inlineStr">
+        <is>
+          <t>4237</t>
         </is>
       </c>
     </row>
@@ -8833,9 +9597,15 @@
       <c r="R129" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S129" t="inlineStr">
-        <is>
-          <t>2011</t>
+      <c r="S129" t="n">
+        <v>2011</v>
+      </c>
+      <c r="T129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U129" t="inlineStr">
+        <is>
+          <t>2008</t>
         </is>
       </c>
     </row>
@@ -8900,7 +9670,13 @@
       <c r="R130" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S130" t="inlineStr">
+      <c r="S130" t="n">
+        <v>0</v>
+      </c>
+      <c r="T130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8967,7 +9743,13 @@
       <c r="R131" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S131" t="inlineStr">
+      <c r="S131" t="n">
+        <v>0</v>
+      </c>
+      <c r="T131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9034,9 +9816,15 @@
       <c r="R132" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S132" t="inlineStr">
-        <is>
-          <t>3984</t>
+      <c r="S132" t="n">
+        <v>3984</v>
+      </c>
+      <c r="T132" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U132" t="inlineStr">
+        <is>
+          <t>4004</t>
         </is>
       </c>
     </row>
@@ -9101,7 +9889,13 @@
       <c r="R133" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S133" t="inlineStr">
+      <c r="S133" t="n">
+        <v>0</v>
+      </c>
+      <c r="T133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9168,9 +9962,15 @@
       <c r="R134" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S134" t="inlineStr">
-        <is>
-          <t>3402</t>
+      <c r="S134" t="n">
+        <v>3402</v>
+      </c>
+      <c r="T134" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U134" t="inlineStr">
+        <is>
+          <t>3475</t>
         </is>
       </c>
     </row>
@@ -9235,9 +10035,15 @@
       <c r="R135" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S135" t="inlineStr">
-        <is>
-          <t>4198</t>
+      <c r="S135" t="n">
+        <v>4198</v>
+      </c>
+      <c r="T135" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U135" t="inlineStr">
+        <is>
+          <t>4203</t>
         </is>
       </c>
     </row>
@@ -9302,9 +10108,15 @@
       <c r="R136" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S136" t="inlineStr">
-        <is>
-          <t>4075</t>
+      <c r="S136" t="n">
+        <v>4075</v>
+      </c>
+      <c r="T136" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U136" t="inlineStr">
+        <is>
+          <t>4135</t>
         </is>
       </c>
     </row>
@@ -9369,7 +10181,13 @@
       <c r="R137" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S137" t="inlineStr">
+      <c r="S137" t="n">
+        <v>0</v>
+      </c>
+      <c r="T137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9436,9 +10254,15 @@
       <c r="R138" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S138" t="inlineStr">
-        <is>
-          <t>1498</t>
+      <c r="S138" t="n">
+        <v>1498</v>
+      </c>
+      <c r="T138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U138" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -9503,9 +10327,15 @@
       <c r="R139" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S139" t="inlineStr">
-        <is>
-          <t>3142</t>
+      <c r="S139" t="n">
+        <v>3142</v>
+      </c>
+      <c r="T139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U139" t="inlineStr">
+        <is>
+          <t>3146</t>
         </is>
       </c>
     </row>
@@ -9570,7 +10400,13 @@
       <c r="R140" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S140" t="inlineStr">
+      <c r="S140" t="n">
+        <v>0</v>
+      </c>
+      <c r="T140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9637,7 +10473,13 @@
       <c r="R141" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S141" t="inlineStr">
+      <c r="S141" t="n">
+        <v>0</v>
+      </c>
+      <c r="T141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9704,9 +10546,15 @@
       <c r="R142" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="S142" t="inlineStr">
-        <is>
-          <t>3261</t>
+      <c r="S142" t="n">
+        <v>3261</v>
+      </c>
+      <c r="T142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U142" t="inlineStr">
+        <is>
+          <t>3245</t>
         </is>
       </c>
     </row>
@@ -9771,7 +10619,13 @@
       <c r="R143" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S143" t="inlineStr">
+      <c r="S143" t="n">
+        <v>0</v>
+      </c>
+      <c r="T143" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9838,9 +10692,15 @@
       <c r="R144" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S144" t="inlineStr">
-        <is>
-          <t>3520</t>
+      <c r="S144" t="n">
+        <v>3520</v>
+      </c>
+      <c r="T144" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U144" t="inlineStr">
+        <is>
+          <t>3789</t>
         </is>
       </c>
     </row>
@@ -9905,7 +10765,13 @@
       <c r="R145" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S145" t="inlineStr">
+      <c r="S145" t="n">
+        <v>0</v>
+      </c>
+      <c r="T145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9972,7 +10838,13 @@
       <c r="R146" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S146" t="inlineStr">
+      <c r="S146" t="n">
+        <v>0</v>
+      </c>
+      <c r="T146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10039,7 +10911,13 @@
       <c r="R147" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="S147" t="inlineStr">
+      <c r="S147" t="n">
+        <v>2148</v>
+      </c>
+      <c r="T147" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U147" t="inlineStr">
         <is>
           <t>2148</t>
         </is>
@@ -10106,7 +10984,13 @@
       <c r="R148" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S148" t="inlineStr">
+      <c r="S148" t="n">
+        <v>0</v>
+      </c>
+      <c r="T148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10173,7 +11057,13 @@
       <c r="R149" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S149" t="inlineStr">
+      <c r="S149" t="n">
+        <v>0</v>
+      </c>
+      <c r="T149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10240,7 +11130,13 @@
       <c r="R150" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S150" t="inlineStr">
+      <c r="S150" t="n">
+        <v>2604</v>
+      </c>
+      <c r="T150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U150" t="inlineStr">
         <is>
           <t>2604</t>
         </is>
@@ -10307,7 +11203,13 @@
       <c r="R151" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S151" t="inlineStr">
+      <c r="S151" t="n">
+        <v>0</v>
+      </c>
+      <c r="T151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10374,7 +11276,13 @@
       <c r="R152" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S152" t="inlineStr">
+      <c r="S152" t="n">
+        <v>0</v>
+      </c>
+      <c r="T152" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10441,7 +11349,13 @@
       <c r="R153" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S153" t="inlineStr">
+      <c r="S153" t="n">
+        <v>0</v>
+      </c>
+      <c r="T153" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10508,9 +11422,15 @@
       <c r="R154" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S154" t="inlineStr">
-        <is>
-          <t>2921</t>
+      <c r="S154" t="n">
+        <v>2921</v>
+      </c>
+      <c r="T154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U154" t="inlineStr">
+        <is>
+          <t>2915</t>
         </is>
       </c>
     </row>
@@ -10575,7 +11495,13 @@
       <c r="R155" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S155" t="inlineStr">
+      <c r="S155" t="n">
+        <v>0</v>
+      </c>
+      <c r="T155" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10642,7 +11568,13 @@
       <c r="R156" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S156" t="inlineStr">
+      <c r="S156" t="n">
+        <v>0</v>
+      </c>
+      <c r="T156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10709,7 +11641,13 @@
       <c r="R157" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S157" t="inlineStr">
+      <c r="S157" t="n">
+        <v>0</v>
+      </c>
+      <c r="T157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10776,9 +11714,15 @@
       <c r="R158" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S158" t="inlineStr">
-        <is>
-          <t>3103</t>
+      <c r="S158" t="n">
+        <v>3103</v>
+      </c>
+      <c r="T158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U158" t="inlineStr">
+        <is>
+          <t>3133</t>
         </is>
       </c>
     </row>
@@ -10824,6 +11768,8 @@
       <c r="Q159" t="inlineStr"/>
       <c r="R159" s="2" t="inlineStr"/>
       <c r="S159" t="inlineStr"/>
+      <c r="T159" s="2" t="inlineStr"/>
+      <c r="U159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="n">
@@ -10880,9 +11826,15 @@
       <c r="R160" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="S160" t="inlineStr">
-        <is>
-          <t>4687</t>
+      <c r="S160" t="n">
+        <v>4687</v>
+      </c>
+      <c r="T160" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="U160" t="inlineStr">
+        <is>
+          <t>4750</t>
         </is>
       </c>
     </row>
@@ -10920,6 +11872,8 @@
       <c r="Q161" t="inlineStr"/>
       <c r="R161" s="2" t="inlineStr"/>
       <c r="S161" t="inlineStr"/>
+      <c r="T161" s="2" t="inlineStr"/>
+      <c r="U161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="n">
@@ -10976,9 +11930,15 @@
       <c r="R162" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="S162" t="inlineStr">
-        <is>
-          <t>3774</t>
+      <c r="S162" t="n">
+        <v>3774</v>
+      </c>
+      <c r="T162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U162" t="inlineStr">
+        <is>
+          <t>3865</t>
         </is>
       </c>
     </row>
@@ -11037,9 +11997,15 @@
       <c r="R163" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="S163" t="inlineStr">
-        <is>
-          <t>2957</t>
+      <c r="S163" t="n">
+        <v>2957</v>
+      </c>
+      <c r="T163" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U163" t="inlineStr">
+        <is>
+          <t>3226</t>
         </is>
       </c>
     </row>
@@ -11094,17 +12060,15 @@
       <c r="R164" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="S164" t="inlineStr">
-        <is>
-          <t>3521</t>
-        </is>
-      </c>
+      <c r="S164" t="n">
+        <v>3521</v>
+      </c>
+      <c r="T164" s="2" t="inlineStr"/>
+      <c r="U164" t="inlineStr"/>
     </row>
     <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>138176</t>
-        </is>
+      <c r="A165" t="n">
+        <v>138176</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
@@ -11133,17 +12097,21 @@
       <c r="R165" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="S165" t="inlineStr">
-        <is>
-          <t>6773</t>
+      <c r="S165" t="n">
+        <v>6773</v>
+      </c>
+      <c r="T165" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="U165" t="inlineStr">
+        <is>
+          <t>7087</t>
         </is>
       </c>
     </row>
     <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>32929656</t>
-        </is>
+      <c r="A166" t="n">
+        <v>32929656</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -11172,9 +12140,138 @@
       <c r="R166" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="S166" t="inlineStr">
-        <is>
-          <t>4508</t>
+      <c r="S166" t="n">
+        <v>4508</v>
+      </c>
+      <c r="T166" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="U166" t="inlineStr">
+        <is>
+          <t>4588</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>49000199</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>SlipperyForester5672</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr"/>
+      <c r="D167" t="inlineStr"/>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F167" s="2" t="inlineStr"/>
+      <c r="G167" t="inlineStr"/>
+      <c r="H167" s="2" t="inlineStr"/>
+      <c r="I167" t="inlineStr"/>
+      <c r="J167" s="2" t="inlineStr"/>
+      <c r="K167" t="inlineStr"/>
+      <c r="L167" s="2" t="inlineStr"/>
+      <c r="M167" t="inlineStr"/>
+      <c r="N167" s="2" t="inlineStr"/>
+      <c r="O167" t="inlineStr"/>
+      <c r="P167" s="2" t="inlineStr"/>
+      <c r="Q167" t="inlineStr"/>
+      <c r="R167" s="2" t="inlineStr"/>
+      <c r="S167" t="inlineStr"/>
+      <c r="T167" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="U167" t="inlineStr">
+        <is>
+          <t>1066</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>52157846</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Hamza</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr"/>
+      <c r="D168" t="inlineStr"/>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F168" s="2" t="inlineStr"/>
+      <c r="G168" t="inlineStr"/>
+      <c r="H168" s="2" t="inlineStr"/>
+      <c r="I168" t="inlineStr"/>
+      <c r="J168" s="2" t="inlineStr"/>
+      <c r="K168" t="inlineStr"/>
+      <c r="L168" s="2" t="inlineStr"/>
+      <c r="M168" t="inlineStr"/>
+      <c r="N168" s="2" t="inlineStr"/>
+      <c r="O168" t="inlineStr"/>
+      <c r="P168" s="2" t="inlineStr"/>
+      <c r="Q168" t="inlineStr"/>
+      <c r="R168" s="2" t="inlineStr"/>
+      <c r="S168" t="inlineStr"/>
+      <c r="T168" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="U168" t="inlineStr">
+        <is>
+          <t>2776</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>59081265</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>爬楼梯</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr"/>
+      <c r="D169" t="inlineStr"/>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F169" s="2" t="inlineStr"/>
+      <c r="G169" t="inlineStr"/>
+      <c r="H169" s="2" t="inlineStr"/>
+      <c r="I169" t="inlineStr"/>
+      <c r="J169" s="2" t="inlineStr"/>
+      <c r="K169" t="inlineStr"/>
+      <c r="L169" s="2" t="inlineStr"/>
+      <c r="M169" t="inlineStr"/>
+      <c r="N169" s="2" t="inlineStr"/>
+      <c r="O169" t="inlineStr"/>
+      <c r="P169" s="2" t="inlineStr"/>
+      <c r="Q169" t="inlineStr"/>
+      <c r="R169" s="2" t="inlineStr"/>
+      <c r="S169" t="inlineStr"/>
+      <c r="T169" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U169" t="inlineStr">
+        <is>
+          <t>1305</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-24 11:30:51
</commit_message>
<xml_diff>
--- a/Season_Attack/86.xlsx
+++ b/Season_Attack/86.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U169"/>
+  <dimension ref="A1:W170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,6 +496,16 @@
           <t>03-22_0</t>
         </is>
       </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>03-23_A</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>03-23_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -564,9 +574,15 @@
       <c r="T2" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>3530</t>
+      <c r="U2" t="n">
+        <v>3530</v>
+      </c>
+      <c r="V2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>3571</t>
         </is>
       </c>
     </row>
@@ -625,9 +641,15 @@
       <c r="T3" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>6514</t>
+      <c r="U3" t="n">
+        <v>6514</v>
+      </c>
+      <c r="V3" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>6847</t>
         </is>
       </c>
     </row>
@@ -698,9 +720,15 @@
       <c r="T4" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>6431</t>
+      <c r="U4" t="n">
+        <v>6431</v>
+      </c>
+      <c r="V4" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>6697</t>
         </is>
       </c>
     </row>
@@ -771,9 +799,15 @@
       <c r="T5" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>6509</t>
+      <c r="U5" t="n">
+        <v>6509</v>
+      </c>
+      <c r="V5" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>6852</t>
         </is>
       </c>
     </row>
@@ -844,9 +878,15 @@
       <c r="T6" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>5974</t>
+      <c r="U6" t="n">
+        <v>5974</v>
+      </c>
+      <c r="V6" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>6367</t>
         </is>
       </c>
     </row>
@@ -917,9 +957,15 @@
       <c r="T7" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>6671</t>
+      <c r="U7" t="n">
+        <v>6671</v>
+      </c>
+      <c r="V7" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>6961</t>
         </is>
       </c>
     </row>
@@ -990,9 +1036,15 @@
       <c r="T8" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>5619</t>
+      <c r="U8" t="n">
+        <v>5619</v>
+      </c>
+      <c r="V8" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>5753</t>
         </is>
       </c>
     </row>
@@ -1063,9 +1115,15 @@
       <c r="T9" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>5809</t>
+      <c r="U9" t="n">
+        <v>5809</v>
+      </c>
+      <c r="V9" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>6196</t>
         </is>
       </c>
     </row>
@@ -1136,9 +1194,15 @@
       <c r="T10" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="U10" t="inlineStr">
-        <is>
-          <t>6645</t>
+      <c r="U10" t="n">
+        <v>6645</v>
+      </c>
+      <c r="V10" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>7028</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1225,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F11" s="2" t="n">
@@ -1193,9 +1257,15 @@
       <c r="T11" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U11" t="inlineStr">
-        <is>
-          <t>5738</t>
+      <c r="U11" t="n">
+        <v>5738</v>
+      </c>
+      <c r="V11" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>5899</t>
         </is>
       </c>
     </row>
@@ -1266,7 +1336,13 @@
       <c r="T12" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U12" t="inlineStr">
+      <c r="U12" t="n">
+        <v>3336</v>
+      </c>
+      <c r="V12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" t="inlineStr">
         <is>
           <t>3336</t>
         </is>
@@ -1339,9 +1415,15 @@
       <c r="T13" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="U13" t="inlineStr">
-        <is>
-          <t>6758</t>
+      <c r="U13" t="n">
+        <v>6758</v>
+      </c>
+      <c r="V13" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>7090</t>
         </is>
       </c>
     </row>
@@ -1412,9 +1494,15 @@
       <c r="T14" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="U14" t="inlineStr">
-        <is>
-          <t>5870</t>
+      <c r="U14" t="n">
+        <v>5870</v>
+      </c>
+      <c r="V14" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>6149</t>
         </is>
       </c>
     </row>
@@ -1469,9 +1557,15 @@
       <c r="T15" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="U15" t="inlineStr">
-        <is>
-          <t>6205</t>
+      <c r="U15" t="n">
+        <v>6205</v>
+      </c>
+      <c r="V15" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>6521</t>
         </is>
       </c>
     </row>
@@ -1542,9 +1636,15 @@
       <c r="T16" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U16" t="inlineStr">
-        <is>
-          <t>5151</t>
+      <c r="U16" t="n">
+        <v>5151</v>
+      </c>
+      <c r="V16" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>5350</t>
         </is>
       </c>
     </row>
@@ -1615,9 +1715,15 @@
       <c r="T17" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="U17" t="inlineStr">
-        <is>
-          <t>5208</t>
+      <c r="U17" t="n">
+        <v>5208</v>
+      </c>
+      <c r="V17" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>5465</t>
         </is>
       </c>
     </row>
@@ -1688,9 +1794,15 @@
       <c r="T18" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="U18" t="inlineStr">
-        <is>
-          <t>6072</t>
+      <c r="U18" t="n">
+        <v>6072</v>
+      </c>
+      <c r="V18" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>6346</t>
         </is>
       </c>
     </row>
@@ -1745,9 +1857,15 @@
       <c r="T19" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U19" t="inlineStr">
-        <is>
-          <t>6972</t>
+      <c r="U19" t="n">
+        <v>6972</v>
+      </c>
+      <c r="V19" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>7304</t>
         </is>
       </c>
     </row>
@@ -1818,7 +1936,13 @@
       <c r="T20" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U20" t="inlineStr">
+      <c r="U20" t="n">
+        <v>4932</v>
+      </c>
+      <c r="V20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W20" t="inlineStr">
         <is>
           <t>4932</t>
         </is>
@@ -1891,9 +2015,15 @@
       <c r="T21" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U21" t="inlineStr">
-        <is>
-          <t>6282</t>
+      <c r="U21" t="n">
+        <v>6282</v>
+      </c>
+      <c r="V21" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>6545</t>
         </is>
       </c>
     </row>
@@ -1964,9 +2094,15 @@
       <c r="T22" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="U22" t="inlineStr">
-        <is>
-          <t>5754</t>
+      <c r="U22" t="n">
+        <v>5754</v>
+      </c>
+      <c r="V22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>5767</t>
         </is>
       </c>
     </row>
@@ -2037,9 +2173,15 @@
       <c r="T23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U23" t="inlineStr">
-        <is>
-          <t>6101</t>
+      <c r="U23" t="n">
+        <v>6101</v>
+      </c>
+      <c r="V23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>6469</t>
         </is>
       </c>
     </row>
@@ -2110,7 +2252,13 @@
       <c r="T24" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U24" t="inlineStr">
+      <c r="U24" t="n">
+        <v>0</v>
+      </c>
+      <c r="V24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2183,9 +2331,15 @@
       <c r="T25" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U25" t="inlineStr">
-        <is>
-          <t>2673</t>
+      <c r="U25" t="n">
+        <v>2673</v>
+      </c>
+      <c r="V25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>2689</t>
         </is>
       </c>
     </row>
@@ -2236,9 +2390,15 @@
       <c r="T26" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="U26" t="inlineStr">
-        <is>
-          <t>6383</t>
+      <c r="U26" t="n">
+        <v>6383</v>
+      </c>
+      <c r="V26" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>6610</t>
         </is>
       </c>
     </row>
@@ -2289,9 +2449,15 @@
       <c r="T27" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="U27" t="inlineStr">
-        <is>
-          <t>5660</t>
+      <c r="U27" t="n">
+        <v>5660</v>
+      </c>
+      <c r="V27" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>6063</t>
         </is>
       </c>
     </row>
@@ -2362,9 +2528,15 @@
       <c r="T28" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U28" t="inlineStr">
-        <is>
-          <t>6532</t>
+      <c r="U28" t="n">
+        <v>6532</v>
+      </c>
+      <c r="V28" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>6988</t>
         </is>
       </c>
     </row>
@@ -2415,9 +2587,15 @@
       <c r="T29" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U29" t="inlineStr">
-        <is>
-          <t>5568</t>
+      <c r="U29" t="n">
+        <v>5568</v>
+      </c>
+      <c r="V29" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>6085</t>
         </is>
       </c>
     </row>
@@ -2488,9 +2666,15 @@
       <c r="T30" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="U30" t="inlineStr">
-        <is>
-          <t>5255</t>
+      <c r="U30" t="n">
+        <v>5255</v>
+      </c>
+      <c r="V30" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>5459</t>
         </is>
       </c>
     </row>
@@ -2561,9 +2745,15 @@
       <c r="T31" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="U31" t="inlineStr">
-        <is>
-          <t>6748</t>
+      <c r="U31" t="n">
+        <v>6748</v>
+      </c>
+      <c r="V31" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>7088</t>
         </is>
       </c>
     </row>
@@ -2586,7 +2776,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F32" s="5" t="n">
@@ -2618,9 +2808,15 @@
       <c r="T32" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="U32" t="inlineStr">
-        <is>
-          <t>4509</t>
+      <c r="U32" t="n">
+        <v>4509</v>
+      </c>
+      <c r="V32" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>4674</t>
         </is>
       </c>
     </row>
@@ -2691,9 +2887,15 @@
       <c r="T33" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="U33" t="inlineStr">
-        <is>
-          <t>5929</t>
+      <c r="U33" t="n">
+        <v>5929</v>
+      </c>
+      <c r="V33" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>6223</t>
         </is>
       </c>
     </row>
@@ -2764,9 +2966,15 @@
       <c r="T34" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="U34" t="inlineStr">
-        <is>
-          <t>6470</t>
+      <c r="U34" t="n">
+        <v>6470</v>
+      </c>
+      <c r="V34" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>6655</t>
         </is>
       </c>
     </row>
@@ -2837,9 +3045,15 @@
       <c r="T35" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U35" t="inlineStr">
-        <is>
-          <t>5921</t>
+      <c r="U35" t="n">
+        <v>5921</v>
+      </c>
+      <c r="V35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>5927</t>
         </is>
       </c>
     </row>
@@ -2890,9 +3104,15 @@
       <c r="T36" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U36" t="inlineStr">
-        <is>
-          <t>5087</t>
+      <c r="U36" t="n">
+        <v>5087</v>
+      </c>
+      <c r="V36" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>5257</t>
         </is>
       </c>
     </row>
@@ -2963,9 +3183,15 @@
       <c r="T37" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="U37" t="inlineStr">
-        <is>
-          <t>6054</t>
+      <c r="U37" t="n">
+        <v>6054</v>
+      </c>
+      <c r="V37" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>6236</t>
         </is>
       </c>
     </row>
@@ -2988,7 +3214,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F38" s="2" t="n">
@@ -3036,9 +3262,15 @@
       <c r="T38" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="U38" t="inlineStr">
-        <is>
-          <t>5716</t>
+      <c r="U38" t="n">
+        <v>5716</v>
+      </c>
+      <c r="V38" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="W38" t="inlineStr">
+        <is>
+          <t>5765</t>
         </is>
       </c>
     </row>
@@ -3109,9 +3341,15 @@
       <c r="T39" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="U39" t="inlineStr">
-        <is>
-          <t>6398</t>
+      <c r="U39" t="n">
+        <v>6398</v>
+      </c>
+      <c r="V39" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>6652</t>
         </is>
       </c>
     </row>
@@ -3182,9 +3420,15 @@
       <c r="T40" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="U40" t="inlineStr">
-        <is>
-          <t>6870</t>
+      <c r="U40" t="n">
+        <v>6870</v>
+      </c>
+      <c r="V40" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="W40" t="inlineStr">
+        <is>
+          <t>7082</t>
         </is>
       </c>
     </row>
@@ -3255,9 +3499,15 @@
       <c r="T41" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U41" t="inlineStr">
-        <is>
-          <t>6095</t>
+      <c r="U41" t="n">
+        <v>6095</v>
+      </c>
+      <c r="V41" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="W41" t="inlineStr">
+        <is>
+          <t>6248</t>
         </is>
       </c>
     </row>
@@ -3328,9 +3578,15 @@
       <c r="T42" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U42" t="inlineStr">
-        <is>
-          <t>6044</t>
+      <c r="U42" t="n">
+        <v>6044</v>
+      </c>
+      <c r="V42" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W42" t="inlineStr">
+        <is>
+          <t>6315</t>
         </is>
       </c>
     </row>
@@ -3401,9 +3657,15 @@
       <c r="T43" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="U43" t="inlineStr">
-        <is>
-          <t>5417</t>
+      <c r="U43" t="n">
+        <v>5417</v>
+      </c>
+      <c r="V43" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="W43" t="inlineStr">
+        <is>
+          <t>5606</t>
         </is>
       </c>
     </row>
@@ -3474,9 +3736,15 @@
       <c r="T44" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="U44" t="inlineStr">
-        <is>
-          <t>5597</t>
+      <c r="U44" t="n">
+        <v>5597</v>
+      </c>
+      <c r="V44" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="W44" t="inlineStr">
+        <is>
+          <t>5947</t>
         </is>
       </c>
     </row>
@@ -3547,7 +3815,13 @@
       <c r="T45" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U45" t="inlineStr">
+      <c r="U45" t="n">
+        <v>5007</v>
+      </c>
+      <c r="V45" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W45" t="inlineStr">
         <is>
           <t>5007</t>
         </is>
@@ -3620,9 +3894,15 @@
       <c r="T46" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="U46" t="inlineStr">
-        <is>
-          <t>6370</t>
+      <c r="U46" t="n">
+        <v>6370</v>
+      </c>
+      <c r="V46" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="W46" t="inlineStr">
+        <is>
+          <t>6703</t>
         </is>
       </c>
     </row>
@@ -3693,9 +3973,15 @@
       <c r="T47" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="U47" t="inlineStr">
-        <is>
-          <t>5406</t>
+      <c r="U47" t="n">
+        <v>5406</v>
+      </c>
+      <c r="V47" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="W47" t="inlineStr">
+        <is>
+          <t>5442</t>
         </is>
       </c>
     </row>
@@ -3766,7 +4052,13 @@
       <c r="T48" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U48" t="inlineStr">
+      <c r="U48" t="n">
+        <v>2548</v>
+      </c>
+      <c r="V48" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W48" t="inlineStr">
         <is>
           <t>2548</t>
         </is>
@@ -3806,6 +4098,8 @@
       <c r="S49" t="inlineStr"/>
       <c r="T49" s="2" t="inlineStr"/>
       <c r="U49" t="inlineStr"/>
+      <c r="V49" s="2" t="inlineStr"/>
+      <c r="W49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -3874,7 +4168,13 @@
       <c r="T50" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U50" t="inlineStr">
+      <c r="U50" t="n">
+        <v>0</v>
+      </c>
+      <c r="V50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W50" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3947,9 +4247,15 @@
       <c r="T51" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U51" t="inlineStr">
-        <is>
-          <t>2818</t>
+      <c r="U51" t="n">
+        <v>2818</v>
+      </c>
+      <c r="V51" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="W51" t="inlineStr">
+        <is>
+          <t>2849</t>
         </is>
       </c>
     </row>
@@ -4020,9 +4326,15 @@
       <c r="T52" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U52" t="inlineStr">
-        <is>
-          <t>3184</t>
+      <c r="U52" t="n">
+        <v>3184</v>
+      </c>
+      <c r="V52" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="W52" t="inlineStr">
+        <is>
+          <t>3300</t>
         </is>
       </c>
     </row>
@@ -4093,9 +4405,15 @@
       <c r="T53" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="U53" t="inlineStr">
-        <is>
-          <t>5797</t>
+      <c r="U53" t="n">
+        <v>5797</v>
+      </c>
+      <c r="V53" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="W53" t="inlineStr">
+        <is>
+          <t>6032</t>
         </is>
       </c>
     </row>
@@ -4166,9 +4484,15 @@
       <c r="T54" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U54" t="inlineStr">
-        <is>
-          <t>4993</t>
+      <c r="U54" t="n">
+        <v>4993</v>
+      </c>
+      <c r="V54" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="W54" t="inlineStr">
+        <is>
+          <t>5055</t>
         </is>
       </c>
     </row>
@@ -4239,9 +4563,15 @@
       <c r="T55" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U55" t="inlineStr">
-        <is>
-          <t>5140</t>
+      <c r="U55" t="n">
+        <v>5140</v>
+      </c>
+      <c r="V55" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W55" t="inlineStr">
+        <is>
+          <t>5222</t>
         </is>
       </c>
     </row>
@@ -4312,9 +4642,15 @@
       <c r="T56" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U56" t="inlineStr">
-        <is>
-          <t>5728</t>
+      <c r="U56" t="n">
+        <v>5728</v>
+      </c>
+      <c r="V56" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W56" t="inlineStr">
+        <is>
+          <t>5950</t>
         </is>
       </c>
     </row>
@@ -4385,9 +4721,15 @@
       <c r="T57" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="U57" t="inlineStr">
-        <is>
-          <t>5062</t>
+      <c r="U57" t="n">
+        <v>5062</v>
+      </c>
+      <c r="V57" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="W57" t="inlineStr">
+        <is>
+          <t>5193</t>
         </is>
       </c>
     </row>
@@ -4458,9 +4800,15 @@
       <c r="T58" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="U58" t="inlineStr">
-        <is>
-          <t>4845</t>
+      <c r="U58" t="n">
+        <v>4845</v>
+      </c>
+      <c r="V58" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="W58" t="inlineStr">
+        <is>
+          <t>4882</t>
         </is>
       </c>
     </row>
@@ -4531,7 +4879,13 @@
       <c r="T59" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U59" t="inlineStr">
+      <c r="U59" t="n">
+        <v>0</v>
+      </c>
+      <c r="V59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W59" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4604,9 +4958,15 @@
       <c r="T60" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="U60" t="inlineStr">
-        <is>
-          <t>5878</t>
+      <c r="U60" t="n">
+        <v>5878</v>
+      </c>
+      <c r="V60" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="W60" t="inlineStr">
+        <is>
+          <t>6147</t>
         </is>
       </c>
     </row>
@@ -4677,7 +5037,13 @@
       <c r="T61" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U61" t="inlineStr">
+      <c r="U61" t="n">
+        <v>2758</v>
+      </c>
+      <c r="V61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W61" t="inlineStr">
         <is>
           <t>2758</t>
         </is>
@@ -4750,9 +5116,15 @@
       <c r="T62" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U62" t="inlineStr">
-        <is>
-          <t>3237</t>
+      <c r="U62" t="n">
+        <v>3237</v>
+      </c>
+      <c r="V62" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W62" t="inlineStr">
+        <is>
+          <t>3230</t>
         </is>
       </c>
     </row>
@@ -4823,9 +5195,15 @@
       <c r="T63" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="U63" t="inlineStr">
-        <is>
-          <t>5476</t>
+      <c r="U63" t="n">
+        <v>5476</v>
+      </c>
+      <c r="V63" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="W63" t="inlineStr">
+        <is>
+          <t>5677</t>
         </is>
       </c>
     </row>
@@ -4896,9 +5274,15 @@
       <c r="T64" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="U64" t="inlineStr">
-        <is>
-          <t>6297</t>
+      <c r="U64" t="n">
+        <v>6297</v>
+      </c>
+      <c r="V64" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W64" t="inlineStr">
+        <is>
+          <t>6662</t>
         </is>
       </c>
     </row>
@@ -4969,9 +5353,15 @@
       <c r="T65" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="U65" t="inlineStr">
-        <is>
-          <t>3760</t>
+      <c r="U65" t="n">
+        <v>3760</v>
+      </c>
+      <c r="V65" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="W65" t="inlineStr">
+        <is>
+          <t>4237</t>
         </is>
       </c>
     </row>
@@ -5042,9 +5432,15 @@
       <c r="T66" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U66" t="inlineStr">
-        <is>
-          <t>5103</t>
+      <c r="U66" t="n">
+        <v>5103</v>
+      </c>
+      <c r="V66" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="W66" t="inlineStr">
+        <is>
+          <t>5224</t>
         </is>
       </c>
     </row>
@@ -5115,9 +5511,15 @@
       <c r="T67" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U67" t="inlineStr">
-        <is>
-          <t>3924</t>
+      <c r="U67" t="n">
+        <v>3924</v>
+      </c>
+      <c r="V67" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="W67" t="inlineStr">
+        <is>
+          <t>4167</t>
         </is>
       </c>
     </row>
@@ -5188,7 +5590,13 @@
       <c r="T68" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U68" t="inlineStr">
+      <c r="U68" t="n">
+        <v>0</v>
+      </c>
+      <c r="V68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5261,9 +5669,15 @@
       <c r="T69" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U69" t="inlineStr">
-        <is>
-          <t>4297</t>
+      <c r="U69" t="n">
+        <v>4297</v>
+      </c>
+      <c r="V69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W69" t="inlineStr">
+        <is>
+          <t>4329</t>
         </is>
       </c>
     </row>
@@ -5334,9 +5748,15 @@
       <c r="T70" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U70" t="inlineStr">
-        <is>
-          <t>4985</t>
+      <c r="U70" t="n">
+        <v>4985</v>
+      </c>
+      <c r="V70" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W70" t="inlineStr">
+        <is>
+          <t>5098</t>
         </is>
       </c>
     </row>
@@ -5407,9 +5827,15 @@
       <c r="T71" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U71" t="inlineStr">
-        <is>
-          <t>3709</t>
+      <c r="U71" t="n">
+        <v>3709</v>
+      </c>
+      <c r="V71" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="W71" t="inlineStr">
+        <is>
+          <t>3914</t>
         </is>
       </c>
     </row>
@@ -5480,9 +5906,15 @@
       <c r="T72" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="U72" t="inlineStr">
-        <is>
-          <t>4778</t>
+      <c r="U72" t="n">
+        <v>4778</v>
+      </c>
+      <c r="V72" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="W72" t="inlineStr">
+        <is>
+          <t>4904</t>
         </is>
       </c>
     </row>
@@ -5553,9 +5985,15 @@
       <c r="T73" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U73" t="inlineStr">
-        <is>
-          <t>5589</t>
+      <c r="U73" t="n">
+        <v>5589</v>
+      </c>
+      <c r="V73" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="W73" t="inlineStr">
+        <is>
+          <t>5680</t>
         </is>
       </c>
     </row>
@@ -5626,7 +6064,13 @@
       <c r="T74" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U74" t="inlineStr">
+      <c r="U74" t="n">
+        <v>0</v>
+      </c>
+      <c r="V74" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5699,7 +6143,13 @@
       <c r="T75" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U75" t="inlineStr">
+      <c r="U75" t="n">
+        <v>0</v>
+      </c>
+      <c r="V75" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5772,9 +6222,15 @@
       <c r="T76" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="U76" t="inlineStr">
-        <is>
-          <t>5560</t>
+      <c r="U76" t="n">
+        <v>5560</v>
+      </c>
+      <c r="V76" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="W76" t="inlineStr">
+        <is>
+          <t>5701</t>
         </is>
       </c>
     </row>
@@ -5845,7 +6301,13 @@
       <c r="T77" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U77" t="inlineStr">
+      <c r="U77" t="n">
+        <v>0</v>
+      </c>
+      <c r="V77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W77" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5918,9 +6380,15 @@
       <c r="T78" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="U78" t="inlineStr">
-        <is>
-          <t>5303</t>
+      <c r="U78" t="n">
+        <v>5303</v>
+      </c>
+      <c r="V78" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="W78" t="inlineStr">
+        <is>
+          <t>5434</t>
         </is>
       </c>
     </row>
@@ -5991,9 +6459,15 @@
       <c r="T79" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U79" t="inlineStr">
-        <is>
-          <t>3331</t>
+      <c r="U79" t="n">
+        <v>3331</v>
+      </c>
+      <c r="V79" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="W79" t="inlineStr">
+        <is>
+          <t>3524</t>
         </is>
       </c>
     </row>
@@ -6031,6 +6505,8 @@
       <c r="S80" t="inlineStr"/>
       <c r="T80" s="2" t="inlineStr"/>
       <c r="U80" t="inlineStr"/>
+      <c r="V80" s="2" t="inlineStr"/>
+      <c r="W80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -6099,9 +6575,15 @@
       <c r="T81" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U81" t="inlineStr">
-        <is>
-          <t>5523</t>
+      <c r="U81" t="n">
+        <v>5523</v>
+      </c>
+      <c r="V81" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W81" t="inlineStr">
+        <is>
+          <t>5654</t>
         </is>
       </c>
     </row>
@@ -6172,9 +6654,15 @@
       <c r="T82" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="U82" t="inlineStr">
-        <is>
-          <t>5221</t>
+      <c r="U82" t="n">
+        <v>5221</v>
+      </c>
+      <c r="V82" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="W82" t="inlineStr">
+        <is>
+          <t>5463</t>
         </is>
       </c>
     </row>
@@ -6245,9 +6733,15 @@
       <c r="T83" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U83" t="inlineStr">
-        <is>
-          <t>5023</t>
+      <c r="U83" t="n">
+        <v>5023</v>
+      </c>
+      <c r="V83" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W83" t="inlineStr">
+        <is>
+          <t>5230</t>
         </is>
       </c>
     </row>
@@ -6318,9 +6812,15 @@
       <c r="T84" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U84" t="inlineStr">
-        <is>
-          <t>4776</t>
+      <c r="U84" t="n">
+        <v>4776</v>
+      </c>
+      <c r="V84" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W84" t="inlineStr">
+        <is>
+          <t>4880</t>
         </is>
       </c>
     </row>
@@ -6391,9 +6891,15 @@
       <c r="T85" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U85" t="inlineStr">
-        <is>
-          <t>4725</t>
+      <c r="U85" t="n">
+        <v>4725</v>
+      </c>
+      <c r="V85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W85" t="inlineStr">
+        <is>
+          <t>4705</t>
         </is>
       </c>
     </row>
@@ -6464,9 +6970,15 @@
       <c r="T86" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U86" t="inlineStr">
-        <is>
-          <t>4392</t>
+      <c r="U86" t="n">
+        <v>4392</v>
+      </c>
+      <c r="V86" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W86" t="inlineStr">
+        <is>
+          <t>4384</t>
         </is>
       </c>
     </row>
@@ -6537,9 +7049,15 @@
       <c r="T87" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U87" t="inlineStr">
-        <is>
-          <t>5247</t>
+      <c r="U87" t="n">
+        <v>5247</v>
+      </c>
+      <c r="V87" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W87" t="inlineStr">
+        <is>
+          <t>5449</t>
         </is>
       </c>
     </row>
@@ -6610,9 +7128,15 @@
       <c r="T88" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U88" t="inlineStr">
-        <is>
-          <t>3804</t>
+      <c r="U88" t="n">
+        <v>3804</v>
+      </c>
+      <c r="V88" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W88" t="inlineStr">
+        <is>
+          <t>3973</t>
         </is>
       </c>
     </row>
@@ -6683,9 +7207,15 @@
       <c r="T89" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U89" t="inlineStr">
-        <is>
-          <t>4133</t>
+      <c r="U89" t="n">
+        <v>4133</v>
+      </c>
+      <c r="V89" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="W89" t="inlineStr">
+        <is>
+          <t>4244</t>
         </is>
       </c>
     </row>
@@ -6756,9 +7286,15 @@
       <c r="T90" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U90" t="inlineStr">
-        <is>
-          <t>3127</t>
+      <c r="U90" t="n">
+        <v>3127</v>
+      </c>
+      <c r="V90" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W90" t="inlineStr">
+        <is>
+          <t>3116</t>
         </is>
       </c>
     </row>
@@ -6829,9 +7365,15 @@
       <c r="T91" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="U91" t="inlineStr">
-        <is>
-          <t>4035</t>
+      <c r="U91" t="n">
+        <v>4035</v>
+      </c>
+      <c r="V91" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="W91" t="inlineStr">
+        <is>
+          <t>4053</t>
         </is>
       </c>
     </row>
@@ -6902,7 +7444,13 @@
       <c r="T92" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U92" t="inlineStr">
+      <c r="U92" t="n">
+        <v>0</v>
+      </c>
+      <c r="V92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6975,9 +7523,15 @@
       <c r="T93" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="U93" t="inlineStr">
-        <is>
-          <t>4095</t>
+      <c r="U93" t="n">
+        <v>4095</v>
+      </c>
+      <c r="V93" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="W93" t="inlineStr">
+        <is>
+          <t>4022</t>
         </is>
       </c>
     </row>
@@ -7048,9 +7602,15 @@
       <c r="T94" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U94" t="inlineStr">
-        <is>
-          <t>2592</t>
+      <c r="U94" t="n">
+        <v>2592</v>
+      </c>
+      <c r="V94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W94" t="inlineStr">
+        <is>
+          <t>2608</t>
         </is>
       </c>
     </row>
@@ -7121,9 +7681,15 @@
       <c r="T95" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U95" t="inlineStr">
-        <is>
-          <t>4317</t>
+      <c r="U95" t="n">
+        <v>4317</v>
+      </c>
+      <c r="V95" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="W95" t="inlineStr">
+        <is>
+          <t>4367</t>
         </is>
       </c>
     </row>
@@ -7194,9 +7760,15 @@
       <c r="T96" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U96" t="inlineStr">
-        <is>
-          <t>2623</t>
+      <c r="U96" t="n">
+        <v>2623</v>
+      </c>
+      <c r="V96" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="W96" t="inlineStr">
+        <is>
+          <t>2648</t>
         </is>
       </c>
     </row>
@@ -7267,9 +7839,15 @@
       <c r="T97" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U97" t="inlineStr">
-        <is>
-          <t>2213</t>
+      <c r="U97" t="n">
+        <v>2213</v>
+      </c>
+      <c r="V97" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W97" t="inlineStr">
+        <is>
+          <t>2207</t>
         </is>
       </c>
     </row>
@@ -7340,9 +7918,15 @@
       <c r="T98" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U98" t="inlineStr">
-        <is>
-          <t>3356</t>
+      <c r="U98" t="n">
+        <v>3356</v>
+      </c>
+      <c r="V98" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W98" t="inlineStr">
+        <is>
+          <t>3715</t>
         </is>
       </c>
     </row>
@@ -7413,9 +7997,15 @@
       <c r="T99" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U99" t="inlineStr">
-        <is>
-          <t>2507</t>
+      <c r="U99" t="n">
+        <v>2507</v>
+      </c>
+      <c r="V99" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="W99" t="inlineStr">
+        <is>
+          <t>2600</t>
         </is>
       </c>
     </row>
@@ -7486,9 +8076,15 @@
       <c r="T100" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U100" t="inlineStr">
-        <is>
-          <t>4181</t>
+      <c r="U100" t="n">
+        <v>4181</v>
+      </c>
+      <c r="V100" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="W100" t="inlineStr">
+        <is>
+          <t>4340</t>
         </is>
       </c>
     </row>
@@ -7559,9 +8155,15 @@
       <c r="T101" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U101" t="inlineStr">
-        <is>
-          <t>2356</t>
+      <c r="U101" t="n">
+        <v>2356</v>
+      </c>
+      <c r="V101" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="W101" t="inlineStr">
+        <is>
+          <t>2386</t>
         </is>
       </c>
     </row>
@@ -7632,9 +8234,15 @@
       <c r="T102" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="U102" t="inlineStr">
-        <is>
-          <t>5267</t>
+      <c r="U102" t="n">
+        <v>5267</v>
+      </c>
+      <c r="V102" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="W102" t="inlineStr">
+        <is>
+          <t>5394</t>
         </is>
       </c>
     </row>
@@ -7705,9 +8313,15 @@
       <c r="T103" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U103" t="inlineStr">
-        <is>
-          <t>4665</t>
+      <c r="U103" t="n">
+        <v>4665</v>
+      </c>
+      <c r="V103" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W103" t="inlineStr">
+        <is>
+          <t>4765</t>
         </is>
       </c>
     </row>
@@ -7778,9 +8392,15 @@
       <c r="T104" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="U104" t="inlineStr">
-        <is>
-          <t>4654</t>
+      <c r="U104" t="n">
+        <v>4654</v>
+      </c>
+      <c r="V104" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="W104" t="inlineStr">
+        <is>
+          <t>4715</t>
         </is>
       </c>
     </row>
@@ -7851,9 +8471,15 @@
       <c r="T105" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="U105" t="inlineStr">
-        <is>
-          <t>5135</t>
+      <c r="U105" t="n">
+        <v>5135</v>
+      </c>
+      <c r="V105" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="W105" t="inlineStr">
+        <is>
+          <t>5332</t>
         </is>
       </c>
     </row>
@@ -7924,9 +8550,15 @@
       <c r="T106" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="U106" t="inlineStr">
-        <is>
-          <t>4720</t>
+      <c r="U106" t="n">
+        <v>4720</v>
+      </c>
+      <c r="V106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W106" t="inlineStr">
+        <is>
+          <t>4804</t>
         </is>
       </c>
     </row>
@@ -7997,11 +8629,11 @@
       <c r="T107" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="U107" t="inlineStr">
-        <is>
-          <t>5272</t>
-        </is>
-      </c>
+      <c r="U107" t="n">
+        <v>5272</v>
+      </c>
+      <c r="V107" s="2" t="inlineStr"/>
+      <c r="W107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -8070,7 +8702,13 @@
       <c r="T108" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U108" t="inlineStr">
+      <c r="U108" t="n">
+        <v>0</v>
+      </c>
+      <c r="V108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8143,9 +8781,15 @@
       <c r="T109" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U109" t="inlineStr">
-        <is>
-          <t>3061</t>
+      <c r="U109" t="n">
+        <v>3061</v>
+      </c>
+      <c r="V109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W109" t="inlineStr">
+        <is>
+          <t>3130</t>
         </is>
       </c>
     </row>
@@ -8216,7 +8860,13 @@
       <c r="T110" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U110" t="inlineStr">
+      <c r="U110" t="n">
+        <v>0</v>
+      </c>
+      <c r="V110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W110" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8289,9 +8939,15 @@
       <c r="T111" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="U111" t="inlineStr">
-        <is>
-          <t>4596</t>
+      <c r="U111" t="n">
+        <v>4596</v>
+      </c>
+      <c r="V111" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W111" t="inlineStr">
+        <is>
+          <t>4627</t>
         </is>
       </c>
     </row>
@@ -8362,9 +9018,15 @@
       <c r="T112" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="U112" t="inlineStr">
-        <is>
-          <t>4710</t>
+      <c r="U112" t="n">
+        <v>4710</v>
+      </c>
+      <c r="V112" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="W112" t="inlineStr">
+        <is>
+          <t>4807</t>
         </is>
       </c>
     </row>
@@ -8435,9 +9097,15 @@
       <c r="T113" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U113" t="inlineStr">
-        <is>
-          <t>4024</t>
+      <c r="U113" t="n">
+        <v>4024</v>
+      </c>
+      <c r="V113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W113" t="inlineStr">
+        <is>
+          <t>4032</t>
         </is>
       </c>
     </row>
@@ -8508,9 +9176,15 @@
       <c r="T114" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U114" t="inlineStr">
-        <is>
-          <t>2660</t>
+      <c r="U114" t="n">
+        <v>2660</v>
+      </c>
+      <c r="V114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W114" t="inlineStr">
+        <is>
+          <t>2653</t>
         </is>
       </c>
     </row>
@@ -8581,9 +9255,15 @@
       <c r="T115" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U115" t="inlineStr">
-        <is>
-          <t>4443</t>
+      <c r="U115" t="n">
+        <v>4443</v>
+      </c>
+      <c r="V115" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="W115" t="inlineStr">
+        <is>
+          <t>4520</t>
         </is>
       </c>
     </row>
@@ -8654,9 +9334,15 @@
       <c r="T116" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U116" t="inlineStr">
-        <is>
-          <t>3356</t>
+      <c r="U116" t="n">
+        <v>3356</v>
+      </c>
+      <c r="V116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W116" t="inlineStr">
+        <is>
+          <t>3497</t>
         </is>
       </c>
     </row>
@@ -8727,9 +9413,15 @@
       <c r="T117" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U117" t="inlineStr">
-        <is>
-          <t>2629</t>
+      <c r="U117" t="n">
+        <v>2629</v>
+      </c>
+      <c r="V117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W117" t="inlineStr">
+        <is>
+          <t>2623</t>
         </is>
       </c>
     </row>
@@ -8800,9 +9492,15 @@
       <c r="T118" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="U118" t="inlineStr">
-        <is>
-          <t>3619</t>
+      <c r="U118" t="n">
+        <v>3619</v>
+      </c>
+      <c r="V118" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="W118" t="inlineStr">
+        <is>
+          <t>3659</t>
         </is>
       </c>
     </row>
@@ -8873,9 +9571,15 @@
       <c r="T119" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="U119" t="inlineStr">
-        <is>
-          <t>4743</t>
+      <c r="U119" t="n">
+        <v>4743</v>
+      </c>
+      <c r="V119" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="W119" t="inlineStr">
+        <is>
+          <t>4808</t>
         </is>
       </c>
     </row>
@@ -8946,9 +9650,15 @@
       <c r="T120" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U120" t="inlineStr">
-        <is>
-          <t>2997</t>
+      <c r="U120" t="n">
+        <v>2997</v>
+      </c>
+      <c r="V120" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W120" t="inlineStr">
+        <is>
+          <t>3056</t>
         </is>
       </c>
     </row>
@@ -9019,9 +9729,15 @@
       <c r="T121" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="U121" t="inlineStr">
-        <is>
-          <t>1728</t>
+      <c r="U121" t="n">
+        <v>1728</v>
+      </c>
+      <c r="V121" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="W121" t="inlineStr">
+        <is>
+          <t>1779</t>
         </is>
       </c>
     </row>
@@ -9092,9 +9808,15 @@
       <c r="T122" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U122" t="inlineStr">
-        <is>
-          <t>3967</t>
+      <c r="U122" t="n">
+        <v>3967</v>
+      </c>
+      <c r="V122" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="W122" t="inlineStr">
+        <is>
+          <t>4039</t>
         </is>
       </c>
     </row>
@@ -9165,9 +9887,15 @@
       <c r="T123" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="U123" t="inlineStr">
-        <is>
-          <t>4633</t>
+      <c r="U123" t="n">
+        <v>4633</v>
+      </c>
+      <c r="V123" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="W123" t="inlineStr">
+        <is>
+          <t>4704</t>
         </is>
       </c>
     </row>
@@ -9238,7 +9966,13 @@
       <c r="T124" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U124" t="inlineStr">
+      <c r="U124" t="n">
+        <v>0</v>
+      </c>
+      <c r="V124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W124" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9311,9 +10045,15 @@
       <c r="T125" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U125" t="inlineStr">
-        <is>
-          <t>4243</t>
+      <c r="U125" t="n">
+        <v>4243</v>
+      </c>
+      <c r="V125" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="W125" t="inlineStr">
+        <is>
+          <t>4307</t>
         </is>
       </c>
     </row>
@@ -9384,9 +10124,15 @@
       <c r="T126" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U126" t="inlineStr">
-        <is>
-          <t>4189</t>
+      <c r="U126" t="n">
+        <v>4189</v>
+      </c>
+      <c r="V126" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W126" t="inlineStr">
+        <is>
+          <t>4344</t>
         </is>
       </c>
     </row>
@@ -9457,9 +10203,15 @@
       <c r="T127" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U127" t="inlineStr">
-        <is>
-          <t>3421</t>
+      <c r="U127" t="n">
+        <v>3421</v>
+      </c>
+      <c r="V127" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W127" t="inlineStr">
+        <is>
+          <t>3435</t>
         </is>
       </c>
     </row>
@@ -9530,9 +10282,15 @@
       <c r="T128" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="U128" t="inlineStr">
-        <is>
-          <t>4237</t>
+      <c r="U128" t="n">
+        <v>4237</v>
+      </c>
+      <c r="V128" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="W128" t="inlineStr">
+        <is>
+          <t>4296</t>
         </is>
       </c>
     </row>
@@ -9603,9 +10361,15 @@
       <c r="T129" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U129" t="inlineStr">
-        <is>
-          <t>2008</t>
+      <c r="U129" t="n">
+        <v>2008</v>
+      </c>
+      <c r="V129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W129" t="inlineStr">
+        <is>
+          <t>2005</t>
         </is>
       </c>
     </row>
@@ -9676,7 +10440,13 @@
       <c r="T130" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U130" t="inlineStr">
+      <c r="U130" t="n">
+        <v>0</v>
+      </c>
+      <c r="V130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9749,7 +10519,13 @@
       <c r="T131" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U131" t="inlineStr">
+      <c r="U131" t="n">
+        <v>0</v>
+      </c>
+      <c r="V131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9822,9 +10598,15 @@
       <c r="T132" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U132" t="inlineStr">
-        <is>
-          <t>4004</t>
+      <c r="U132" t="n">
+        <v>4004</v>
+      </c>
+      <c r="V132" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W132" t="inlineStr">
+        <is>
+          <t>4071</t>
         </is>
       </c>
     </row>
@@ -9895,7 +10677,13 @@
       <c r="T133" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U133" t="inlineStr">
+      <c r="U133" t="n">
+        <v>0</v>
+      </c>
+      <c r="V133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9968,9 +10756,15 @@
       <c r="T134" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U134" t="inlineStr">
-        <is>
-          <t>3475</t>
+      <c r="U134" t="n">
+        <v>3475</v>
+      </c>
+      <c r="V134" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W134" t="inlineStr">
+        <is>
+          <t>3557</t>
         </is>
       </c>
     </row>
@@ -10041,9 +10835,15 @@
       <c r="T135" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U135" t="inlineStr">
-        <is>
-          <t>4203</t>
+      <c r="U135" t="n">
+        <v>4203</v>
+      </c>
+      <c r="V135" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W135" t="inlineStr">
+        <is>
+          <t>4348</t>
         </is>
       </c>
     </row>
@@ -10114,9 +10914,15 @@
       <c r="T136" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U136" t="inlineStr">
-        <is>
-          <t>4135</t>
+      <c r="U136" t="n">
+        <v>4135</v>
+      </c>
+      <c r="V136" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W136" t="inlineStr">
+        <is>
+          <t>4271</t>
         </is>
       </c>
     </row>
@@ -10187,7 +10993,13 @@
       <c r="T137" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U137" t="inlineStr">
+      <c r="U137" t="n">
+        <v>0</v>
+      </c>
+      <c r="V137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10260,7 +11072,13 @@
       <c r="T138" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U138" t="inlineStr">
+      <c r="U138" t="n">
+        <v>0</v>
+      </c>
+      <c r="V138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W138" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10333,9 +11151,15 @@
       <c r="T139" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U139" t="inlineStr">
-        <is>
-          <t>3146</t>
+      <c r="U139" t="n">
+        <v>3146</v>
+      </c>
+      <c r="V139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W139" t="inlineStr">
+        <is>
+          <t>3137</t>
         </is>
       </c>
     </row>
@@ -10406,7 +11230,13 @@
       <c r="T140" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U140" t="inlineStr">
+      <c r="U140" t="n">
+        <v>0</v>
+      </c>
+      <c r="V140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10479,7 +11309,13 @@
       <c r="T141" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U141" t="inlineStr">
+      <c r="U141" t="n">
+        <v>0</v>
+      </c>
+      <c r="V141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10552,9 +11388,15 @@
       <c r="T142" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U142" t="inlineStr">
-        <is>
-          <t>3245</t>
+      <c r="U142" t="n">
+        <v>3245</v>
+      </c>
+      <c r="V142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W142" t="inlineStr">
+        <is>
+          <t>3238</t>
         </is>
       </c>
     </row>
@@ -10625,7 +11467,13 @@
       <c r="T143" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U143" t="inlineStr">
+      <c r="U143" t="n">
+        <v>0</v>
+      </c>
+      <c r="V143" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10698,9 +11546,15 @@
       <c r="T144" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U144" t="inlineStr">
-        <is>
-          <t>3789</t>
+      <c r="U144" t="n">
+        <v>3789</v>
+      </c>
+      <c r="V144" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W144" t="inlineStr">
+        <is>
+          <t>3785</t>
         </is>
       </c>
     </row>
@@ -10771,7 +11625,13 @@
       <c r="T145" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U145" t="inlineStr">
+      <c r="U145" t="n">
+        <v>0</v>
+      </c>
+      <c r="V145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10844,7 +11704,13 @@
       <c r="T146" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U146" t="inlineStr">
+      <c r="U146" t="n">
+        <v>0</v>
+      </c>
+      <c r="V146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10917,9 +11783,15 @@
       <c r="T147" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U147" t="inlineStr">
-        <is>
-          <t>2148</t>
+      <c r="U147" t="n">
+        <v>2148</v>
+      </c>
+      <c r="V147" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="W147" t="inlineStr">
+        <is>
+          <t>2166</t>
         </is>
       </c>
     </row>
@@ -10990,7 +11862,13 @@
       <c r="T148" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U148" t="inlineStr">
+      <c r="U148" t="n">
+        <v>0</v>
+      </c>
+      <c r="V148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11063,7 +11941,13 @@
       <c r="T149" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U149" t="inlineStr">
+      <c r="U149" t="n">
+        <v>0</v>
+      </c>
+      <c r="V149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11136,7 +12020,13 @@
       <c r="T150" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U150" t="inlineStr">
+      <c r="U150" t="n">
+        <v>2604</v>
+      </c>
+      <c r="V150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W150" t="inlineStr">
         <is>
           <t>2604</t>
         </is>
@@ -11209,7 +12099,13 @@
       <c r="T151" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U151" t="inlineStr">
+      <c r="U151" t="n">
+        <v>0</v>
+      </c>
+      <c r="V151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11282,7 +12178,13 @@
       <c r="T152" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U152" t="inlineStr">
+      <c r="U152" t="n">
+        <v>0</v>
+      </c>
+      <c r="V152" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11355,7 +12257,13 @@
       <c r="T153" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U153" t="inlineStr">
+      <c r="U153" t="n">
+        <v>0</v>
+      </c>
+      <c r="V153" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11428,9 +12336,15 @@
       <c r="T154" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U154" t="inlineStr">
-        <is>
-          <t>2915</t>
+      <c r="U154" t="n">
+        <v>2915</v>
+      </c>
+      <c r="V154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W154" t="inlineStr">
+        <is>
+          <t>2926</t>
         </is>
       </c>
     </row>
@@ -11501,7 +12415,13 @@
       <c r="T155" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U155" t="inlineStr">
+      <c r="U155" t="n">
+        <v>0</v>
+      </c>
+      <c r="V155" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11574,7 +12494,13 @@
       <c r="T156" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U156" t="inlineStr">
+      <c r="U156" t="n">
+        <v>0</v>
+      </c>
+      <c r="V156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11647,7 +12573,13 @@
       <c r="T157" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U157" t="inlineStr">
+      <c r="U157" t="n">
+        <v>0</v>
+      </c>
+      <c r="V157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11720,9 +12652,15 @@
       <c r="T158" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U158" t="inlineStr">
-        <is>
-          <t>3133</t>
+      <c r="U158" t="n">
+        <v>3133</v>
+      </c>
+      <c r="V158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W158" t="inlineStr">
+        <is>
+          <t>3189</t>
         </is>
       </c>
     </row>
@@ -11770,6 +12708,8 @@
       <c r="S159" t="inlineStr"/>
       <c r="T159" s="2" t="inlineStr"/>
       <c r="U159" t="inlineStr"/>
+      <c r="V159" s="2" t="inlineStr"/>
+      <c r="W159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="n">
@@ -11832,9 +12772,15 @@
       <c r="T160" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="U160" t="inlineStr">
-        <is>
-          <t>4750</t>
+      <c r="U160" t="n">
+        <v>4750</v>
+      </c>
+      <c r="V160" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="W160" t="inlineStr">
+        <is>
+          <t>4960</t>
         </is>
       </c>
     </row>
@@ -11874,6 +12820,8 @@
       <c r="S161" t="inlineStr"/>
       <c r="T161" s="2" t="inlineStr"/>
       <c r="U161" t="inlineStr"/>
+      <c r="V161" s="2" t="inlineStr"/>
+      <c r="W161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="n">
@@ -11936,9 +12884,15 @@
       <c r="T162" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="U162" t="inlineStr">
-        <is>
-          <t>3865</t>
+      <c r="U162" t="n">
+        <v>3865</v>
+      </c>
+      <c r="V162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W162" t="inlineStr">
+        <is>
+          <t>3917</t>
         </is>
       </c>
     </row>
@@ -12003,9 +12957,15 @@
       <c r="T163" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U163" t="inlineStr">
-        <is>
-          <t>3226</t>
+      <c r="U163" t="n">
+        <v>3226</v>
+      </c>
+      <c r="V163" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="W163" t="inlineStr">
+        <is>
+          <t>3274</t>
         </is>
       </c>
     </row>
@@ -12065,6 +13025,8 @@
       </c>
       <c r="T164" s="2" t="inlineStr"/>
       <c r="U164" t="inlineStr"/>
+      <c r="V164" s="2" t="inlineStr"/>
+      <c r="W164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -12103,9 +13065,15 @@
       <c r="T165" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="U165" t="inlineStr">
-        <is>
-          <t>7087</t>
+      <c r="U165" t="n">
+        <v>7087</v>
+      </c>
+      <c r="V165" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W165" t="inlineStr">
+        <is>
+          <t>7392</t>
         </is>
       </c>
     </row>
@@ -12146,17 +13114,21 @@
       <c r="T166" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="U166" t="inlineStr">
-        <is>
-          <t>4588</t>
+      <c r="U166" t="n">
+        <v>4588</v>
+      </c>
+      <c r="V166" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="W166" t="inlineStr">
+        <is>
+          <t>4663</t>
         </is>
       </c>
     </row>
     <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>49000199</t>
-        </is>
+      <c r="A167" t="n">
+        <v>49000199</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
@@ -12187,17 +13159,21 @@
       <c r="T167" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="U167" t="inlineStr">
-        <is>
-          <t>1066</t>
+      <c r="U167" t="n">
+        <v>1066</v>
+      </c>
+      <c r="V167" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="W167" t="inlineStr">
+        <is>
+          <t>1126</t>
         </is>
       </c>
     </row>
     <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>52157846</t>
-        </is>
+      <c r="A168" t="n">
+        <v>52157846</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
@@ -12228,17 +13204,21 @@
       <c r="T168" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="U168" t="inlineStr">
-        <is>
-          <t>2776</t>
+      <c r="U168" t="n">
+        <v>2776</v>
+      </c>
+      <c r="V168" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="W168" t="inlineStr">
+        <is>
+          <t>3147</t>
         </is>
       </c>
     </row>
     <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>59081265</t>
-        </is>
+      <c r="A169" t="n">
+        <v>59081265</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
@@ -12269,9 +13249,58 @@
       <c r="T169" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="U169" t="inlineStr">
-        <is>
-          <t>1305</t>
+      <c r="U169" t="n">
+        <v>1305</v>
+      </c>
+      <c r="V169" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="W169" t="inlineStr">
+        <is>
+          <t>1602</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>45404911</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>小伙伴666</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr"/>
+      <c r="D170" t="inlineStr"/>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F170" s="2" t="inlineStr"/>
+      <c r="G170" t="inlineStr"/>
+      <c r="H170" s="2" t="inlineStr"/>
+      <c r="I170" t="inlineStr"/>
+      <c r="J170" s="2" t="inlineStr"/>
+      <c r="K170" t="inlineStr"/>
+      <c r="L170" s="2" t="inlineStr"/>
+      <c r="M170" t="inlineStr"/>
+      <c r="N170" s="2" t="inlineStr"/>
+      <c r="O170" t="inlineStr"/>
+      <c r="P170" s="2" t="inlineStr"/>
+      <c r="Q170" t="inlineStr"/>
+      <c r="R170" s="2" t="inlineStr"/>
+      <c r="S170" t="inlineStr"/>
+      <c r="T170" s="2" t="inlineStr"/>
+      <c r="U170" t="inlineStr"/>
+      <c r="V170" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W170" t="inlineStr">
+        <is>
+          <t>3975</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-24 12:41:42
</commit_message>
<xml_diff>
--- a/Season_Attack/86.xlsx
+++ b/Season_Attack/86.xlsx
@@ -13262,10 +13262,8 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>45404911</t>
-        </is>
+      <c r="A170" t="n">
+        <v>45404911</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>

</xml_diff>